<commit_message>
Add second family for minimal install
</commit_message>
<xml_diff>
--- a/src/Resources/fixtures/minimal/init.xlsx
+++ b/src/Resources/fixtures/minimal/init.xlsx
@@ -5,22 +5,23 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="attributes" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="family main" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="attribute_groups" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="options" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="channels" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="categories" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="group_types" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="association_types" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="choices" sheetId="10" state="hidden" r:id="rId11"/>
-    <sheet name="attribute_types" sheetId="11" state="hidden" r:id="rId12"/>
-    <sheet name="metric_types" sheetId="12" state="hidden" r:id="rId13"/>
-    <sheet name="metric_units" sheetId="13" state="hidden" r:id="rId14"/>
+    <sheet name="family secondary" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="attribute_groups" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="options" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="channels" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="categories" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="group_types" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="association_types" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="choices" sheetId="11" state="hidden" r:id="rId12"/>
+    <sheet name="attribute_types" sheetId="12" state="hidden" r:id="rId13"/>
+    <sheet name="metric_types" sheetId="13" state="hidden" r:id="rId14"/>
+    <sheet name="metric_units" sheetId="14" state="hidden" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="attribute_groups" vbProcedure="false">attribute_groups!$A$4:$A$100</definedName>
@@ -32,7 +33,7 @@
     <definedName function="false" hidden="false" name="validation_choices" vbProcedure="false">choices!$B$1:$B$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">attributes!$B$6:$AU$9</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'family main'!$C$5:$AW$8</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">attribute_groups!$A$4:$C$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">attribute_groups!$A$4:$C$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -171,7 +172,62 @@
 </comments>
 </file>
 
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="Y4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Insert the allowed extensions, separated by a comma.
+For example : 
+jpg, jpeg, png</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Determines how many characters should be typed for select attributes before an option is presented.
+This should be used for attributes which have a large number of options.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Set to 1 if the attribute is required in this family for the concerned channel.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
     <author/>
@@ -212,7 +268,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="269">
   <si>
     <t>End user HOWTO</t>
   </si>
@@ -509,6 +565,12 @@
   </si>
   <si>
     <t>use_as_label</t>
+  </si>
+  <si>
+    <t>second_family</t>
+  </si>
+  <si>
+    <t>Second family</t>
   </si>
   <si>
     <t>Group properties</t>
@@ -1350,15 +1412,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>901080</xdr:colOff>
+      <xdr:colOff>927720</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>142200</xdr:rowOff>
+      <xdr:rowOff>141840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1367,8 +1429,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="8590680" cy="9531720"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="8466480" cy="9531360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1395,15 +1457,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>901080</xdr:colOff>
+      <xdr:colOff>927720</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>142200</xdr:rowOff>
+      <xdr:rowOff>141840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1412,8 +1474,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="8590680" cy="9531720"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="8466480" cy="9531360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1445,15 +1507,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>53280</xdr:colOff>
+      <xdr:colOff>79920</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>142560</xdr:rowOff>
+      <xdr:rowOff>142200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1462,8 +1524,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="6142680" cy="10202040"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="6047280" cy="10201680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1490,15 +1552,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>53280</xdr:colOff>
+      <xdr:colOff>79920</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>142560</xdr:rowOff>
+      <xdr:rowOff>142200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1507,8 +1569,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="6142680" cy="10202040"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="6047280" cy="10201680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1540,15 +1602,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>901080</xdr:colOff>
+      <xdr:colOff>927720</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>142200</xdr:rowOff>
+      <xdr:rowOff>141840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1557,8 +1619,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="9762480" cy="9531720"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="9619200" cy="9531360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1585,15 +1647,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>901080</xdr:colOff>
+      <xdr:colOff>927720</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>142200</xdr:rowOff>
+      <xdr:rowOff>141840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1602,8 +1664,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="9762480" cy="9531720"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="9619200" cy="9531360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1643,8 +1705,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1829,50 +1891,84 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="48.4642857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+    <row r="1" s="28" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="B7" s="28" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>143</v>
-      </c>
-    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B4" type="none">
+      <formula1>ouinon</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -1886,137 +1982,54 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="C3" s="0" t="s">
         <v>145</v>
-      </c>
-    </row>
-    <row r="2" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>167</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
@@ -2029,21 +2042,22 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2051,103 +2065,103 @@
         <v>60</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>168</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>169</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2166,6 +2180,147 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:B89"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -2174,13 +2329,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B1" s="16"/>
     </row>
@@ -2189,703 +2345,703 @@
         <v>62</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -2912,36 +3068,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="44" min="26" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="7" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="8" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="48" min="47" style="7" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="49" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="44" min="26" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="7" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="8" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="48" min="47" style="7" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="49" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3323,49 +3479,48 @@
   </sheetPr>
   <dimension ref="A1:AX7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3742,6 +3897,413 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:AX6"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.50510204081633"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D1" s="3"/>
+      <c r="E1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
+      <c r="H1" s="0"/>
+      <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
+      <c r="AA1" s="0"/>
+      <c r="AU1" s="0"/>
+      <c r="AV1" s="0"/>
+      <c r="AW1" s="0"/>
+      <c r="AX1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" s="0"/>
+      <c r="G2" s="0"/>
+      <c r="H2" s="0"/>
+      <c r="J2" s="0"/>
+      <c r="K2" s="0"/>
+      <c r="AA2" s="0"/>
+      <c r="AU2" s="0"/>
+      <c r="AV2" s="0"/>
+      <c r="AW2" s="0"/>
+      <c r="AX2" s="0"/>
+    </row>
+    <row r="3" s="12" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="P4" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q4" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="R4" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="S4" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="T4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="U4" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="V4" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="W4" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="X4" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y4" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z4" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA4" s="21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="N5" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="O5" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="P5" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q5" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="R5" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="S5" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="T5" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="U5" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="V5" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="W5" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="X5" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y5" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z5" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA5" s="22"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="19"/>
+      <c r="X6" s="19"/>
+      <c r="Y6" s="19"/>
+      <c r="Z6" s="19"/>
+      <c r="AA6" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="19"/>
+      <c r="AC6" s="19"/>
+      <c r="AD6" s="19"/>
+      <c r="AE6" s="19"/>
+      <c r="AF6" s="19"/>
+      <c r="AG6" s="19"/>
+      <c r="AH6" s="19"/>
+      <c r="AI6" s="19"/>
+      <c r="AJ6" s="19"/>
+      <c r="AK6" s="19"/>
+      <c r="AL6" s="19"/>
+      <c r="AM6" s="19"/>
+      <c r="AN6" s="19"/>
+      <c r="AO6" s="19"/>
+      <c r="AP6" s="19"/>
+      <c r="AQ6" s="19"/>
+      <c r="AR6" s="19"/>
+      <c r="AS6" s="19"/>
+      <c r="AT6" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D3:Z3"/>
+  </mergeCells>
+  <dataValidations count="13">
+    <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="T6" type="decimal">
+      <formula1>$P$7</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6" type="whole">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="N6" type="none">
+      <formula1>ouinon</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B6 G6:H6 J6:K6 O6 R6:S6" type="list">
+      <formula1>boolean_choices</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L6" type="whole">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M6" type="list">
+      <formula1>validation_choices</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X6 Z6" type="whole">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AA6" type="list">
+      <formula1>boolean_choices</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P6:Q6" type="whole">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="V3:V6" type="list">
+      <formula1>metric_types</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="W3:W6" type="list">
+      <formula1>metric_units</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D3:D6" type="list">
+      <formula1>attribute_types</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E3:E6" type="list">
+      <formula1>attribute_groups</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -3750,15 +4312,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="16.3316326530612"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="25" t="s">
@@ -3767,10 +4329,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>36</v>
@@ -3795,18 +4357,18 @@
         <v>1</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -3823,7 +4385,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -3836,14 +4398,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="16.3316326530612"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="25" t="s">
@@ -3855,7 +4417,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>36</v>
@@ -3863,7 +4425,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>60</v>
@@ -3887,7 +4449,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -3900,18 +4462,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1016" min="6" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="1017" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1016" min="6" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="1017" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -3920,19 +4482,19 @@
     </row>
     <row r="2" customFormat="false" ht="49.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="9.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3940,16 +4502,16 @@
         <v>60</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="19.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3963,7 +4525,7 @@
         <v>36</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>93</v>
@@ -3991,7 +4553,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -4004,14 +4566,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="16.3316326530612"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="25" t="s">
@@ -4020,10 +4582,10 @@
     </row>
     <row r="2" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>36</v>
@@ -4034,7 +4596,7 @@
         <v>60</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C3" s="26" t="s">
         <v>61</v>
@@ -4045,7 +4607,7 @@
         <v>93</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -4069,7 +4631,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -4082,14 +4644,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B1" s="24"/>
     </row>
@@ -4098,7 +4660,7 @@
         <v>60</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4106,12 +4668,12 @@
         <v>60</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -4119,7 +4681,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -4143,95 +4705,4 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="49"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="28" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>137</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B4" type="none">
-      <formula1>ouinon</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add dummy header only for first tab (#2)
* Add dummy header only for first tab
* Add second family for minimal install
</commit_message>
<xml_diff>
--- a/src/Resources/fixtures/minimal/init.xlsx
+++ b/src/Resources/fixtures/minimal/init.xlsx
@@ -5,22 +5,23 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="attributes" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="family main" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="attribute_groups" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="options" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="channels" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="categories" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="group_types" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="association_types" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="choices" sheetId="10" state="hidden" r:id="rId11"/>
-    <sheet name="attribute_types" sheetId="11" state="hidden" r:id="rId12"/>
-    <sheet name="metric_types" sheetId="12" state="hidden" r:id="rId13"/>
-    <sheet name="metric_units" sheetId="13" state="hidden" r:id="rId14"/>
+    <sheet name="family secondary" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="attribute_groups" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="options" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="channels" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="categories" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="group_types" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="association_types" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="choices" sheetId="11" state="hidden" r:id="rId12"/>
+    <sheet name="attribute_types" sheetId="12" state="hidden" r:id="rId13"/>
+    <sheet name="metric_types" sheetId="13" state="hidden" r:id="rId14"/>
+    <sheet name="metric_units" sheetId="14" state="hidden" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="attribute_groups" vbProcedure="false">attribute_groups!$A$4:$A$100</definedName>
@@ -32,7 +33,7 @@
     <definedName function="false" hidden="false" name="validation_choices" vbProcedure="false">choices!$B$1:$B$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">attributes!$B$6:$AU$9</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'family main'!$C$5:$AW$8</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">attribute_groups!$A$4:$C$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">attribute_groups!$A$4:$C$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -171,7 +172,62 @@
 </comments>
 </file>
 
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="Y4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Insert the allowed extensions, separated by a comma.
+For example : 
+jpg, jpeg, png</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Determines how many characters should be typed for select attributes before an option is presented.
+This should be used for attributes which have a large number of options.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Set to 1 if the attribute is required in this family for the concerned channel.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
     <author/>
@@ -212,7 +268,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="269">
   <si>
     <t>End user HOWTO</t>
   </si>
@@ -509,6 +565,12 @@
   </si>
   <si>
     <t>use_as_label</t>
+  </si>
+  <si>
+    <t>second_family</t>
+  </si>
+  <si>
+    <t>Second family</t>
   </si>
   <si>
     <t>Group properties</t>
@@ -1350,15 +1412,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>901080</xdr:colOff>
+      <xdr:colOff>927720</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>142200</xdr:rowOff>
+      <xdr:rowOff>141840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1367,8 +1429,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="8590680" cy="9531720"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="8466480" cy="9531360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1395,15 +1457,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>901080</xdr:colOff>
+      <xdr:colOff>927720</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>142200</xdr:rowOff>
+      <xdr:rowOff>141840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1412,8 +1474,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="8590680" cy="9531720"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="8466480" cy="9531360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1445,15 +1507,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>53280</xdr:colOff>
+      <xdr:colOff>79920</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>142560</xdr:rowOff>
+      <xdr:rowOff>142200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1462,8 +1524,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="6142680" cy="10202040"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="6047280" cy="10201680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1490,15 +1552,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>53280</xdr:colOff>
+      <xdr:colOff>79920</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>142560</xdr:rowOff>
+      <xdr:rowOff>142200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1507,8 +1569,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="6142680" cy="10202040"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="6047280" cy="10201680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1540,15 +1602,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>901080</xdr:colOff>
+      <xdr:colOff>927720</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>142200</xdr:rowOff>
+      <xdr:rowOff>141840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1557,8 +1619,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="9762480" cy="9531720"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="9619200" cy="9531360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1585,15 +1647,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>901080</xdr:colOff>
+      <xdr:colOff>927720</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>142200</xdr:rowOff>
+      <xdr:rowOff>141840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1602,8 +1664,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="0"/>
-          <a:ext cx="9762480" cy="9531720"/>
+          <a:off x="81000" y="0"/>
+          <a:ext cx="9619200" cy="9531360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1643,8 +1705,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1829,50 +1891,84 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="48.4642857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+    <row r="1" s="28" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="B7" s="28" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>143</v>
-      </c>
-    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B4" type="none">
+      <formula1>ouinon</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -1886,137 +1982,54 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="C3" s="0" t="s">
         <v>145</v>
-      </c>
-    </row>
-    <row r="2" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>167</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
@@ -2029,21 +2042,22 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2051,103 +2065,103 @@
         <v>60</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>168</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>169</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2166,6 +2180,147 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:B89"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -2174,13 +2329,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B1" s="16"/>
     </row>
@@ -2189,703 +2345,703 @@
         <v>62</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -2912,36 +3068,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="44" min="26" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="7" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="8" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="48" min="47" style="7" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="49" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="44" min="26" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="7" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="8" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="48" min="47" style="7" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="49" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3323,49 +3479,48 @@
   </sheetPr>
   <dimension ref="A1:AX7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3742,6 +3897,413 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:AX6"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.50510204081633"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D1" s="3"/>
+      <c r="E1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
+      <c r="H1" s="0"/>
+      <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
+      <c r="AA1" s="0"/>
+      <c r="AU1" s="0"/>
+      <c r="AV1" s="0"/>
+      <c r="AW1" s="0"/>
+      <c r="AX1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" s="0"/>
+      <c r="G2" s="0"/>
+      <c r="H2" s="0"/>
+      <c r="J2" s="0"/>
+      <c r="K2" s="0"/>
+      <c r="AA2" s="0"/>
+      <c r="AU2" s="0"/>
+      <c r="AV2" s="0"/>
+      <c r="AW2" s="0"/>
+      <c r="AX2" s="0"/>
+    </row>
+    <row r="3" s="12" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="P4" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q4" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="R4" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="S4" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="T4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="U4" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="V4" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="W4" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="X4" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y4" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z4" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA4" s="21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="N5" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="O5" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="P5" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q5" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="R5" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="S5" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="T5" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="U5" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="V5" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="W5" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="X5" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y5" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z5" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA5" s="22"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="19"/>
+      <c r="X6" s="19"/>
+      <c r="Y6" s="19"/>
+      <c r="Z6" s="19"/>
+      <c r="AA6" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="19"/>
+      <c r="AC6" s="19"/>
+      <c r="AD6" s="19"/>
+      <c r="AE6" s="19"/>
+      <c r="AF6" s="19"/>
+      <c r="AG6" s="19"/>
+      <c r="AH6" s="19"/>
+      <c r="AI6" s="19"/>
+      <c r="AJ6" s="19"/>
+      <c r="AK6" s="19"/>
+      <c r="AL6" s="19"/>
+      <c r="AM6" s="19"/>
+      <c r="AN6" s="19"/>
+      <c r="AO6" s="19"/>
+      <c r="AP6" s="19"/>
+      <c r="AQ6" s="19"/>
+      <c r="AR6" s="19"/>
+      <c r="AS6" s="19"/>
+      <c r="AT6" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D3:Z3"/>
+  </mergeCells>
+  <dataValidations count="13">
+    <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="T6" type="decimal">
+      <formula1>$P$7</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6" type="whole">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="N6" type="none">
+      <formula1>ouinon</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B6 G6:H6 J6:K6 O6 R6:S6" type="list">
+      <formula1>boolean_choices</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L6" type="whole">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M6" type="list">
+      <formula1>validation_choices</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X6 Z6" type="whole">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AA6" type="list">
+      <formula1>boolean_choices</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P6:Q6" type="whole">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="V3:V6" type="list">
+      <formula1>metric_types</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="W3:W6" type="list">
+      <formula1>metric_units</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D3:D6" type="list">
+      <formula1>attribute_types</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E3:E6" type="list">
+      <formula1>attribute_groups</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -3750,15 +4312,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="16.3316326530612"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="25" t="s">
@@ -3767,10 +4329,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>36</v>
@@ -3795,18 +4357,18 @@
         <v>1</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -3823,7 +4385,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -3836,14 +4398,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="16.3316326530612"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="25" t="s">
@@ -3855,7 +4417,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>36</v>
@@ -3863,7 +4425,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>60</v>
@@ -3887,7 +4449,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -3900,18 +4462,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1016" min="6" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="1017" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1016" min="6" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="1017" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -3920,19 +4482,19 @@
     </row>
     <row r="2" customFormat="false" ht="49.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="9.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3940,16 +4502,16 @@
         <v>60</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="19.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3963,7 +4525,7 @@
         <v>36</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>93</v>
@@ -3991,7 +4553,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -4004,14 +4566,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="16.3316326530612"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="25" t="s">
@@ -4020,10 +4582,10 @@
     </row>
     <row r="2" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>36</v>
@@ -4034,7 +4596,7 @@
         <v>60</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C3" s="26" t="s">
         <v>61</v>
@@ -4045,7 +4607,7 @@
         <v>93</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -4069,7 +4631,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -4082,14 +4644,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B1" s="24"/>
     </row>
@@ -4098,7 +4660,7 @@
         <v>60</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4106,12 +4668,12 @@
         <v>60</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -4119,7 +4681,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -4143,95 +4705,4 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="49"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="28" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>137</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B4" type="none">
-      <formula1>ouinon</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix english init.xls for "group_types" tab
The user readable headers must not be the same as the technical headers. The first column must be `Group code` to not mix up with the technical `code` header
</commit_message>
<xml_diff>
--- a/src/Resources/fixtures/minimal/init.xlsx
+++ b/src/Resources/fixtures/minimal/init.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -1412,15 +1412,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>81000</xdr:colOff>
+      <xdr:colOff>108000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>927720</xdr:colOff>
+      <xdr:colOff>954360</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>141840</xdr:rowOff>
+      <xdr:rowOff>141480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1429,8 +1429,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="81000" y="0"/>
-          <a:ext cx="8466480" cy="9531360"/>
+          <a:off x="108000" y="0"/>
+          <a:ext cx="8342280" cy="9531000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1457,15 +1457,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>81000</xdr:colOff>
+      <xdr:colOff>108000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>927720</xdr:colOff>
+      <xdr:colOff>954360</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>141840</xdr:rowOff>
+      <xdr:rowOff>141480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1474,8 +1474,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="81000" y="0"/>
-          <a:ext cx="8466480" cy="9531360"/>
+          <a:off x="108000" y="0"/>
+          <a:ext cx="8342280" cy="9531000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1507,15 +1507,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>81000</xdr:colOff>
+      <xdr:colOff>108000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>79920</xdr:colOff>
+      <xdr:colOff>106560</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>142200</xdr:rowOff>
+      <xdr:rowOff>141840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1524,8 +1524,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="81000" y="0"/>
-          <a:ext cx="6047280" cy="10201680"/>
+          <a:off x="108000" y="0"/>
+          <a:ext cx="5951520" cy="10201320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1552,15 +1552,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>81000</xdr:colOff>
+      <xdr:colOff>108000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>79920</xdr:colOff>
+      <xdr:colOff>106560</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>142200</xdr:rowOff>
+      <xdr:rowOff>141840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1569,8 +1569,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="81000" y="0"/>
-          <a:ext cx="6047280" cy="10201680"/>
+          <a:off x="108000" y="0"/>
+          <a:ext cx="5951520" cy="10201320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1602,15 +1602,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>81000</xdr:colOff>
+      <xdr:colOff>108000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>927720</xdr:colOff>
+      <xdr:colOff>954360</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>141840</xdr:rowOff>
+      <xdr:rowOff>141480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1619,8 +1619,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="81000" y="0"/>
-          <a:ext cx="9619200" cy="9531360"/>
+          <a:off x="108000" y="0"/>
+          <a:ext cx="9475920" cy="9531000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1647,15 +1647,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>81000</xdr:colOff>
+      <xdr:colOff>108000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>927720</xdr:colOff>
+      <xdr:colOff>954360</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>141840</xdr:rowOff>
+      <xdr:rowOff>141480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1664,8 +1664,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="81000" y="0"/>
-          <a:ext cx="9619200" cy="9531360"/>
+          <a:off x="108000" y="0"/>
+          <a:ext cx="9475920" cy="9531000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1705,8 +1705,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.12755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.99489795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1899,9 +1899,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="48.4642857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="47.7857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="28" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1990,7 +1990,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2047,9 +2047,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2188,9 +2188,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2329,9 +2329,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3068,36 +3068,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="44" min="26" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="7" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="8" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="48" min="47" style="7" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="49" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="44" min="26" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="7" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="8" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="48" min="47" style="7" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="49" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3485,42 +3485,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3899,48 +3899,48 @@
   </sheetPr>
   <dimension ref="A1:AX6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4312,10 +4312,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="16.0663265306122"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4398,9 +4397,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6275510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4462,13 +4460,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="1016" min="6" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="1017" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="1017" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4566,9 +4563,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6275510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4638,15 +4634,15 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4655,9 +4651,9 @@
       </c>
       <c r="B1" s="24"/>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>127</v>

</xml_diff>

<commit_message>
README tab: do not remove the "other" attribute group
</commit_message>
<xml_diff>
--- a/src/Resources/fixtures/minimal/init.xlsx
+++ b/src/Resources/fixtures/minimal/init.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -268,7 +268,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="270">
   <si>
     <t>End user HOWTO</t>
   </si>
@@ -316,6 +316,9 @@
   </si>
   <si>
     <t>This tab contains all informations for attribute groups</t>
+  </si>
+  <si>
+    <t>You should not delete the mandatory “other” group</t>
   </si>
   <si>
     <t>Options</t>
@@ -1412,15 +1415,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>135000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>954360</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>380880</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>141480</xdr:rowOff>
+      <xdr:rowOff>141120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1429,8 +1432,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="0"/>
-          <a:ext cx="8342280" cy="9531000"/>
+          <a:off x="135000" y="0"/>
+          <a:ext cx="6160680" cy="9530640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1457,15 +1460,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>135000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>954360</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>380880</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>141480</xdr:rowOff>
+      <xdr:rowOff>141120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1474,8 +1477,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="0"/>
-          <a:ext cx="8342280" cy="9531000"/>
+          <a:off x="135000" y="0"/>
+          <a:ext cx="6160680" cy="9530640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1507,15 +1510,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>135000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>106560</xdr:colOff>
+      <xdr:colOff>133200</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>141840</xdr:rowOff>
+      <xdr:rowOff>141480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1524,8 +1527,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="0"/>
-          <a:ext cx="5951520" cy="10201320"/>
+          <a:off x="135000" y="0"/>
+          <a:ext cx="5865480" cy="10200960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1552,15 +1555,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>135000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>106560</xdr:colOff>
+      <xdr:colOff>133200</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>141840</xdr:rowOff>
+      <xdr:rowOff>141480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1569,8 +1572,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="0"/>
-          <a:ext cx="5951520" cy="10201320"/>
+          <a:off x="135000" y="0"/>
+          <a:ext cx="5865480" cy="10200960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1602,15 +1605,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>135000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>954360</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>380880</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>141480</xdr:rowOff>
+      <xdr:rowOff>141120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1619,8 +1622,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="0"/>
-          <a:ext cx="9475920" cy="9531000"/>
+          <a:off x="135000" y="0"/>
+          <a:ext cx="6760800" cy="9530640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1647,15 +1650,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>135000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>954360</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>380880</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>141480</xdr:rowOff>
+      <xdr:rowOff>141120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1664,8 +1667,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="0"/>
-          <a:ext cx="9475920" cy="9531000"/>
+          <a:off x="135000" y="0"/>
+          <a:ext cx="6760800" cy="9530640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1697,16 +1700,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.99489795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.86224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1795,84 +1797,89 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="2" t="s">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="2" t="s">
+    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="s">
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="0" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="2" t="s">
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0" t="s">
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="0" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="2" t="s">
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="0" t="s">
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="2" t="s">
+    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="5" t="s">
+    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="0" t="s">
+    <row r="51" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1899,65 +1906,64 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="47.7857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="47.1122448979592"/>
   </cols>
   <sheetData>
     <row r="1" s="28" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1989,19 +1995,16 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.1224489795918"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2009,18 +2012,18 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2047,121 +2050,121 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2188,121 +2191,121 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -2329,719 +2332,719 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B1" s="16"/>
     </row>
     <row r="2" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -3068,41 +3071,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="44" min="26" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="7" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="8" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="48" min="47" style="7" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="49" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="7" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="8" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="48" min="47" style="7" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -3133,10 +3133,10 @@
     <row r="4" s="12" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9"/>
       <c r="B4" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
@@ -3163,170 +3163,170 @@
     </row>
     <row r="5" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M5" s="13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N5" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="O5" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="P5" s="13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q5" s="13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="R5" s="13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="S5" s="13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="T5" s="13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="U5" s="13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="V5" s="13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="W5" s="13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="X5" s="13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Y5" s="13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="N6" s="16" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="P6" s="16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Q6" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="R6" s="16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="S6" s="16" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="T6" s="16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="U6" s="16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="V6" s="16" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="W6" s="16" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="X6" s="16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="Y6" s="16" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E7" s="6" t="n">
         <v>1</v>
@@ -3380,16 +3380,16 @@
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="E8" s="6" t="n">
         <v>2</v>
@@ -3485,48 +3485,48 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="13.5"/>
+    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F1" s="0"/>
       <c r="G1" s="0"/>
@@ -3541,16 +3541,16 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F2" s="0"/>
       <c r="G2" s="0"/>
@@ -3567,10 +3567,10 @@
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
@@ -3595,176 +3595,176 @@
       <c r="Y3" s="11"/>
       <c r="Z3" s="11"/>
       <c r="AA3" s="20" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N4" s="13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="O4" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="P4" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="Q4" s="13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="R4" s="13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="S4" s="13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="T4" s="13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="U4" s="13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="V4" s="13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="W4" s="13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="X4" s="13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Y4" s="13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z4" s="13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA4" s="21" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="N5" s="16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="P5" s="16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Q5" s="16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="R5" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="S5" s="16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="T5" s="16" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="U5" s="16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="V5" s="16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="W5" s="16" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="X5" s="16" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="Y5" s="16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="Z5" s="16" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AA5" s="22"/>
     </row>
     <row r="6" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -3812,7 +3812,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1</v>
@@ -3905,48 +3905,48 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="13.5"/>
+    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F1" s="0"/>
       <c r="G1" s="0"/>
@@ -3961,16 +3961,16 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F2" s="0"/>
       <c r="G2" s="0"/>
@@ -3987,10 +3987,10 @@
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
@@ -4015,176 +4015,176 @@
       <c r="Y3" s="11"/>
       <c r="Z3" s="11"/>
       <c r="AA3" s="20" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N4" s="13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="O4" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="P4" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="Q4" s="13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="R4" s="13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="S4" s="13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="T4" s="13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="U4" s="13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="V4" s="13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="W4" s="13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="X4" s="13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Y4" s="13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z4" s="13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA4" s="21" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="N5" s="16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="P5" s="16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Q5" s="16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="R5" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="S5" s="16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="T5" s="16" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="U5" s="16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="V5" s="16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="W5" s="16" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="X5" s="16" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="Y5" s="16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="Z5" s="16" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AA5" s="22"/>
     </row>
     <row r="6" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -4312,62 +4312,63 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="11.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B4" s="19" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -4397,39 +4398,40 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -4460,17 +4462,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="1017" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1016" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1017" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -4479,53 +4482,53 @@
     </row>
     <row r="2" customFormat="false" ht="49.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="9.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="19.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -4563,47 +4566,48 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -4634,42 +4638,41 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.3826530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="24"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -4677,7 +4680,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
currencies, user groups, user roles and users fixtures moved in the init.xlsx import
</commit_message>
<xml_diff>
--- a/src/Resources/fixtures/minimal/init.xlsx
+++ b/src/Resources/fixtures/minimal/init.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,6 +22,10 @@
     <sheet name="attribute_types" sheetId="12" state="hidden" r:id="rId13"/>
     <sheet name="metric_types" sheetId="13" state="hidden" r:id="rId14"/>
     <sheet name="metric_units" sheetId="14" state="hidden" r:id="rId15"/>
+    <sheet name="user_groups" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="user_roles" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="users" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="currencies" sheetId="18" state="visible" r:id="rId19"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="attribute_groups" vbProcedure="false">attribute_groups!$A$4:$A$100</definedName>
@@ -60,7 +64,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Insert the name of the locales, separated by ",".
+          <t xml:space="preserve">Insert the name of the locales, separated by ",".
 For example : "en_US, fr_FR"
 </t>
         </r>
@@ -76,7 +80,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Insert the allowed extensions, separated by a comma.
+          <t xml:space="preserve">Insert the allowed extensions, separated by a comma.
 For example : 
 jpg, jpeg, png</t>
         </r>
@@ -92,7 +96,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Determines how many characters should be typed for select attributes before an option is presented.
+          <t xml:space="preserve">Determines how many characters should be typed for select attributes before an option is presented.
 This should be used for attributes which have a large number of options.</t>
         </r>
       </text>
@@ -117,7 +121,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Insert the name of the locales, separated by ",".
+          <t xml:space="preserve">Insert the name of the locales, separated by ",".
 For example : "en_US, fr_FR"
 </t>
         </r>
@@ -133,7 +137,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Insert the allowed extensions, separated by a comma.
+          <t xml:space="preserve">Insert the allowed extensions, separated by a comma.
 For example : 
 jpg, jpeg, png</t>
         </r>
@@ -149,7 +153,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Determines how many characters should be typed for select attributes before an option is presented.
+          <t xml:space="preserve">Determines how many characters should be typed for select attributes before an option is presented.
 This should be used for attributes which have a large number of options.</t>
         </r>
       </text>
@@ -164,7 +168,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Set to 1 if the attribute is required in this family for the concerned channel.</t>
+          <t xml:space="preserve">Set to 1 if the attribute is required in this family for the concerned channel.</t>
         </r>
       </text>
     </comment>
@@ -188,7 +192,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Insert the allowed extensions, separated by a comma.
+          <t xml:space="preserve">Insert the allowed extensions, separated by a comma.
 For example : 
 jpg, jpeg, png</t>
         </r>
@@ -204,7 +208,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Determines how many characters should be typed for select attributes before an option is presented.
+          <t xml:space="preserve">Determines how many characters should be typed for select attributes before an option is presented.
 This should be used for attributes which have a large number of options.</t>
         </r>
       </text>
@@ -219,7 +223,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Set to 1 if the attribute is required in this family for the concerned channel.</t>
+          <t xml:space="preserve">Set to 1 if the attribute is required in this family for the concerned channel.</t>
         </r>
       </text>
     </comment>
@@ -243,7 +247,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Multiple locales should be separated by a comma.
+          <t xml:space="preserve">Multiple locales should be separated by a comma.
 For example : "fr_FR, en_US"</t>
         </r>
       </text>
@@ -258,7 +262,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Multiple currency codes should be separated by a comma.
+          <t xml:space="preserve">Multiple currency codes should be separated by a comma.
 For example: "EUR,USD"</t>
         </r>
       </text>
@@ -268,816 +272,1209 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="270">
-  <si>
-    <t>End user HOWTO</t>
-  </si>
-  <si>
-    <t>Global rules</t>
-  </si>
-  <si>
-    <t>Do not modify the headers of the files</t>
-  </si>
-  <si>
-    <t>Do not open this file in Open Office, as it will break the validation</t>
-  </si>
-  <si>
-    <t>Do not save this file with another extension than xlsx</t>
-  </si>
-  <si>
-    <t>Do not modify hidden rows</t>
-  </si>
-  <si>
-    <t>Attributes tab</t>
-  </si>
-  <si>
-    <t>The attributes tab can be used to define the properties of attributes which are not linked to families, or which are shared by families.</t>
-  </si>
-  <si>
-    <t>This tab can be duplicated to shorten the list. All attributes tab titles should start with "attributes"</t>
-  </si>
-  <si>
-    <t>Family tabs</t>
-  </si>
-  <si>
-    <t>The family tab contains all information for a family : code, labels, attributes and completion rules</t>
-  </si>
-  <si>
-    <t>To create a new family, simply duplicate the tab. All family tabs titles must start with "family"</t>
-  </si>
-  <si>
-    <t>If an attribute is present in multiple families, only fill the blue and pink columns (attribute properties and translations) once </t>
-  </si>
-  <si>
-    <t>To add completion for other channels, simply add columns on the right of the table. The label should be the code of the channel.</t>
-  </si>
-  <si>
-    <t>Attribute groups</t>
-  </si>
-  <si>
-    <t>This tab contains all informations for attribute groups</t>
-  </si>
-  <si>
-    <t>You should not delete the mandatory “other” group</t>
-  </si>
-  <si>
-    <t>Options</t>
-  </si>
-  <si>
-    <t>This tab contains the list of options for select attributes.</t>
-  </si>
-  <si>
-    <t>This tab can be duplicated to divide the contents by attribute. All options tab titles should start with "options"</t>
-  </si>
-  <si>
-    <t>Channels</t>
-  </si>
-  <si>
-    <t>This tab contains all information about channels.</t>
-  </si>
-  <si>
-    <t>After editing this tab, you might have to update your family tabs so they use the right family codes</t>
-  </si>
-  <si>
-    <t>Categories</t>
-  </si>
-  <si>
-    <t>This tab contains all information about categories</t>
-  </si>
-  <si>
-    <t>This tab can be duplicated to divide its content between trees. All category tabs should start with "categories"</t>
-  </si>
-  <si>
-    <t>Association types</t>
-  </si>
-  <si>
-    <t>This tab contains all information about association types</t>
-  </si>
-  <si>
-    <t>Group types</t>
-  </si>
-  <si>
-    <t>This tab contains all information about group types</t>
-  </si>
-  <si>
-    <t>Integrator HOWTO</t>
-  </si>
-  <si>
-    <t>All tabs contain a hidden row with the codes of the properties. If you add some columns, do not forget to update them.</t>
-  </si>
-  <si>
-    <t>The codes for label translations are always of the form "label-&lt;locale&gt;". For example, the french label has the code "label-fr_FR"</t>
-  </si>
-  <si>
-    <t>Common and unaffected attribute properties</t>
-  </si>
-  <si>
-    <t>Labels</t>
-  </si>
-  <si>
-    <t>Attribute properties</t>
-  </si>
-  <si>
-    <t>Attribute code</t>
-  </si>
-  <si>
-    <t>en_US</t>
-  </si>
-  <si>
-    <t>Attribute type</t>
-  </si>
-  <si>
-    <t>Attribute group</t>
-  </si>
-  <si>
-    <t>Sort order</t>
-  </si>
-  <si>
-    <t>Is unique*</t>
-  </si>
-  <si>
-    <t>Is localizable*</t>
-  </si>
-  <si>
-    <t>Specific to locales</t>
-  </si>
-  <si>
-    <t>Is scopable*</t>
-  </si>
-  <si>
-    <t>Useable as grid filter*</t>
-  </si>
-  <si>
-    <t>Max characters</t>
-  </si>
-  <si>
-    <t>Validation rule</t>
-  </si>
-  <si>
-    <t>Validation regexp</t>
-  </si>
-  <si>
-    <t>Rich text</t>
-  </si>
-  <si>
-    <t>Minimum number</t>
-  </si>
-  <si>
-    <t>Maximum number</t>
-  </si>
-  <si>
-    <t>Decimals allowed</t>
-  </si>
-  <si>
-    <t>Negative allowed</t>
-  </si>
-  <si>
-    <t>Minimum date</t>
-  </si>
-  <si>
-    <t>Maximum date</t>
-  </si>
-  <si>
-    <t>Metric family</t>
-  </si>
-  <si>
-    <t>Default metric  unit</t>
-  </si>
-  <si>
-    <t>Max file size</t>
-  </si>
-  <si>
-    <t>Allowed extensions</t>
-  </si>
-  <si>
-    <t>Minimum input length</t>
-  </si>
-  <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>label-en_US</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>group</t>
-  </si>
-  <si>
-    <t>sort_order</t>
-  </si>
-  <si>
-    <t>unique</t>
-  </si>
-  <si>
-    <t>localizable</t>
-  </si>
-  <si>
-    <t>available_locales</t>
-  </si>
-  <si>
-    <t>scopable</t>
-  </si>
-  <si>
-    <t>useable_as_grid_filter</t>
-  </si>
-  <si>
-    <t>max_characters</t>
-  </si>
-  <si>
-    <t>validation_rule</t>
-  </si>
-  <si>
-    <t>validation_regexp</t>
-  </si>
-  <si>
-    <t>wysiwyg_enabled</t>
-  </si>
-  <si>
-    <t>number_min</t>
-  </si>
-  <si>
-    <t>number_max</t>
-  </si>
-  <si>
-    <t>decimals_allowed</t>
-  </si>
-  <si>
-    <t>negative_allowed</t>
-  </si>
-  <si>
-    <t>date_min</t>
-  </si>
-  <si>
-    <t>date_max</t>
-  </si>
-  <si>
-    <t>metric_family</t>
-  </si>
-  <si>
-    <t>default_metric_unit</t>
-  </si>
-  <si>
-    <t>max_file_size</t>
-  </si>
-  <si>
-    <t>allowed_extensions</t>
-  </si>
-  <si>
-    <t>minimum_input length</t>
-  </si>
-  <si>
-    <t>sku</t>
-  </si>
-  <si>
-    <t>Code article</t>
-  </si>
-  <si>
-    <t>Identifier</t>
-  </si>
-  <si>
-    <t>global</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>Family code</t>
-  </si>
-  <si>
-    <t>main</t>
-  </si>
-  <si>
-    <t>Label</t>
-  </si>
-  <si>
-    <t>Main</t>
-  </si>
-  <si>
-    <t>Completeness</t>
-  </si>
-  <si>
-    <t>Use as label</t>
-  </si>
-  <si>
-    <t>use_as_label</t>
-  </si>
-  <si>
-    <t>second_family</t>
-  </si>
-  <si>
-    <t>Second family</t>
-  </si>
-  <si>
-    <t>Group properties</t>
-  </si>
-  <si>
-    <t>Group code</t>
-  </si>
-  <si>
-    <t>Position</t>
-  </si>
-  <si>
-    <t>Global</t>
-  </si>
-  <si>
-    <t>other</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Option properties</t>
-  </si>
-  <si>
-    <t>Option code</t>
-  </si>
-  <si>
-    <t>attribute</t>
-  </si>
-  <si>
-    <t>Channel properties</t>
-  </si>
-  <si>
-    <t>Channel code</t>
-  </si>
-  <si>
-    <t>Channel label</t>
-  </si>
-  <si>
-    <t>Channel locales</t>
-  </si>
-  <si>
-    <t>Channel currencies</t>
-  </si>
-  <si>
-    <t>Category tree</t>
-  </si>
-  <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>locales</t>
-  </si>
-  <si>
-    <t>currencies</t>
-  </si>
-  <si>
-    <t>tree</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>Category properties</t>
-  </si>
-  <si>
-    <t>Category code</t>
-  </si>
-  <si>
-    <t>Parent category code</t>
-  </si>
-  <si>
-    <t>parent</t>
-  </si>
-  <si>
-    <t>Main category</t>
-  </si>
-  <si>
-    <t>Group type properties</t>
-  </si>
-  <si>
-    <t>variant</t>
-  </si>
-  <si>
-    <t>VARIANT</t>
-  </si>
-  <si>
-    <t>RELATED</t>
-  </si>
-  <si>
-    <t>Association type properties</t>
-  </si>
-  <si>
-    <t>Association type code</t>
-  </si>
-  <si>
-    <t>X_SELL</t>
-  </si>
-  <si>
-    <t>Cross sell</t>
-  </si>
-  <si>
-    <t>UPSELL</t>
-  </si>
-  <si>
-    <t>Upsell</t>
-  </si>
-  <si>
-    <t>SUBSTITUTION</t>
-  </si>
-  <si>
-    <t>Substitution</t>
-  </si>
-  <si>
-    <t>PACK</t>
-  </si>
-  <si>
-    <t>Pack</t>
-  </si>
-  <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>regexp</t>
-  </si>
-  <si>
-    <t>datetime</t>
-  </si>
-  <si>
-    <t>Attribute type code</t>
-  </si>
-  <si>
-    <t>Attribute type label</t>
-  </si>
-  <si>
-    <t>pim_catalog_identifier</t>
-  </si>
-  <si>
-    <t>pim_catalog_text</t>
-  </si>
-  <si>
-    <t>pim_catalog_textarea</t>
-  </si>
-  <si>
-    <t>Text area</t>
-  </si>
-  <si>
-    <t>pim_catalog_multiselect</t>
-  </si>
-  <si>
-    <t>Multiple select</t>
-  </si>
-  <si>
-    <t>pim_catalog_simpleselect</t>
-  </si>
-  <si>
-    <t>Simple select</t>
-  </si>
-  <si>
-    <t>pim_catalog_price_collection</t>
-  </si>
-  <si>
-    <t>Price collection</t>
-  </si>
-  <si>
-    <t>pim_catalog_number</t>
-  </si>
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>pim_catalog_boolean</t>
-  </si>
-  <si>
-    <t>Boolean</t>
-  </si>
-  <si>
-    <t>pim_catalog_date</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>pim_catalog_file</t>
-  </si>
-  <si>
-    <t>File</t>
-  </si>
-  <si>
-    <t>pim_catalog_image</t>
-  </si>
-  <si>
-    <t>Image</t>
-  </si>
-  <si>
-    <t>pim_catalog_metric</t>
-  </si>
-  <si>
-    <t>Metric</t>
-  </si>
-  <si>
-    <t>Area</t>
-  </si>
-  <si>
-    <t>Binary</t>
-  </si>
-  <si>
-    <t>Frequency</t>
-  </si>
-  <si>
-    <t>Length</t>
-  </si>
-  <si>
-    <t>Power</t>
-  </si>
-  <si>
-    <t>Speed</t>
-  </si>
-  <si>
-    <t>Temperature</t>
-  </si>
-  <si>
-    <t>Volume</t>
-  </si>
-  <si>
-    <t>Weight</t>
-  </si>
-  <si>
-    <t>Voltage</t>
-  </si>
-  <si>
-    <t>Intensity</t>
-  </si>
-  <si>
-    <t>Resistance</t>
-  </si>
-  <si>
-    <t>unit</t>
-  </si>
-  <si>
-    <t>ACRE</t>
-  </si>
-  <si>
-    <t>ARE</t>
-  </si>
-  <si>
-    <t>ARPENT</t>
-  </si>
-  <si>
-    <t>CENTIARE</t>
-  </si>
-  <si>
-    <t>HECTARE</t>
-  </si>
-  <si>
-    <t>SQUARE_CENTIMETER</t>
-  </si>
-  <si>
-    <t>SQUARE_DECIMETER</t>
-  </si>
-  <si>
-    <t>SQUARE_DEKAMETER</t>
-  </si>
-  <si>
-    <t>SQUARE_FOOT</t>
-  </si>
-  <si>
-    <t>SQUARE_FURLONG</t>
-  </si>
-  <si>
-    <t>SQUARE_HECTOMETER</t>
-  </si>
-  <si>
-    <t>SQUARE_INCH</t>
-  </si>
-  <si>
-    <t>SQUARE_KILOMETER</t>
-  </si>
-  <si>
-    <t>SQUARE_METER</t>
-  </si>
-  <si>
-    <t>SQUARE_MIL</t>
-  </si>
-  <si>
-    <t>SQUARE_MILE</t>
-  </si>
-  <si>
-    <t>SQUARE_MILLIMETER</t>
-  </si>
-  <si>
-    <t>SQUARE_YARD</t>
-  </si>
-  <si>
-    <t>BIT</t>
-  </si>
-  <si>
-    <t>BYTE</t>
-  </si>
-  <si>
-    <t>KILOBYTE</t>
-  </si>
-  <si>
-    <t>MEGABYTE</t>
-  </si>
-  <si>
-    <t>GIGABYTE</t>
-  </si>
-  <si>
-    <t>TERABYTE</t>
-  </si>
-  <si>
-    <t>GIGAHERTZ</t>
-  </si>
-  <si>
-    <t>KILOHERTZ</t>
-  </si>
-  <si>
-    <t>MEGAHERTZ</t>
-  </si>
-  <si>
-    <t>TERAHERTZ</t>
-  </si>
-  <si>
-    <t>HERTZ</t>
-  </si>
-  <si>
-    <t>CENTIMETER</t>
-  </si>
-  <si>
-    <t>CHAIN</t>
-  </si>
-  <si>
-    <t>DECIMETER</t>
-  </si>
-  <si>
-    <t>DEKAMETER</t>
-  </si>
-  <si>
-    <t>FEET</t>
-  </si>
-  <si>
-    <t>FURLONG</t>
-  </si>
-  <si>
-    <t>INCH</t>
-  </si>
-  <si>
-    <t>HECTOMETER</t>
-  </si>
-  <si>
-    <t>KILOMETER</t>
-  </si>
-  <si>
-    <t>METER</t>
-  </si>
-  <si>
-    <t>MIL</t>
-  </si>
-  <si>
-    <t>MILE</t>
-  </si>
-  <si>
-    <t>MILLIMETER</t>
-  </si>
-  <si>
-    <t>YARD</t>
-  </si>
-  <si>
-    <t>GIGAWATT</t>
-  </si>
-  <si>
-    <t>KILOWATT</t>
-  </si>
-  <si>
-    <t>MEGAWATT</t>
-  </si>
-  <si>
-    <t>TERAWATT</t>
-  </si>
-  <si>
-    <t>WATT</t>
-  </si>
-  <si>
-    <t>FOOT_PER_SECOND</t>
-  </si>
-  <si>
-    <t>FOOT_PER_HOUR</t>
-  </si>
-  <si>
-    <t>KILOMETER_PER_HOUR</t>
-  </si>
-  <si>
-    <t>METER_PER_HOUR</t>
-  </si>
-  <si>
-    <t>METER_PER_MINUTE</t>
-  </si>
-  <si>
-    <t>METER_PER_SECOND</t>
-  </si>
-  <si>
-    <t>MILE_PER_HOUR</t>
-  </si>
-  <si>
-    <t>YARD_PER_HOUR</t>
-  </si>
-  <si>
-    <t>CELSIUS</t>
-  </si>
-  <si>
-    <t>FAHRENHEIT</t>
-  </si>
-  <si>
-    <t>KELVIN</t>
-  </si>
-  <si>
-    <t>RANKINE</t>
-  </si>
-  <si>
-    <t>REAUMUR</t>
-  </si>
-  <si>
-    <t>BARREL</t>
-  </si>
-  <si>
-    <t>CENTILITER</t>
-  </si>
-  <si>
-    <t>CUBIC_CENTIMETER</t>
-  </si>
-  <si>
-    <t>CUBIC_DECIMETER</t>
-  </si>
-  <si>
-    <t>CUBIC_FOOT</t>
-  </si>
-  <si>
-    <t>CUBIC_INCH</t>
-  </si>
-  <si>
-    <t>CUBIC_METER</t>
-  </si>
-  <si>
-    <t>CUBIC_MILLIMETER</t>
-  </si>
-  <si>
-    <t>CUBIC_YARD</t>
-  </si>
-  <si>
-    <t>DECILITER</t>
-  </si>
-  <si>
-    <t>GALLON</t>
-  </si>
-  <si>
-    <t>LITER</t>
-  </si>
-  <si>
-    <t>MILLILITER</t>
-  </si>
-  <si>
-    <t>OUNCE</t>
-  </si>
-  <si>
-    <t>PINT</t>
-  </si>
-  <si>
-    <t>DENIER</t>
-  </si>
-  <si>
-    <t>GRAIN</t>
-  </si>
-  <si>
-    <t>GRAM</t>
-  </si>
-  <si>
-    <t>KILOGRAM</t>
-  </si>
-  <si>
-    <t>LIVRE</t>
-  </si>
-  <si>
-    <t>MARC</t>
-  </si>
-  <si>
-    <t>MILLIGRAM</t>
-  </si>
-  <si>
-    <t>ONCE</t>
-  </si>
-  <si>
-    <t>POUND</t>
-  </si>
-  <si>
-    <t>TON</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="401">
+  <si>
+    <t xml:space="preserve">End user HOWTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Global rules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do not modify the headers of the files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do not open this file in Open Office, as it will break the validation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do not save this file with another extension than xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do not modify hidden rows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attributes tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The attributes tab can be used to define the properties of attributes which are not linked to families, or which are shared by families.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This tab can be duplicated to shorten the list. All attributes tab titles should start with "attributes"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family tabs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The family tab contains all information for a family : code, labels, attributes and completion rules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To create a new family, simply duplicate the tab. All family tabs titles must start with "family"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If an attribute is present in multiple families, only fill the blue and pink columns (attribute properties and translations) once </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To add completion for other channels, simply add columns on the right of the table. The label should be the code of the channel.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attribute groups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This tab contains all informations for attribute groups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You should not delete the mandatory “other” group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This tab contains the list of options for select attributes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This tab can be duplicated to divide the contents by attribute. All options tab titles should start with "options"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This tab contains all information about channels.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After editing this tab, you might have to update your family tabs so they use the right family codes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Categories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This tab contains all information about categories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This tab can be duplicated to divide its content between trees. All category tabs should start with "categories"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Association types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This tab contains all information about association types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This tab contains all information about group types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrator HOWTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All tabs contain a hidden row with the codes of the properties. If you add some columns, do not forget to update them.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The codes for label translations are always of the form "label-&lt;locale&gt;". For example, the french label has the code "label-fr_FR"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Common and unaffected attribute properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Labels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attribute properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attribute code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">en_US</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attribute type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attribute group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sort order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is unique*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is localizable*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specific to locales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is scopable*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Useable as grid filter*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validation rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validation regexp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rich text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decimals allowed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Negative allowed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metric family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default metric  unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max file size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allowed extensions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum input length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label-en_US</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sort_order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">localizable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">available_locales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scopable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">useable_as_grid_filter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validation_rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validation_regexp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wysiwyg_enabled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number_min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number_max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">decimals_allowed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">negative_allowed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metric_family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default_metric_unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_file_size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allowed_extensions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimum_input length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code article</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">global</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">main</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Completeness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use as label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use_as_label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">second_family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Second family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Global</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Option properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Option code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">attribute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel locales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel currencies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">currencies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parent category code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group type properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">variant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VARIANT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RELATED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Association type properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Association type code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X_SELL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cross sell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPSELL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upsell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUBSTITUTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Substitution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regexp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">datetime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attribute type code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attribute type label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pim_catalog_identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pim_catalog_text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pim_catalog_textarea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pim_catalog_multiselect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiple select</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pim_catalog_simpleselect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simple select</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pim_catalog_price_collection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price collection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pim_catalog_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pim_catalog_boolean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boolean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pim_catalog_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pim_catalog_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pim_catalog_image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pim_catalog_metric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Binary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intensity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARPENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CENTIARE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HECTARE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQUARE_CENTIMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQUARE_DECIMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQUARE_DEKAMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQUARE_FOOT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQUARE_FURLONG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQUARE_HECTOMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQUARE_INCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQUARE_KILOMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQUARE_METER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQUARE_MIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQUARE_MILE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQUARE_MILLIMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQUARE_YARD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BYTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KILOBYTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEGABYTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIGABYTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TERABYTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIGAHERTZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KILOHERTZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEGAHERTZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TERAHERTZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HERTZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CENTIMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHAIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DECIMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEKAMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FEET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FURLONG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HECTOMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KILOMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">METER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MILE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MILLIMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YARD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIGAWATT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KILOWATT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEGAWATT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TERAWATT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WATT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FOOT_PER_SECOND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FOOT_PER_HOUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KILOMETER_PER_HOUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">METER_PER_HOUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">METER_PER_MINUTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">METER_PER_SECOND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MILE_PER_HOUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YARD_PER_HOUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CELSIUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAHRENHEIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KELVIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RANKINE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REAUMUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BARREL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CENTILITER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUBIC_CENTIMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUBIC_DECIMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUBIC_FOOT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUBIC_INCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUBIC_METER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUBIC_MILLIMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUBIC_YARD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DECILITER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GALLON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LITER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MILLILITER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUNCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PINT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DENIER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRAIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KILOGRAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIVRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MILLIGRAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ONCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POUND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it_support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">redactor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redactor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROLE_ADMINISTRATOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROLE_CATALOG_MANAGER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Catalog manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROLE_USER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">first_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">last_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">catalog_locale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user_locale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">catalog_scope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default_tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">groups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enabled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AFA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AOK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AZM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BEC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BEF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BGL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BGM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BGO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BYB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EEK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GHC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GYD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IEP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KRH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LUF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LVR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MGF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MKN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MXP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MZE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MZM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UYP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VEB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VNN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XAU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XBA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XBB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XBC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XBD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XEU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XFO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XFU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XPD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XDR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XSU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XXX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YUD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YUN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZMK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZRN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZRZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZWD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZWL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZWR</t>
   </si>
 </sst>
 </file>
@@ -1085,7 +1482,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -1421,9 +1818,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>380880</xdr:colOff>
+      <xdr:colOff>379440</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>141120</xdr:rowOff>
+      <xdr:rowOff>139680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1433,7 +1830,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="6160680" cy="9530640"/>
+          <a:ext cx="6006960" cy="9529200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1466,9 +1863,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>380880</xdr:colOff>
+      <xdr:colOff>379440</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>141120</xdr:rowOff>
+      <xdr:rowOff>139680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1478,7 +1875,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="6160680" cy="9530640"/>
+          <a:ext cx="6006960" cy="9529200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1516,9 +1913,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>133200</xdr:colOff>
+      <xdr:colOff>131760</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>141480</xdr:rowOff>
+      <xdr:rowOff>140040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1528,7 +1925,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="5865480" cy="10200960"/>
+          <a:ext cx="5597280" cy="10199520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1561,9 +1958,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>133200</xdr:colOff>
+      <xdr:colOff>131760</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>141480</xdr:rowOff>
+      <xdr:rowOff>140040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1573,7 +1970,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="5865480" cy="10200960"/>
+          <a:ext cx="5597280" cy="10199520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1611,9 +2008,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>380880</xdr:colOff>
+      <xdr:colOff>379800</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>141120</xdr:rowOff>
+      <xdr:rowOff>140040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1623,7 +2020,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="6760800" cy="9530640"/>
+          <a:ext cx="6940800" cy="9529560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1656,9 +2053,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>380880</xdr:colOff>
+      <xdr:colOff>379800</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>141120</xdr:rowOff>
+      <xdr:rowOff>140040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1668,7 +2065,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="6760800" cy="9530640"/>
+          <a:ext cx="6940800" cy="9529560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1702,13 +2099,13 @@
   </sheetPr>
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.32142857142857"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1906,8 +2303,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="47.1122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="44.8163265306122"/>
   </cols>
   <sheetData>
     <row r="1" s="28" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2050,8 +2447,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
@@ -2191,8 +2588,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
@@ -2332,8 +2729,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
@@ -3045,6 +3442,1087 @@
       </c>
       <c r="B89" s="0" t="s">
         <v>269</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M10" activeCellId="0" sqref="M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>277</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.0357142857143"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>284</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.50510204081633"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B102"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>332</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>338</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>342</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>345</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>357</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="B63" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>362</v>
+      </c>
+      <c r="B64" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="B65" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>364</v>
+      </c>
+      <c r="B66" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="B67" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>366</v>
+      </c>
+      <c r="B68" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="B69" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>368</v>
+      </c>
+      <c r="B70" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="B71" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="B72" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="B73" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>372</v>
+      </c>
+      <c r="B74" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="B75" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="B76" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="B77" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="B78" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="B79" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="B80" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>379</v>
+      </c>
+      <c r="B81" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="B82" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>381</v>
+      </c>
+      <c r="B83" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="B84" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="B85" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="B86" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="B87" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="B88" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="B89" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>388</v>
+      </c>
+      <c r="B90" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="B91" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="B92" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="B93" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="B94" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>393</v>
+      </c>
+      <c r="B95" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="B96" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>395</v>
+      </c>
+      <c r="B97" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="B98" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>397</v>
+      </c>
+      <c r="B99" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="B100" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="B101" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="B102" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3065,39 +4543,39 @@
   </sheetPr>
   <dimension ref="A1:AV8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="7" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="8" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="48" min="47" style="7" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="7" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="8" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="48" min="47" style="7" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3479,46 +4957,46 @@
   </sheetPr>
   <dimension ref="A1:AX7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="13.5"/>
-    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="12.1479591836735"/>
     <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="15.2551020408163"/>
     <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.50510204081633"/>
     <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.23469387755102"/>
   </cols>
@@ -3905,40 +5383,40 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="13.5"/>
-    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="12.1479591836735"/>
     <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="15.2551020408163"/>
     <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.50510204081633"/>
     <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.23469387755102"/>
   </cols>
@@ -4312,9 +5790,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="15.2551020408163"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
@@ -4398,8 +5876,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
@@ -4457,16 +5935,16 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="15.2551020408163"/>
     <col collapsed="false" hidden="false" max="1016" min="6" style="0" width="8.50510204081633"/>
     <col collapsed="false" hidden="false" max="1025" min="1017" style="0" width="8.23469387755102"/>
   </cols>
@@ -4566,9 +6044,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4644,8 +6123,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3061224489796"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Excel init - fix empty data issue
</commit_message>
<xml_diff>
--- a/src/Resources/fixtures/minimal/init.xlsx
+++ b/src/Resources/fixtures/minimal/init.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -1871,9 +1871,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>379800</xdr:colOff>
+      <xdr:colOff>379440</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>140400</xdr:rowOff>
+      <xdr:rowOff>140040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1883,7 +1883,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="6417000" cy="9529920"/>
+          <a:ext cx="6483240" cy="9529560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1916,9 +1916,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>379800</xdr:colOff>
+      <xdr:colOff>379440</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>140400</xdr:rowOff>
+      <xdr:rowOff>140040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1928,7 +1928,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="6417000" cy="9529920"/>
+          <a:ext cx="6483240" cy="9529560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1967,8 +1967,8 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>132480</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>140760</xdr:rowOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>140400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1978,7 +1978,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="5674320" cy="9921960"/>
+          <a:ext cx="5598000" cy="8420760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2012,8 +2012,8 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>132480</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>140760</xdr:rowOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>140400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2023,7 +2023,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="5674320" cy="9921960"/>
+          <a:ext cx="5598000" cy="8420760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2061,9 +2061,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>380160</xdr:colOff>
+      <xdr:colOff>379800</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>140400</xdr:rowOff>
+      <xdr:rowOff>140040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2073,7 +2073,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="8341200" cy="9529920"/>
+          <a:ext cx="8407440" cy="9529560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2106,9 +2106,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>380160</xdr:colOff>
+      <xdr:colOff>379800</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>140400</xdr:rowOff>
+      <xdr:rowOff>140040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2118,7 +2118,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="8341200" cy="9529920"/>
+          <a:ext cx="8407440" cy="9529560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2152,15 +2152,14 @@
   </sheetPr>
   <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B62" activeCellId="0" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.45408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="112.862244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.32142857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="111.637755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2381,9 +2380,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="28" width="31.0459183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="32" width="31.0459183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="28" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="32" width="30.6428571428571"/>
   </cols>
   <sheetData>
     <row r="1" s="33" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2472,8 +2470,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2540,8 +2539,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2600,18 +2600,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="28.3469387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.9438775510204"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2714,8 +2714,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3557,9 +3558,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -3615,9 +3613,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3756,9 +3754,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3897,9 +3895,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4636,36 +4634,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="44" min="26" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="7" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="8" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="48" min="47" style="7" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="49" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="7" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="8" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="48" min="47" style="7" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5057,43 +5052,43 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5482,42 +5477,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="6" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="6" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5893,9 +5888,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="28" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="28" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5978,9 +5974,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="28" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="28" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6036,18 +6033,19 @@
   </sheetPr>
   <dimension ref="A1:E65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="28" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="24" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="24" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="1017" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="28" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="24" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="24" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1016" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1017" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="49.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6067,7 +6065,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="9.3" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="9.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="21" t="s">
         <v>61</v>
       </c>
@@ -6101,6 +6099,16 @@
         <v>94</v>
       </c>
     </row>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="1">
@@ -6134,9 +6142,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="28" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="28" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.9438775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6212,9 +6221,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="28" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="28" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3061224489796"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Fix group types to correctly set `is_variant` Delete fixtures from the example bundle for maintenance purpose
</commit_message>
<xml_diff>
--- a/src/Resources/fixtures/minimal/init.xlsx
+++ b/src/Resources/fixtures/minimal/init.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="README-EN" sheetId="1" state="visible" r:id="rId2"/>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="447">
   <si>
     <t xml:space="preserve">End user HOWTO</t>
   </si>
@@ -672,6 +672,9 @@
   </si>
   <si>
     <t xml:space="preserve">variant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is_variant</t>
   </si>
   <si>
     <t xml:space="preserve">VARIANT</t>
@@ -1900,9 +1903,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>378360</xdr:colOff>
+      <xdr:colOff>377640</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>138960</xdr:rowOff>
+      <xdr:rowOff>138240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1912,7 +1915,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="6205680" cy="9528480"/>
+          <a:ext cx="6157440" cy="9527760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1945,9 +1948,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>378360</xdr:colOff>
+      <xdr:colOff>377640</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>138960</xdr:rowOff>
+      <xdr:rowOff>138240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1957,7 +1960,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="6205680" cy="9528480"/>
+          <a:ext cx="6157440" cy="9527760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1995,9 +1998,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>131400</xdr:colOff>
+      <xdr:colOff>130680</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>138960</xdr:rowOff>
+      <xdr:rowOff>138240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2007,7 +2010,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="6035040" cy="8419680"/>
+          <a:ext cx="5853240" cy="8418960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2040,9 +2043,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>131400</xdr:colOff>
+      <xdr:colOff>130680</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>138960</xdr:rowOff>
+      <xdr:rowOff>138240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2052,7 +2055,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="6035040" cy="8419680"/>
+          <a:ext cx="5853240" cy="8418960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2090,9 +2093,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>378720</xdr:colOff>
+      <xdr:colOff>378000</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>138960</xdr:rowOff>
+      <xdr:rowOff>138240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2102,7 +2105,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="8082720" cy="9528480"/>
+          <a:ext cx="8034120" cy="9527760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2135,9 +2138,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>378720</xdr:colOff>
+      <xdr:colOff>378000</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>138960</xdr:rowOff>
+      <xdr:rowOff>138240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2147,7 +2150,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="8082720" cy="9528480"/>
+          <a:ext cx="8034120" cy="9527760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2182,14 +2185,14 @@
   <dimension ref="A1:B58"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J25" activeCellId="0" sqref="J25"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="3:3 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="107.724489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.59183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="113.663265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2404,15 +2407,15 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="3:3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2429,17 +2432,17 @@
         <v>174</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="32" t="s">
         <v>93</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="29" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -2447,7 +2450,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -2481,19 +2484,19 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="1" sqref="3:3 B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="34" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="34" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="35" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B1" s="31" t="s">
         <v>67</v>
@@ -2501,7 +2504,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="36" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B2" s="31" t="s">
         <v>130</v>
@@ -2517,34 +2520,34 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="29" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="29" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="29" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2572,13 +2575,14 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2591,34 +2595,34 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -2640,18 +2644,19 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="38" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B1" s="38" t="s">
         <v>159</v>
@@ -2659,26 +2664,26 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2700,78 +2705,77 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="3:3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="38" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C1" s="38" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D1" s="38" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E1" s="38" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F1" s="38" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G1" s="38" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H1" s="38" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="I1" s="38" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="J1" s="38" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="K1" s="38" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="L1" s="38" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>215</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>216</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>214</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>130</v>
@@ -2786,10 +2790,10 @@
         <v>133</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="L2" s="0" t="n">
         <v>1</v>
@@ -2814,13 +2818,13 @@
   <dimension ref="A1:B102"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+      <selection pane="topLeft" activeCell="H12" activeCellId="1" sqref="3:3 H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2828,7 +2832,7 @@
         <v>93</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2841,7 +2845,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -2849,7 +2853,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0</v>
@@ -2857,7 +2861,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -2865,7 +2869,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0</v>
@@ -2873,7 +2877,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0</v>
@@ -2881,7 +2885,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
@@ -2889,7 +2893,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0</v>
@@ -2897,7 +2901,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0</v>
@@ -2905,7 +2909,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0</v>
@@ -2913,7 +2917,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0</v>
@@ -2921,7 +2925,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0</v>
@@ -2929,7 +2933,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0</v>
@@ -2937,7 +2941,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0</v>
@@ -2945,7 +2949,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0</v>
@@ -2953,7 +2957,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0</v>
@@ -2961,7 +2965,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0</v>
@@ -2969,7 +2973,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0</v>
@@ -2977,7 +2981,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0</v>
@@ -2985,7 +2989,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0</v>
@@ -2993,7 +2997,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0</v>
@@ -3001,7 +3005,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>0</v>
@@ -3009,7 +3013,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>0</v>
@@ -3017,7 +3021,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>0</v>
@@ -3025,7 +3029,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>0</v>
@@ -3033,7 +3037,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>0</v>
@@ -3041,7 +3045,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>0</v>
@@ -3049,7 +3053,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0</v>
@@ -3057,7 +3061,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>0</v>
@@ -3065,7 +3069,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>0</v>
@@ -3073,7 +3077,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>0</v>
@@ -3081,7 +3085,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>0</v>
@@ -3089,7 +3093,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>0</v>
@@ -3097,7 +3101,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>0</v>
@@ -3105,7 +3109,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>0</v>
@@ -3113,7 +3117,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>0</v>
@@ -3121,7 +3125,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>0</v>
@@ -3129,7 +3133,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>0</v>
@@ -3137,7 +3141,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>0</v>
@@ -3145,7 +3149,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>0</v>
@@ -3153,7 +3157,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>0</v>
@@ -3161,7 +3165,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>0</v>
@@ -3169,7 +3173,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>0</v>
@@ -3177,7 +3181,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>0</v>
@@ -3185,7 +3189,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>0</v>
@@ -3193,7 +3197,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>0</v>
@@ -3201,7 +3205,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>0</v>
@@ -3209,7 +3213,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>0</v>
@@ -3217,7 +3221,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>0</v>
@@ -3225,7 +3229,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>0</v>
@@ -3233,7 +3237,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>0</v>
@@ -3241,7 +3245,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>0</v>
@@ -3249,7 +3253,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>0</v>
@@ -3257,7 +3261,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>0</v>
@@ -3265,7 +3269,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>0</v>
@@ -3273,7 +3277,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>0</v>
@@ -3281,7 +3285,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>0</v>
@@ -3289,7 +3293,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>0</v>
@@ -3297,7 +3301,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>0</v>
@@ -3305,7 +3309,7 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>0</v>
@@ -3313,7 +3317,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>0</v>
@@ -3321,7 +3325,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>0</v>
@@ -3329,7 +3333,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>0</v>
@@ -3337,7 +3341,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>0</v>
@@ -3345,7 +3349,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>0</v>
@@ -3353,7 +3357,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>0</v>
@@ -3361,7 +3365,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>0</v>
@@ -3369,7 +3373,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>0</v>
@@ -3377,7 +3381,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>0</v>
@@ -3385,7 +3389,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>0</v>
@@ -3393,7 +3397,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>0</v>
@@ -3401,7 +3405,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>0</v>
@@ -3409,7 +3413,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>0</v>
@@ -3417,7 +3421,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>0</v>
@@ -3425,7 +3429,7 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>0</v>
@@ -3433,7 +3437,7 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>0</v>
@@ -3441,7 +3445,7 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>0</v>
@@ -3449,7 +3453,7 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>0</v>
@@ -3457,7 +3461,7 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>0</v>
@@ -3465,7 +3469,7 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B81" s="0" t="n">
         <v>0</v>
@@ -3473,7 +3477,7 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>0</v>
@@ -3481,7 +3485,7 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>0</v>
@@ -3489,7 +3493,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>0</v>
@@ -3497,7 +3501,7 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B85" s="0" t="n">
         <v>0</v>
@@ -3505,7 +3509,7 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B86" s="0" t="n">
         <v>0</v>
@@ -3513,7 +3517,7 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B87" s="0" t="n">
         <v>0</v>
@@ -3521,7 +3525,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B88" s="0" t="n">
         <v>0</v>
@@ -3529,7 +3533,7 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B89" s="0" t="n">
         <v>0</v>
@@ -3537,7 +3541,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B90" s="0" t="n">
         <v>0</v>
@@ -3545,7 +3549,7 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B91" s="0" t="n">
         <v>0</v>
@@ -3553,7 +3557,7 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B92" s="0" t="n">
         <v>0</v>
@@ -3561,7 +3565,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B93" s="0" t="n">
         <v>0</v>
@@ -3569,7 +3573,7 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B94" s="0" t="n">
         <v>0</v>
@@ -3577,7 +3581,7 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B95" s="0" t="n">
         <v>0</v>
@@ -3585,7 +3589,7 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B96" s="0" t="n">
         <v>0</v>
@@ -3593,7 +3597,7 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B97" s="0" t="n">
         <v>0</v>
@@ -3601,7 +3605,7 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B98" s="0" t="n">
         <v>0</v>
@@ -3609,7 +3613,7 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B99" s="0" t="n">
         <v>0</v>
@@ -3617,7 +3621,7 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B100" s="0" t="n">
         <v>0</v>
@@ -3625,7 +3629,7 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B101" s="0" t="n">
         <v>0</v>
@@ -3633,7 +3637,7 @@
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B102" s="0" t="n">
         <v>0</v>
@@ -3658,12 +3662,12 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="3:3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3671,10 +3675,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3682,18 +3686,18 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -3715,22 +3719,21 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="32" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3743,7 +3746,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>122</v>
@@ -3751,7 +3754,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>126</v>
@@ -3759,7 +3762,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>129</v>
@@ -3767,74 +3770,74 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -3856,22 +3859,21 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="32" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3884,98 +3886,98 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -3997,19 +3999,18 @@
   <dimension ref="A1:B89"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="32" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B1" s="32"/>
     </row>
@@ -4018,703 +4019,703 @@
         <v>96</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
   </sheetData>
@@ -4735,15 +4736,13 @@
   </sheetPr>
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B30" activeCellId="1" sqref="3:3 B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="178.127551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="174.137755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4936,42 +4935,42 @@
   <dimension ref="A1:AW9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+      <selection pane="topLeft" activeCell="B25" activeCellId="1" sqref="3:3 B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="45" min="27" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="7" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="8" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="49" min="48" style="7" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="50" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="45" min="27" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="7" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="8" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="49" min="48" style="7" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="50" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5410,48 +5409,48 @@
   <dimension ref="A1:AX8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="3:3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5731,47 +5730,47 @@
   <dimension ref="A1:BE7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="1" sqref="3:3 C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="6" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="6" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6041,14 +6040,15 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="1" sqref="3:3 C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6126,14 +6126,15 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6190,17 +6191,17 @@
   <dimension ref="A1:E65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="1" sqref="3:3 E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="23" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="1017" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="23" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1016" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="49.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6309,14 +6310,15 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
+      <selection pane="topLeft" activeCell="H18" activeCellId="1" sqref="3:3 H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Fix group types (#23)
* Fix group types to correctly set `is_variant`
* Delete fixtures from the example bundle for maintenance purpose
</commit_message>
<xml_diff>
--- a/src/Resources/fixtures/minimal/init.xlsx
+++ b/src/Resources/fixtures/minimal/init.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="README-EN" sheetId="1" state="visible" r:id="rId2"/>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="447">
   <si>
     <t xml:space="preserve">End user HOWTO</t>
   </si>
@@ -672,6 +672,9 @@
   </si>
   <si>
     <t xml:space="preserve">variant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is_variant</t>
   </si>
   <si>
     <t xml:space="preserve">VARIANT</t>
@@ -1900,9 +1903,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>378360</xdr:colOff>
+      <xdr:colOff>377640</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>138960</xdr:rowOff>
+      <xdr:rowOff>138240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1912,7 +1915,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="6205680" cy="9528480"/>
+          <a:ext cx="6157440" cy="9527760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1945,9 +1948,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>378360</xdr:colOff>
+      <xdr:colOff>377640</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>138960</xdr:rowOff>
+      <xdr:rowOff>138240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1957,7 +1960,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="6205680" cy="9528480"/>
+          <a:ext cx="6157440" cy="9527760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1995,9 +1998,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>131400</xdr:colOff>
+      <xdr:colOff>130680</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>138960</xdr:rowOff>
+      <xdr:rowOff>138240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2007,7 +2010,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="6035040" cy="8419680"/>
+          <a:ext cx="5853240" cy="8418960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2040,9 +2043,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>131400</xdr:colOff>
+      <xdr:colOff>130680</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>138960</xdr:rowOff>
+      <xdr:rowOff>138240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2052,7 +2055,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="6035040" cy="8419680"/>
+          <a:ext cx="5853240" cy="8418960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2090,9 +2093,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>378720</xdr:colOff>
+      <xdr:colOff>378000</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>138960</xdr:rowOff>
+      <xdr:rowOff>138240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2102,7 +2105,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="8082720" cy="9528480"/>
+          <a:ext cx="8034120" cy="9527760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2135,9 +2138,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>378720</xdr:colOff>
+      <xdr:colOff>378000</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>138960</xdr:rowOff>
+      <xdr:rowOff>138240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2147,7 +2150,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="8082720" cy="9528480"/>
+          <a:ext cx="8034120" cy="9527760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2182,14 +2185,14 @@
   <dimension ref="A1:B58"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J25" activeCellId="0" sqref="J25"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="3:3 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="107.724489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.59183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="113.663265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2404,15 +2407,15 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="3:3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2429,17 +2432,17 @@
         <v>174</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="32" t="s">
         <v>93</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="29" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -2447,7 +2450,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -2481,19 +2484,19 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="1" sqref="3:3 B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="34" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="34" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="35" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B1" s="31" t="s">
         <v>67</v>
@@ -2501,7 +2504,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="36" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B2" s="31" t="s">
         <v>130</v>
@@ -2517,34 +2520,34 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="29" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="29" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="29" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2572,13 +2575,14 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2591,34 +2595,34 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -2640,18 +2644,19 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="38" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B1" s="38" t="s">
         <v>159</v>
@@ -2659,26 +2664,26 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2700,78 +2705,77 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="3:3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="38" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C1" s="38" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D1" s="38" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E1" s="38" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F1" s="38" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G1" s="38" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H1" s="38" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="I1" s="38" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="J1" s="38" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="K1" s="38" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="L1" s="38" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>215</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>216</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>214</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>130</v>
@@ -2786,10 +2790,10 @@
         <v>133</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="L2" s="0" t="n">
         <v>1</v>
@@ -2814,13 +2818,13 @@
   <dimension ref="A1:B102"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+      <selection pane="topLeft" activeCell="H12" activeCellId="1" sqref="3:3 H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2828,7 +2832,7 @@
         <v>93</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2841,7 +2845,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -2849,7 +2853,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0</v>
@@ -2857,7 +2861,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -2865,7 +2869,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0</v>
@@ -2873,7 +2877,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0</v>
@@ -2881,7 +2885,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
@@ -2889,7 +2893,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0</v>
@@ -2897,7 +2901,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0</v>
@@ -2905,7 +2909,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0</v>
@@ -2913,7 +2917,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0</v>
@@ -2921,7 +2925,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0</v>
@@ -2929,7 +2933,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0</v>
@@ -2937,7 +2941,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0</v>
@@ -2945,7 +2949,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0</v>
@@ -2953,7 +2957,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0</v>
@@ -2961,7 +2965,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0</v>
@@ -2969,7 +2973,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0</v>
@@ -2977,7 +2981,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0</v>
@@ -2985,7 +2989,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0</v>
@@ -2993,7 +2997,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0</v>
@@ -3001,7 +3005,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>0</v>
@@ -3009,7 +3013,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>0</v>
@@ -3017,7 +3021,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>0</v>
@@ -3025,7 +3029,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>0</v>
@@ -3033,7 +3037,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>0</v>
@@ -3041,7 +3045,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>0</v>
@@ -3049,7 +3053,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0</v>
@@ -3057,7 +3061,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>0</v>
@@ -3065,7 +3069,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>0</v>
@@ -3073,7 +3077,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>0</v>
@@ -3081,7 +3085,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>0</v>
@@ -3089,7 +3093,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>0</v>
@@ -3097,7 +3101,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>0</v>
@@ -3105,7 +3109,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>0</v>
@@ -3113,7 +3117,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>0</v>
@@ -3121,7 +3125,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>0</v>
@@ -3129,7 +3133,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>0</v>
@@ -3137,7 +3141,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>0</v>
@@ -3145,7 +3149,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>0</v>
@@ -3153,7 +3157,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>0</v>
@@ -3161,7 +3165,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>0</v>
@@ -3169,7 +3173,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>0</v>
@@ -3177,7 +3181,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>0</v>
@@ -3185,7 +3189,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>0</v>
@@ -3193,7 +3197,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>0</v>
@@ -3201,7 +3205,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>0</v>
@@ -3209,7 +3213,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>0</v>
@@ -3217,7 +3221,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>0</v>
@@ -3225,7 +3229,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>0</v>
@@ -3233,7 +3237,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>0</v>
@@ -3241,7 +3245,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>0</v>
@@ -3249,7 +3253,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>0</v>
@@ -3257,7 +3261,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>0</v>
@@ -3265,7 +3269,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>0</v>
@@ -3273,7 +3277,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>0</v>
@@ -3281,7 +3285,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>0</v>
@@ -3289,7 +3293,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>0</v>
@@ -3297,7 +3301,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>0</v>
@@ -3305,7 +3309,7 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>0</v>
@@ -3313,7 +3317,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>0</v>
@@ -3321,7 +3325,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>0</v>
@@ -3329,7 +3333,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>0</v>
@@ -3337,7 +3341,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>0</v>
@@ -3345,7 +3349,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>0</v>
@@ -3353,7 +3357,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>0</v>
@@ -3361,7 +3365,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>0</v>
@@ -3369,7 +3373,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>0</v>
@@ -3377,7 +3381,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>0</v>
@@ -3385,7 +3389,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>0</v>
@@ -3393,7 +3397,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>0</v>
@@ -3401,7 +3405,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>0</v>
@@ -3409,7 +3413,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>0</v>
@@ -3417,7 +3421,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>0</v>
@@ -3425,7 +3429,7 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>0</v>
@@ -3433,7 +3437,7 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>0</v>
@@ -3441,7 +3445,7 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>0</v>
@@ -3449,7 +3453,7 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>0</v>
@@ -3457,7 +3461,7 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>0</v>
@@ -3465,7 +3469,7 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B81" s="0" t="n">
         <v>0</v>
@@ -3473,7 +3477,7 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>0</v>
@@ -3481,7 +3485,7 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>0</v>
@@ -3489,7 +3493,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>0</v>
@@ -3497,7 +3501,7 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B85" s="0" t="n">
         <v>0</v>
@@ -3505,7 +3509,7 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B86" s="0" t="n">
         <v>0</v>
@@ -3513,7 +3517,7 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B87" s="0" t="n">
         <v>0</v>
@@ -3521,7 +3525,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B88" s="0" t="n">
         <v>0</v>
@@ -3529,7 +3533,7 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B89" s="0" t="n">
         <v>0</v>
@@ -3537,7 +3541,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B90" s="0" t="n">
         <v>0</v>
@@ -3545,7 +3549,7 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B91" s="0" t="n">
         <v>0</v>
@@ -3553,7 +3557,7 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B92" s="0" t="n">
         <v>0</v>
@@ -3561,7 +3565,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B93" s="0" t="n">
         <v>0</v>
@@ -3569,7 +3573,7 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B94" s="0" t="n">
         <v>0</v>
@@ -3577,7 +3581,7 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B95" s="0" t="n">
         <v>0</v>
@@ -3585,7 +3589,7 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B96" s="0" t="n">
         <v>0</v>
@@ -3593,7 +3597,7 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B97" s="0" t="n">
         <v>0</v>
@@ -3601,7 +3605,7 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B98" s="0" t="n">
         <v>0</v>
@@ -3609,7 +3613,7 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B99" s="0" t="n">
         <v>0</v>
@@ -3617,7 +3621,7 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B100" s="0" t="n">
         <v>0</v>
@@ -3625,7 +3629,7 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B101" s="0" t="n">
         <v>0</v>
@@ -3633,7 +3637,7 @@
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B102" s="0" t="n">
         <v>0</v>
@@ -3658,12 +3662,12 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="3:3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3671,10 +3675,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3682,18 +3686,18 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -3715,22 +3719,21 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="32" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3743,7 +3746,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>122</v>
@@ -3751,7 +3754,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>126</v>
@@ -3759,7 +3762,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>129</v>
@@ -3767,74 +3770,74 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -3856,22 +3859,21 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="32" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3884,98 +3886,98 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -3997,19 +3999,18 @@
   <dimension ref="A1:B89"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="32" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B1" s="32"/>
     </row>
@@ -4018,703 +4019,703 @@
         <v>96</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
   </sheetData>
@@ -4735,15 +4736,13 @@
   </sheetPr>
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B30" activeCellId="1" sqref="3:3 B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="178.127551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="174.137755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4936,42 +4935,42 @@
   <dimension ref="A1:AW9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+      <selection pane="topLeft" activeCell="B25" activeCellId="1" sqref="3:3 B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="45" min="27" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="7" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="8" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="49" min="48" style="7" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="50" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="45" min="27" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="7" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="8" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="49" min="48" style="7" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="50" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5410,48 +5409,48 @@
   <dimension ref="A1:AX8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="3:3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5731,47 +5730,47 @@
   <dimension ref="A1:BE7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="1" sqref="3:3 C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="6" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="6" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6041,14 +6040,15 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="1" sqref="3:3 C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6126,14 +6126,15 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6190,17 +6191,17 @@
   <dimension ref="A1:E65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="1" sqref="3:3 E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="23" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="1017" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="23" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1016" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="49.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6309,14 +6310,15 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
+      <selection pane="topLeft" activeCell="H18" activeCellId="1" sqref="3:3 H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Fix group types to correctly set `is_variant`
</commit_message>
<xml_diff>
--- a/src/Resources/fixtures/minimal/init.xlsx
+++ b/src/Resources/fixtures/minimal/init.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -60,7 +60,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Insert the name of the locales, separated by ",".
+          <t xml:space="preserve">Insert the name of the locales, separated by ",".
 For example : "en_US, fr_FR"
 </t>
         </r>
@@ -76,7 +76,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Insert the allowed extensions, separated by a comma.
+          <t xml:space="preserve">Insert the allowed extensions, separated by a comma.
 For example : 
 jpg, jpeg, png</t>
         </r>
@@ -92,7 +92,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Determines how many characters should be typed for select attributes before an option is presented.
+          <t xml:space="preserve">Determines how many characters should be typed for select attributes before an option is presented.
 This should be used for attributes which have a large number of options.</t>
         </r>
       </text>
@@ -117,7 +117,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Insert the name of the locales, separated by ",".
+          <t xml:space="preserve">Insert the name of the locales, separated by ",".
 For example : "en_US, fr_FR"
 </t>
         </r>
@@ -133,7 +133,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Insert the allowed extensions, separated by a comma.
+          <t xml:space="preserve">Insert the allowed extensions, separated by a comma.
 For example : 
 jpg, jpeg, png</t>
         </r>
@@ -149,7 +149,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Determines how many characters should be typed for select attributes before an option is presented.
+          <t xml:space="preserve">Determines how many characters should be typed for select attributes before an option is presented.
 This should be used for attributes which have a large number of options.</t>
         </r>
       </text>
@@ -164,7 +164,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Set to 1 if the attribute is required in this family for the concerned channel.</t>
+          <t xml:space="preserve">Set to 1 if the attribute is required in this family for the concerned channel.</t>
         </r>
       </text>
     </comment>
@@ -188,7 +188,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Insert the allowed extensions, separated by a comma.
+          <t xml:space="preserve">Insert the allowed extensions, separated by a comma.
 For example : 
 jpg, jpeg, png</t>
         </r>
@@ -204,7 +204,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Determines how many characters should be typed for select attributes before an option is presented.
+          <t xml:space="preserve">Determines how many characters should be typed for select attributes before an option is presented.
 This should be used for attributes which have a large number of options.</t>
         </r>
       </text>
@@ -219,7 +219,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Set to 1 if the attribute is required in this family for the concerned channel.</t>
+          <t xml:space="preserve">Set to 1 if the attribute is required in this family for the concerned channel.</t>
         </r>
       </text>
     </comment>
@@ -243,7 +243,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Multiple locales should be separated by a comma.
+          <t xml:space="preserve">Multiple locales should be separated by a comma.
 For example : "fr_FR, en_US"</t>
         </r>
       </text>
@@ -258,7 +258,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Multiple currency codes should be separated by a comma.
+          <t xml:space="preserve">Multiple currency codes should be separated by a comma.
 For example: "EUR,USD"</t>
         </r>
       </text>
@@ -268,816 +268,819 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="270">
-  <si>
-    <t>End user HOWTO</t>
-  </si>
-  <si>
-    <t>Global rules</t>
-  </si>
-  <si>
-    <t>Do not modify the headers of the files</t>
-  </si>
-  <si>
-    <t>Do not open this file in Open Office, as it will break the validation</t>
-  </si>
-  <si>
-    <t>Do not save this file with another extension than xlsx</t>
-  </si>
-  <si>
-    <t>Do not modify hidden rows</t>
-  </si>
-  <si>
-    <t>Attributes tab</t>
-  </si>
-  <si>
-    <t>The attributes tab can be used to define the properties of attributes which are not linked to families, or which are shared by families.</t>
-  </si>
-  <si>
-    <t>This tab can be duplicated to shorten the list. All attributes tab titles should start with "attributes"</t>
-  </si>
-  <si>
-    <t>Family tabs</t>
-  </si>
-  <si>
-    <t>The family tab contains all information for a family : code, labels, attributes and completion rules</t>
-  </si>
-  <si>
-    <t>To create a new family, simply duplicate the tab. All family tabs titles must start with "family"</t>
-  </si>
-  <si>
-    <t>If an attribute is present in multiple families, only fill the blue and pink columns (attribute properties and translations) once </t>
-  </si>
-  <si>
-    <t>To add completion for other channels, simply add columns on the right of the table. The label should be the code of the channel.</t>
-  </si>
-  <si>
-    <t>Attribute groups</t>
-  </si>
-  <si>
-    <t>This tab contains all informations for attribute groups</t>
-  </si>
-  <si>
-    <t>You should not delete the mandatory “other” group</t>
-  </si>
-  <si>
-    <t>Options</t>
-  </si>
-  <si>
-    <t>This tab contains the list of options for select attributes.</t>
-  </si>
-  <si>
-    <t>This tab can be duplicated to divide the contents by attribute. All options tab titles should start with "options"</t>
-  </si>
-  <si>
-    <t>Channels</t>
-  </si>
-  <si>
-    <t>This tab contains all information about channels.</t>
-  </si>
-  <si>
-    <t>After editing this tab, you might have to update your family tabs so they use the right family codes</t>
-  </si>
-  <si>
-    <t>Categories</t>
-  </si>
-  <si>
-    <t>This tab contains all information about categories</t>
-  </si>
-  <si>
-    <t>This tab can be duplicated to divide its content between trees. All category tabs should start with "categories"</t>
-  </si>
-  <si>
-    <t>Association types</t>
-  </si>
-  <si>
-    <t>This tab contains all information about association types</t>
-  </si>
-  <si>
-    <t>Group types</t>
-  </si>
-  <si>
-    <t>This tab contains all information about group types</t>
-  </si>
-  <si>
-    <t>Integrator HOWTO</t>
-  </si>
-  <si>
-    <t>All tabs contain a hidden row with the codes of the properties. If you add some columns, do not forget to update them.</t>
-  </si>
-  <si>
-    <t>The codes for label translations are always of the form "label-&lt;locale&gt;". For example, the french label has the code "label-fr_FR"</t>
-  </si>
-  <si>
-    <t>Common and unaffected attribute properties</t>
-  </si>
-  <si>
-    <t>Labels</t>
-  </si>
-  <si>
-    <t>Attribute properties</t>
-  </si>
-  <si>
-    <t>Attribute code</t>
-  </si>
-  <si>
-    <t>en_US</t>
-  </si>
-  <si>
-    <t>Attribute type</t>
-  </si>
-  <si>
-    <t>Attribute group</t>
-  </si>
-  <si>
-    <t>Sort order</t>
-  </si>
-  <si>
-    <t>Is unique*</t>
-  </si>
-  <si>
-    <t>Is localizable*</t>
-  </si>
-  <si>
-    <t>Specific to locales</t>
-  </si>
-  <si>
-    <t>Is scopable*</t>
-  </si>
-  <si>
-    <t>Useable as grid filter*</t>
-  </si>
-  <si>
-    <t>Max characters</t>
-  </si>
-  <si>
-    <t>Validation rule</t>
-  </si>
-  <si>
-    <t>Validation regexp</t>
-  </si>
-  <si>
-    <t>Rich text</t>
-  </si>
-  <si>
-    <t>Minimum number</t>
-  </si>
-  <si>
-    <t>Maximum number</t>
-  </si>
-  <si>
-    <t>Decimals allowed</t>
-  </si>
-  <si>
-    <t>Negative allowed</t>
-  </si>
-  <si>
-    <t>Minimum date</t>
-  </si>
-  <si>
-    <t>Maximum date</t>
-  </si>
-  <si>
-    <t>Metric family</t>
-  </si>
-  <si>
-    <t>Default metric  unit</t>
-  </si>
-  <si>
-    <t>Max file size</t>
-  </si>
-  <si>
-    <t>Allowed extensions</t>
-  </si>
-  <si>
-    <t>Minimum input length</t>
-  </si>
-  <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>label-en_US</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>group</t>
-  </si>
-  <si>
-    <t>sort_order</t>
-  </si>
-  <si>
-    <t>unique</t>
-  </si>
-  <si>
-    <t>localizable</t>
-  </si>
-  <si>
-    <t>available_locales</t>
-  </si>
-  <si>
-    <t>scopable</t>
-  </si>
-  <si>
-    <t>useable_as_grid_filter</t>
-  </si>
-  <si>
-    <t>max_characters</t>
-  </si>
-  <si>
-    <t>validation_rule</t>
-  </si>
-  <si>
-    <t>validation_regexp</t>
-  </si>
-  <si>
-    <t>wysiwyg_enabled</t>
-  </si>
-  <si>
-    <t>number_min</t>
-  </si>
-  <si>
-    <t>number_max</t>
-  </si>
-  <si>
-    <t>decimals_allowed</t>
-  </si>
-  <si>
-    <t>negative_allowed</t>
-  </si>
-  <si>
-    <t>date_min</t>
-  </si>
-  <si>
-    <t>date_max</t>
-  </si>
-  <si>
-    <t>metric_family</t>
-  </si>
-  <si>
-    <t>default_metric_unit</t>
-  </si>
-  <si>
-    <t>max_file_size</t>
-  </si>
-  <si>
-    <t>allowed_extensions</t>
-  </si>
-  <si>
-    <t>minimum_input length</t>
-  </si>
-  <si>
-    <t>sku</t>
-  </si>
-  <si>
-    <t>Code article</t>
-  </si>
-  <si>
-    <t>Identifier</t>
-  </si>
-  <si>
-    <t>global</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>Family code</t>
-  </si>
-  <si>
-    <t>main</t>
-  </si>
-  <si>
-    <t>Label</t>
-  </si>
-  <si>
-    <t>Main</t>
-  </si>
-  <si>
-    <t>Completeness</t>
-  </si>
-  <si>
-    <t>Use as label</t>
-  </si>
-  <si>
-    <t>use_as_label</t>
-  </si>
-  <si>
-    <t>second_family</t>
-  </si>
-  <si>
-    <t>Second family</t>
-  </si>
-  <si>
-    <t>Group properties</t>
-  </si>
-  <si>
-    <t>Group code</t>
-  </si>
-  <si>
-    <t>Position</t>
-  </si>
-  <si>
-    <t>Global</t>
-  </si>
-  <si>
-    <t>other</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Option properties</t>
-  </si>
-  <si>
-    <t>Option code</t>
-  </si>
-  <si>
-    <t>attribute</t>
-  </si>
-  <si>
-    <t>Channel properties</t>
-  </si>
-  <si>
-    <t>Channel code</t>
-  </si>
-  <si>
-    <t>Channel label</t>
-  </si>
-  <si>
-    <t>Channel locales</t>
-  </si>
-  <si>
-    <t>Channel currencies</t>
-  </si>
-  <si>
-    <t>Category tree</t>
-  </si>
-  <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>locales</t>
-  </si>
-  <si>
-    <t>currencies</t>
-  </si>
-  <si>
-    <t>tree</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>Category properties</t>
-  </si>
-  <si>
-    <t>Category code</t>
-  </si>
-  <si>
-    <t>Parent category code</t>
-  </si>
-  <si>
-    <t>parent</t>
-  </si>
-  <si>
-    <t>Main category</t>
-  </si>
-  <si>
-    <t>Group type properties</t>
-  </si>
-  <si>
-    <t>variant</t>
-  </si>
-  <si>
-    <t>VARIANT</t>
-  </si>
-  <si>
-    <t>RELATED</t>
-  </si>
-  <si>
-    <t>Association type properties</t>
-  </si>
-  <si>
-    <t>Association type code</t>
-  </si>
-  <si>
-    <t>X_SELL</t>
-  </si>
-  <si>
-    <t>Cross sell</t>
-  </si>
-  <si>
-    <t>UPSELL</t>
-  </si>
-  <si>
-    <t>Upsell</t>
-  </si>
-  <si>
-    <t>SUBSTITUTION</t>
-  </si>
-  <si>
-    <t>Substitution</t>
-  </si>
-  <si>
-    <t>PACK</t>
-  </si>
-  <si>
-    <t>Pack</t>
-  </si>
-  <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>regexp</t>
-  </si>
-  <si>
-    <t>datetime</t>
-  </si>
-  <si>
-    <t>Attribute type code</t>
-  </si>
-  <si>
-    <t>Attribute type label</t>
-  </si>
-  <si>
-    <t>pim_catalog_identifier</t>
-  </si>
-  <si>
-    <t>pim_catalog_text</t>
-  </si>
-  <si>
-    <t>pim_catalog_textarea</t>
-  </si>
-  <si>
-    <t>Text area</t>
-  </si>
-  <si>
-    <t>pim_catalog_multiselect</t>
-  </si>
-  <si>
-    <t>Multiple select</t>
-  </si>
-  <si>
-    <t>pim_catalog_simpleselect</t>
-  </si>
-  <si>
-    <t>Simple select</t>
-  </si>
-  <si>
-    <t>pim_catalog_price_collection</t>
-  </si>
-  <si>
-    <t>Price collection</t>
-  </si>
-  <si>
-    <t>pim_catalog_number</t>
-  </si>
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>pim_catalog_boolean</t>
-  </si>
-  <si>
-    <t>Boolean</t>
-  </si>
-  <si>
-    <t>pim_catalog_date</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>pim_catalog_file</t>
-  </si>
-  <si>
-    <t>File</t>
-  </si>
-  <si>
-    <t>pim_catalog_image</t>
-  </si>
-  <si>
-    <t>Image</t>
-  </si>
-  <si>
-    <t>pim_catalog_metric</t>
-  </si>
-  <si>
-    <t>Metric</t>
-  </si>
-  <si>
-    <t>Area</t>
-  </si>
-  <si>
-    <t>Binary</t>
-  </si>
-  <si>
-    <t>Frequency</t>
-  </si>
-  <si>
-    <t>Length</t>
-  </si>
-  <si>
-    <t>Power</t>
-  </si>
-  <si>
-    <t>Speed</t>
-  </si>
-  <si>
-    <t>Temperature</t>
-  </si>
-  <si>
-    <t>Volume</t>
-  </si>
-  <si>
-    <t>Weight</t>
-  </si>
-  <si>
-    <t>Voltage</t>
-  </si>
-  <si>
-    <t>Intensity</t>
-  </si>
-  <si>
-    <t>Resistance</t>
-  </si>
-  <si>
-    <t>unit</t>
-  </si>
-  <si>
-    <t>ACRE</t>
-  </si>
-  <si>
-    <t>ARE</t>
-  </si>
-  <si>
-    <t>ARPENT</t>
-  </si>
-  <si>
-    <t>CENTIARE</t>
-  </si>
-  <si>
-    <t>HECTARE</t>
-  </si>
-  <si>
-    <t>SQUARE_CENTIMETER</t>
-  </si>
-  <si>
-    <t>SQUARE_DECIMETER</t>
-  </si>
-  <si>
-    <t>SQUARE_DEKAMETER</t>
-  </si>
-  <si>
-    <t>SQUARE_FOOT</t>
-  </si>
-  <si>
-    <t>SQUARE_FURLONG</t>
-  </si>
-  <si>
-    <t>SQUARE_HECTOMETER</t>
-  </si>
-  <si>
-    <t>SQUARE_INCH</t>
-  </si>
-  <si>
-    <t>SQUARE_KILOMETER</t>
-  </si>
-  <si>
-    <t>SQUARE_METER</t>
-  </si>
-  <si>
-    <t>SQUARE_MIL</t>
-  </si>
-  <si>
-    <t>SQUARE_MILE</t>
-  </si>
-  <si>
-    <t>SQUARE_MILLIMETER</t>
-  </si>
-  <si>
-    <t>SQUARE_YARD</t>
-  </si>
-  <si>
-    <t>BIT</t>
-  </si>
-  <si>
-    <t>BYTE</t>
-  </si>
-  <si>
-    <t>KILOBYTE</t>
-  </si>
-  <si>
-    <t>MEGABYTE</t>
-  </si>
-  <si>
-    <t>GIGABYTE</t>
-  </si>
-  <si>
-    <t>TERABYTE</t>
-  </si>
-  <si>
-    <t>GIGAHERTZ</t>
-  </si>
-  <si>
-    <t>KILOHERTZ</t>
-  </si>
-  <si>
-    <t>MEGAHERTZ</t>
-  </si>
-  <si>
-    <t>TERAHERTZ</t>
-  </si>
-  <si>
-    <t>HERTZ</t>
-  </si>
-  <si>
-    <t>CENTIMETER</t>
-  </si>
-  <si>
-    <t>CHAIN</t>
-  </si>
-  <si>
-    <t>DECIMETER</t>
-  </si>
-  <si>
-    <t>DEKAMETER</t>
-  </si>
-  <si>
-    <t>FEET</t>
-  </si>
-  <si>
-    <t>FURLONG</t>
-  </si>
-  <si>
-    <t>INCH</t>
-  </si>
-  <si>
-    <t>HECTOMETER</t>
-  </si>
-  <si>
-    <t>KILOMETER</t>
-  </si>
-  <si>
-    <t>METER</t>
-  </si>
-  <si>
-    <t>MIL</t>
-  </si>
-  <si>
-    <t>MILE</t>
-  </si>
-  <si>
-    <t>MILLIMETER</t>
-  </si>
-  <si>
-    <t>YARD</t>
-  </si>
-  <si>
-    <t>GIGAWATT</t>
-  </si>
-  <si>
-    <t>KILOWATT</t>
-  </si>
-  <si>
-    <t>MEGAWATT</t>
-  </si>
-  <si>
-    <t>TERAWATT</t>
-  </si>
-  <si>
-    <t>WATT</t>
-  </si>
-  <si>
-    <t>FOOT_PER_SECOND</t>
-  </si>
-  <si>
-    <t>FOOT_PER_HOUR</t>
-  </si>
-  <si>
-    <t>KILOMETER_PER_HOUR</t>
-  </si>
-  <si>
-    <t>METER_PER_HOUR</t>
-  </si>
-  <si>
-    <t>METER_PER_MINUTE</t>
-  </si>
-  <si>
-    <t>METER_PER_SECOND</t>
-  </si>
-  <si>
-    <t>MILE_PER_HOUR</t>
-  </si>
-  <si>
-    <t>YARD_PER_HOUR</t>
-  </si>
-  <si>
-    <t>CELSIUS</t>
-  </si>
-  <si>
-    <t>FAHRENHEIT</t>
-  </si>
-  <si>
-    <t>KELVIN</t>
-  </si>
-  <si>
-    <t>RANKINE</t>
-  </si>
-  <si>
-    <t>REAUMUR</t>
-  </si>
-  <si>
-    <t>BARREL</t>
-  </si>
-  <si>
-    <t>CENTILITER</t>
-  </si>
-  <si>
-    <t>CUBIC_CENTIMETER</t>
-  </si>
-  <si>
-    <t>CUBIC_DECIMETER</t>
-  </si>
-  <si>
-    <t>CUBIC_FOOT</t>
-  </si>
-  <si>
-    <t>CUBIC_INCH</t>
-  </si>
-  <si>
-    <t>CUBIC_METER</t>
-  </si>
-  <si>
-    <t>CUBIC_MILLIMETER</t>
-  </si>
-  <si>
-    <t>CUBIC_YARD</t>
-  </si>
-  <si>
-    <t>DECILITER</t>
-  </si>
-  <si>
-    <t>GALLON</t>
-  </si>
-  <si>
-    <t>LITER</t>
-  </si>
-  <si>
-    <t>MILLILITER</t>
-  </si>
-  <si>
-    <t>OUNCE</t>
-  </si>
-  <si>
-    <t>PINT</t>
-  </si>
-  <si>
-    <t>DENIER</t>
-  </si>
-  <si>
-    <t>GRAIN</t>
-  </si>
-  <si>
-    <t>GRAM</t>
-  </si>
-  <si>
-    <t>KILOGRAM</t>
-  </si>
-  <si>
-    <t>LIVRE</t>
-  </si>
-  <si>
-    <t>MARC</t>
-  </si>
-  <si>
-    <t>MILLIGRAM</t>
-  </si>
-  <si>
-    <t>ONCE</t>
-  </si>
-  <si>
-    <t>POUND</t>
-  </si>
-  <si>
-    <t>TON</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="271">
+  <si>
+    <t xml:space="preserve">End user HOWTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Global rules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do not modify the headers of the files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do not open this file in Open Office, as it will break the validation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do not save this file with another extension than xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do not modify hidden rows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attributes tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The attributes tab can be used to define the properties of attributes which are not linked to families, or which are shared by families.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This tab can be duplicated to shorten the list. All attributes tab titles should start with "attributes"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family tabs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The family tab contains all information for a family : code, labels, attributes and completion rules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To create a new family, simply duplicate the tab. All family tabs titles must start with "family"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If an attribute is present in multiple families, only fill the blue and pink columns (attribute properties and translations) once </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To add completion for other channels, simply add columns on the right of the table. The label should be the code of the channel.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attribute groups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This tab contains all informations for attribute groups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You should not delete the mandatory “other” group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This tab contains the list of options for select attributes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This tab can be duplicated to divide the contents by attribute. All options tab titles should start with "options"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This tab contains all information about channels.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After editing this tab, you might have to update your family tabs so they use the right family codes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Categories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This tab contains all information about categories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This tab can be duplicated to divide its content between trees. All category tabs should start with "categories"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Association types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This tab contains all information about association types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This tab contains all information about group types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrator HOWTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All tabs contain a hidden row with the codes of the properties. If you add some columns, do not forget to update them.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The codes for label translations are always of the form "label-&lt;locale&gt;". For example, the french label has the code "label-fr_FR"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Common and unaffected attribute properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Labels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attribute properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attribute code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">en_US</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attribute type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attribute group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sort order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is unique*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is localizable*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specific to locales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is scopable*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Useable as grid filter*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validation rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validation regexp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rich text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decimals allowed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Negative allowed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metric family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default metric  unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max file size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allowed extensions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum input length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label-en_US</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sort_order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">localizable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">available_locales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scopable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">useable_as_grid_filter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validation_rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validation_regexp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wysiwyg_enabled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number_min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number_max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">decimals_allowed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">negative_allowed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metric_family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default_metric_unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_file_size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allowed_extensions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimum_input length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code article</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">global</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">main</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Completeness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use as label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use_as_label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">second_family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Second family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Global</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Option properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Option code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">attribute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel locales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel currencies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">currencies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parent category code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group type properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">variant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is_variant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VARIANT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RELATED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Association type properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Association type code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X_SELL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cross sell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPSELL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upsell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUBSTITUTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Substitution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regexp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">datetime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attribute type code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attribute type label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pim_catalog_identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pim_catalog_text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pim_catalog_textarea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pim_catalog_multiselect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiple select</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pim_catalog_simpleselect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simple select</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pim_catalog_price_collection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price collection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pim_catalog_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pim_catalog_boolean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boolean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pim_catalog_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pim_catalog_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pim_catalog_image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pim_catalog_metric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Binary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intensity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARPENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CENTIARE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HECTARE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQUARE_CENTIMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQUARE_DECIMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQUARE_DEKAMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQUARE_FOOT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQUARE_FURLONG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQUARE_HECTOMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQUARE_INCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQUARE_KILOMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQUARE_METER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQUARE_MIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQUARE_MILE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQUARE_MILLIMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQUARE_YARD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BYTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KILOBYTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEGABYTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIGABYTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TERABYTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIGAHERTZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KILOHERTZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEGAHERTZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TERAHERTZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HERTZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CENTIMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHAIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DECIMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEKAMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FEET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FURLONG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HECTOMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KILOMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">METER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MILE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MILLIMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YARD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIGAWATT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KILOWATT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEGAWATT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TERAWATT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WATT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FOOT_PER_SECOND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FOOT_PER_HOUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KILOMETER_PER_HOUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">METER_PER_HOUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">METER_PER_MINUTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">METER_PER_SECOND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MILE_PER_HOUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YARD_PER_HOUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CELSIUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAHRENHEIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KELVIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RANKINE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REAUMUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BARREL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CENTILITER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUBIC_CENTIMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUBIC_DECIMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUBIC_FOOT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUBIC_INCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUBIC_METER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUBIC_MILLIMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUBIC_YARD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DECILITER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GALLON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LITER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MILLILITER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUNCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PINT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DENIER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRAIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KILOGRAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIVRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MILLIGRAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ONCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POUND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TON</t>
   </si>
 </sst>
 </file>
@@ -1085,7 +1088,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -1421,9 +1424,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>380880</xdr:colOff>
+      <xdr:colOff>380520</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>141120</xdr:rowOff>
+      <xdr:rowOff>140760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1433,7 +1436,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="6160680" cy="9530640"/>
+          <a:ext cx="6074640" cy="9530280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1466,9 +1469,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>380880</xdr:colOff>
+      <xdr:colOff>380520</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>141120</xdr:rowOff>
+      <xdr:rowOff>140760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1478,7 +1481,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="6160680" cy="9530640"/>
+          <a:ext cx="6074640" cy="9530280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1516,9 +1519,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>133200</xdr:colOff>
+      <xdr:colOff>132840</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>141480</xdr:rowOff>
+      <xdr:rowOff>141120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1528,7 +1531,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="5865480" cy="10200960"/>
+          <a:ext cx="5798520" cy="10200600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1561,9 +1564,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>133200</xdr:colOff>
+      <xdr:colOff>132840</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>141480</xdr:rowOff>
+      <xdr:rowOff>141120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1573,7 +1576,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="5865480" cy="10200960"/>
+          <a:ext cx="5798520" cy="10200600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1611,9 +1614,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>380880</xdr:colOff>
+      <xdr:colOff>380520</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>141120</xdr:rowOff>
+      <xdr:rowOff>140760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1623,7 +1626,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="6760800" cy="9530640"/>
+          <a:ext cx="6665040" cy="9530280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1656,9 +1659,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>380880</xdr:colOff>
+      <xdr:colOff>380520</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>141120</xdr:rowOff>
+      <xdr:rowOff>140760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1668,7 +1671,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="6760800" cy="9530640"/>
+          <a:ext cx="6665040" cy="9530280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1702,13 +1705,14 @@
   </sheetPr>
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B25" activeCellId="1" sqref="3:3 B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1901,18 +1905,19 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="47.1122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="46.5714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="28" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B1" s="25" t="s">
         <v>34</v>
@@ -1920,7 +1925,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>37</v>
@@ -1936,34 +1941,34 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1991,20 +1996,23 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+      <selection pane="topLeft" activeCell="D26" activeCellId="1" sqref="3:3 D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2012,18 +2020,18 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -2045,22 +2053,21 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="1" sqref="3:3 B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2073,7 +2080,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>88</v>
@@ -2081,7 +2088,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>92</v>
@@ -2089,82 +2096,82 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2186,22 +2193,21 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="1" sqref="3:3 B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2214,98 +2220,98 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -2327,19 +2333,18 @@
   <dimension ref="A1:B89"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="3:3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B1" s="16"/>
     </row>
@@ -2348,703 +2353,703 @@
         <v>63</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -3066,38 +3071,41 @@
   <dimension ref="A1:AV8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="1" sqref="3:3 C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="7" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="8" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="48" min="47" style="7" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="44" min="26" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="7" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="8" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="48" min="47" style="7" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="49" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3480,47 +3488,47 @@
   <dimension ref="A1:AX7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="3:3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="13.5"/>
-    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3900,47 +3908,47 @@
   <dimension ref="A1:AX6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="1" sqref="3:3 B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="13.5"/>
-    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4307,15 +4315,15 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="3:3 A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4393,14 +4401,14 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4457,18 +4465,17 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+      <selection pane="topLeft" activeCell="F22" activeCellId="1" sqref="3:3 F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="1016" min="6" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="1017" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1016" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4561,14 +4568,14 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4638,14 +4645,15 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="3:3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4662,17 +4670,17 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
         <v>61</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -4680,7 +4688,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Fix CE init fixtures labels
</commit_message>
<xml_diff>
--- a/src/Resources/fixtures/minimal/init.xlsx
+++ b/src/Resources/fixtures/minimal/init.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="README-EN" sheetId="1" state="visible" r:id="rId2"/>
@@ -112,7 +112,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -127,7 +127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="450">
   <si>
     <t xml:space="preserve">End user HOWTO</t>
   </si>
@@ -602,6 +602,9 @@
     <t xml:space="preserve">Other</t>
   </si>
   <si>
+    <t xml:space="preserve">Autres</t>
+  </si>
+  <si>
     <t xml:space="preserve">Option properties</t>
   </si>
   <si>
@@ -626,118 +629,124 @@
     <t xml:space="preserve">Category tree</t>
   </si>
   <si>
+    <t xml:space="preserve">locales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">currencies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecommerce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-commerce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">en_US,fr_FR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USD,EUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parent category code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Catégorie principale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group type properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">variant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is_variant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VARIANT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RELATED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Association type properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Association type code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X_SELL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cross sell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPSELL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upsell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUBSTITUTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Substitution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it_support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">redactor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redactor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">role</t>
+  </si>
+  <si>
     <t xml:space="preserve">label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">locales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">currencies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tree</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ecommerce</t>
-  </si>
-  <si>
-    <t xml:space="preserve">en_US,fr_FR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USD,EUR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mobile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category properties</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parent category code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Main category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group type properties</t>
-  </si>
-  <si>
-    <t xml:space="preserve">variant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">is_variant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VARIANT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RELATED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Association type properties</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Association type code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X_SELL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cross sell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPSELL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Upsell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUBSTITUTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Substitution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PACK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">it_support</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IT support</t>
-  </si>
-  <si>
-    <t xml:space="preserve">manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">redactor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Redactor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">all</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All</t>
-  </si>
-  <si>
-    <t xml:space="preserve">role</t>
   </si>
   <si>
     <t xml:space="preserve">ROLE_ADMINISTRATOR</t>
@@ -1902,10 +1911,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>377640</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>138240</xdr:rowOff>
+      <xdr:rowOff>137880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1915,7 +1924,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="6157440" cy="9527760"/>
+          <a:ext cx="7156800" cy="9563760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1947,10 +1956,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>377640</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>138240</xdr:rowOff>
+      <xdr:rowOff>137880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1960,7 +1969,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="6157440" cy="9527760"/>
+          <a:ext cx="7156800" cy="9563760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1997,10 +2006,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>130680</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>130320</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>138240</xdr:rowOff>
+      <xdr:rowOff>110160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2010,7 +2019,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="5853240" cy="8418960"/>
+          <a:ext cx="6986520" cy="8418960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2042,10 +2051,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>130680</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>130320</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>138240</xdr:rowOff>
+      <xdr:rowOff>110160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2055,7 +2064,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="5853240" cy="8418960"/>
+          <a:ext cx="6986520" cy="8418960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2092,7 +2101,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>378000</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>138240</xdr:rowOff>
@@ -2105,7 +2114,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="8034120" cy="9527760"/>
+          <a:ext cx="9545400" cy="9400680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2137,7 +2146,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>378000</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>138240</xdr:rowOff>
@@ -2150,7 +2159,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="8034120" cy="9527760"/>
+          <a:ext cx="9545400" cy="9400680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2185,14 +2194,14 @@
   <dimension ref="A1:B58"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="3:3 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.59183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="113.663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.45408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="112.448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2407,20 +2416,20 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="3:3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B1" s="30"/>
     </row>
@@ -2429,7 +2438,7 @@
         <v>146</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2437,12 +2446,12 @@
         <v>93</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="29" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -2450,7 +2459,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -2481,78 +2490,90 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="1" sqref="3:3 B16"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="34" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="34" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="34" width="27.780612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="35" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B1" s="31" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1" s="31"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="36" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B2" s="31" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="31" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="32" t="s">
         <v>93</v>
       </c>
       <c r="B3" s="33" t="s">
         <v>94</v>
       </c>
+      <c r="C3" s="33" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="29" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>183</v>
+      </c>
+      <c r="C4" s="37"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>185</v>
+      </c>
+      <c r="C5" s="35"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="29" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>187</v>
+      </c>
+      <c r="C6" s="35"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="29" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>187</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="C7" s="35"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B4" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B4:C4" type="none">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2575,14 +2596,14 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2595,34 +2616,34 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -2644,46 +2665,46 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5612244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="38" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>159</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -2705,77 +2726,77 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="3:3"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.3214285714286"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="38" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C1" s="38" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D1" s="38" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="E1" s="38" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="F1" s="38" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="G1" s="38" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="H1" s="38" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="I1" s="38" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="J1" s="38" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="K1" s="38" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L1" s="38" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>218</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>215</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>130</v>
@@ -2790,10 +2811,10 @@
         <v>133</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="L2" s="0" t="n">
         <v>1</v>
@@ -2817,14 +2838,14 @@
   </sheetPr>
   <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="1" sqref="3:3 H12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P25" activeCellId="0" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2832,12 +2853,12 @@
         <v>93</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -2845,7 +2866,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -2853,7 +2874,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0</v>
@@ -2861,7 +2882,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -2869,7 +2890,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0</v>
@@ -2877,7 +2898,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0</v>
@@ -2885,7 +2906,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
@@ -2893,7 +2914,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0</v>
@@ -2901,7 +2922,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0</v>
@@ -2909,7 +2930,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0</v>
@@ -2917,7 +2938,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0</v>
@@ -2925,7 +2946,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0</v>
@@ -2933,7 +2954,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0</v>
@@ -2941,7 +2962,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0</v>
@@ -2949,7 +2970,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0</v>
@@ -2957,7 +2978,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0</v>
@@ -2965,7 +2986,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0</v>
@@ -2973,7 +2994,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0</v>
@@ -2981,7 +3002,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0</v>
@@ -2989,7 +3010,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0</v>
@@ -2997,7 +3018,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0</v>
@@ -3005,7 +3026,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>0</v>
@@ -3013,7 +3034,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>0</v>
@@ -3021,7 +3042,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>0</v>
@@ -3029,7 +3050,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>0</v>
@@ -3037,7 +3058,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>0</v>
@@ -3045,7 +3066,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>0</v>
@@ -3053,7 +3074,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0</v>
@@ -3061,7 +3082,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>0</v>
@@ -3069,7 +3090,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>0</v>
@@ -3077,7 +3098,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>0</v>
@@ -3085,7 +3106,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>0</v>
@@ -3093,7 +3114,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>0</v>
@@ -3101,7 +3122,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>0</v>
@@ -3109,7 +3130,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>0</v>
@@ -3117,7 +3138,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>0</v>
@@ -3125,7 +3146,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>0</v>
@@ -3133,7 +3154,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>0</v>
@@ -3141,7 +3162,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>0</v>
@@ -3149,7 +3170,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>0</v>
@@ -3157,7 +3178,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>0</v>
@@ -3165,7 +3186,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>0</v>
@@ -3173,7 +3194,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>0</v>
@@ -3181,7 +3202,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>0</v>
@@ -3189,7 +3210,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>0</v>
@@ -3197,7 +3218,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>0</v>
@@ -3205,7 +3226,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>0</v>
@@ -3213,7 +3234,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>0</v>
@@ -3221,7 +3242,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>0</v>
@@ -3229,7 +3250,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>0</v>
@@ -3237,7 +3258,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>0</v>
@@ -3245,7 +3266,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>0</v>
@@ -3253,7 +3274,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>0</v>
@@ -3261,7 +3282,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>0</v>
@@ -3269,7 +3290,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>0</v>
@@ -3277,7 +3298,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>0</v>
@@ -3285,7 +3306,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>0</v>
@@ -3293,7 +3314,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>0</v>
@@ -3301,7 +3322,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>0</v>
@@ -3309,7 +3330,7 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>0</v>
@@ -3317,7 +3338,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>0</v>
@@ -3325,7 +3346,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>0</v>
@@ -3333,7 +3354,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>0</v>
@@ -3341,7 +3362,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>0</v>
@@ -3349,7 +3370,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>0</v>
@@ -3357,7 +3378,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>0</v>
@@ -3365,7 +3386,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>0</v>
@@ -3373,7 +3394,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>0</v>
@@ -3381,7 +3402,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>0</v>
@@ -3389,7 +3410,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>0</v>
@@ -3397,7 +3418,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>0</v>
@@ -3405,7 +3426,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>0</v>
@@ -3413,7 +3434,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>0</v>
@@ -3421,7 +3442,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>0</v>
@@ -3429,7 +3450,7 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>0</v>
@@ -3437,7 +3458,7 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>0</v>
@@ -3445,7 +3466,7 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>0</v>
@@ -3453,7 +3474,7 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>0</v>
@@ -3461,7 +3482,7 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>0</v>
@@ -3469,7 +3490,7 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="B81" s="0" t="n">
         <v>0</v>
@@ -3477,7 +3498,7 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>0</v>
@@ -3485,7 +3506,7 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>0</v>
@@ -3493,7 +3514,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>0</v>
@@ -3501,7 +3522,7 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="B85" s="0" t="n">
         <v>0</v>
@@ -3509,7 +3530,7 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="B86" s="0" t="n">
         <v>0</v>
@@ -3517,7 +3538,7 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="B87" s="0" t="n">
         <v>0</v>
@@ -3525,7 +3546,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="B88" s="0" t="n">
         <v>0</v>
@@ -3533,7 +3554,7 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="B89" s="0" t="n">
         <v>0</v>
@@ -3541,7 +3562,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B90" s="0" t="n">
         <v>0</v>
@@ -3549,7 +3570,7 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="B91" s="0" t="n">
         <v>0</v>
@@ -3557,7 +3578,7 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="B92" s="0" t="n">
         <v>0</v>
@@ -3565,7 +3586,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="B93" s="0" t="n">
         <v>0</v>
@@ -3573,7 +3594,7 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="B94" s="0" t="n">
         <v>0</v>
@@ -3581,7 +3602,7 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="B95" s="0" t="n">
         <v>0</v>
@@ -3589,7 +3610,7 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="B96" s="0" t="n">
         <v>0</v>
@@ -3597,7 +3618,7 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="B97" s="0" t="n">
         <v>0</v>
@@ -3605,7 +3626,7 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="B98" s="0" t="n">
         <v>0</v>
@@ -3613,7 +3634,7 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="B99" s="0" t="n">
         <v>0</v>
@@ -3621,7 +3642,7 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="B100" s="0" t="n">
         <v>0</v>
@@ -3629,7 +3650,7 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="B101" s="0" t="n">
         <v>0</v>
@@ -3637,7 +3658,7 @@
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="B102" s="0" t="n">
         <v>0</v>
@@ -3662,12 +3683,12 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="3:3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3675,10 +3696,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3686,18 +3707,18 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -3719,21 +3740,22 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="32" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3741,12 +3763,12 @@
         <v>93</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>159</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>122</v>
@@ -3754,7 +3776,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>126</v>
@@ -3762,7 +3784,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>129</v>
@@ -3770,74 +3792,74 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -3859,21 +3881,22 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="32" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3881,103 +3904,103 @@
         <v>93</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>159</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -3999,18 +4022,19 @@
   <dimension ref="A1:B89"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="32" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="B1" s="32"/>
     </row>
@@ -4019,703 +4043,703 @@
         <v>96</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -4737,12 +4761,14 @@
   <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="1" sqref="3:3 B30"/>
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="174.137755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="172.25"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4935,42 +4961,42 @@
   <dimension ref="A1:AW9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="1" sqref="3:3 B25"/>
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="45" min="27" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="7" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="8" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="49" min="48" style="7" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="50" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="45" min="27" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="7" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="8" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="49" min="48" style="7" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="50" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5409,48 +5435,48 @@
   <dimension ref="A1:AX8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="3:3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5730,47 +5756,47 @@
   <dimension ref="A1:BE7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="1" sqref="3:3 C12"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="6" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="6" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6037,18 +6063,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="1" sqref="3:3 C16"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="14.5867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6059,6 +6086,7 @@
       <c r="C1" s="31" t="s">
         <v>67</v>
       </c>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="32" t="s">
@@ -6070,6 +6098,9 @@
       <c r="C2" s="33" t="s">
         <v>130</v>
       </c>
+      <c r="D2" s="33" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="11.15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="32" t="s">
@@ -6081,6 +6112,9 @@
       <c r="C3" s="33" t="s">
         <v>94</v>
       </c>
+      <c r="D3" s="33" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -6092,6 +6126,9 @@
       <c r="C4" s="0" t="s">
         <v>148</v>
       </c>
+      <c r="D4" s="0" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -6102,6 +6139,9 @@
       </c>
       <c r="C5" s="0" t="s">
         <v>150</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -6123,49 +6163,57 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.515306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="31" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1" s="31"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="32" t="s">
         <v>69</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C2" s="33" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="33" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="32" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B3" s="32" t="s">
         <v>93</v>
       </c>
       <c r="C3" s="33" t="s">
         <v>94</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -6188,37 +6236,40 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E65536"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="1" sqref="3:3 E5"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="13.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="23" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="1016" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="23" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="23" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1017" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1018" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="49.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="32" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>155</v>
-      </c>
-      <c r="C1" s="32" t="s">
         <v>156</v>
       </c>
+      <c r="C1" s="32"/>
       <c r="D1" s="32" t="s">
         <v>157</v>
       </c>
       <c r="E1" s="32" t="s">
         <v>158</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="9.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6226,15 +6277,18 @@
         <v>93</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>159</v>
+        <v>94</v>
       </c>
       <c r="C2" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="E2" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="F2" s="32" t="s">
         <v>162</v>
       </c>
     </row>
@@ -6245,13 +6299,16 @@
       <c r="B3" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="0" t="s">
         <v>164</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>165</v>
       </c>
       <c r="E3" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>133</v>
       </c>
     </row>
@@ -6260,32 +6317,21 @@
         <v>140</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="C4" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="D4" s="23" t="s">
-        <v>167</v>
-      </c>
       <c r="E4" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="F4" s="23" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C3:E3" type="none">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D3:F3" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6307,49 +6353,57 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H18" activeCellId="1" sqref="3:3 H18"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.3214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="31" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1" s="31"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="32" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C2" s="33" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="33" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="32" t="s">
         <v>93</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C3" s="33" t="s">
         <v>94</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6357,7 +6411,10 @@
         <v>133</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -6365,7 +6422,7 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4:D4" type="none">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Fix channel labels (#36)
* Fix CE init fixtures labels
* Fix EE init fixtures labels
</commit_message>
<xml_diff>
--- a/src/Resources/fixtures/minimal/init.xlsx
+++ b/src/Resources/fixtures/minimal/init.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="README-EN" sheetId="1" state="visible" r:id="rId2"/>
@@ -112,7 +112,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -127,7 +127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="450">
   <si>
     <t xml:space="preserve">End user HOWTO</t>
   </si>
@@ -602,6 +602,9 @@
     <t xml:space="preserve">Other</t>
   </si>
   <si>
+    <t xml:space="preserve">Autres</t>
+  </si>
+  <si>
     <t xml:space="preserve">Option properties</t>
   </si>
   <si>
@@ -626,118 +629,124 @@
     <t xml:space="preserve">Category tree</t>
   </si>
   <si>
+    <t xml:space="preserve">locales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">currencies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecommerce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-commerce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">en_US,fr_FR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USD,EUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parent category code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Catégorie principale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group type properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">variant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is_variant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VARIANT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RELATED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Association type properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Association type code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X_SELL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cross sell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPSELL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upsell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUBSTITUTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Substitution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it_support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">redactor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redactor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">role</t>
+  </si>
+  <si>
     <t xml:space="preserve">label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">locales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">currencies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tree</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ecommerce</t>
-  </si>
-  <si>
-    <t xml:space="preserve">en_US,fr_FR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USD,EUR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mobile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category properties</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parent category code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Main category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group type properties</t>
-  </si>
-  <si>
-    <t xml:space="preserve">variant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">is_variant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VARIANT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RELATED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Association type properties</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Association type code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X_SELL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cross sell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPSELL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Upsell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUBSTITUTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Substitution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PACK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">it_support</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IT support</t>
-  </si>
-  <si>
-    <t xml:space="preserve">manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">redactor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Redactor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">all</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All</t>
-  </si>
-  <si>
-    <t xml:space="preserve">role</t>
   </si>
   <si>
     <t xml:space="preserve">ROLE_ADMINISTRATOR</t>
@@ -1902,10 +1911,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>377640</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>138240</xdr:rowOff>
+      <xdr:rowOff>137880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1915,7 +1924,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="6157440" cy="9527760"/>
+          <a:ext cx="7156800" cy="9563760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1947,10 +1956,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>377640</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>138240</xdr:rowOff>
+      <xdr:rowOff>137880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1960,7 +1969,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="6157440" cy="9527760"/>
+          <a:ext cx="7156800" cy="9563760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1997,10 +2006,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>130680</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>130320</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>138240</xdr:rowOff>
+      <xdr:rowOff>110160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2010,7 +2019,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="5853240" cy="8418960"/>
+          <a:ext cx="6986520" cy="8418960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2042,10 +2051,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>130680</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>130320</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>138240</xdr:rowOff>
+      <xdr:rowOff>110160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2055,7 +2064,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="5853240" cy="8418960"/>
+          <a:ext cx="6986520" cy="8418960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2092,7 +2101,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>378000</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>138240</xdr:rowOff>
@@ -2105,7 +2114,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="8034120" cy="9527760"/>
+          <a:ext cx="9545400" cy="9400680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2137,7 +2146,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>378000</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>138240</xdr:rowOff>
@@ -2150,7 +2159,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="8034120" cy="9527760"/>
+          <a:ext cx="9545400" cy="9400680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2185,14 +2194,14 @@
   <dimension ref="A1:B58"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="3:3 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.59183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="113.663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.45408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="112.448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2407,20 +2416,20 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="3:3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B1" s="30"/>
     </row>
@@ -2429,7 +2438,7 @@
         <v>146</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2437,12 +2446,12 @@
         <v>93</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="29" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -2450,7 +2459,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -2481,78 +2490,90 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="1" sqref="3:3 B16"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="34" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="34" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="34" width="27.780612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="35" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B1" s="31" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1" s="31"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="36" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B2" s="31" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="31" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="32" t="s">
         <v>93</v>
       </c>
       <c r="B3" s="33" t="s">
         <v>94</v>
       </c>
+      <c r="C3" s="33" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="29" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>183</v>
+      </c>
+      <c r="C4" s="37"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>185</v>
+      </c>
+      <c r="C5" s="35"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="29" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>187</v>
+      </c>
+      <c r="C6" s="35"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="29" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>187</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="C7" s="35"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B4" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B4:C4" type="none">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2575,14 +2596,14 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2595,34 +2616,34 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -2644,46 +2665,46 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5612244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="38" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>159</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -2705,77 +2726,77 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="3:3"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.3214285714286"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="38" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C1" s="38" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D1" s="38" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="E1" s="38" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="F1" s="38" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="G1" s="38" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="H1" s="38" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="I1" s="38" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="J1" s="38" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="K1" s="38" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L1" s="38" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>218</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>215</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>130</v>
@@ -2790,10 +2811,10 @@
         <v>133</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="L2" s="0" t="n">
         <v>1</v>
@@ -2817,14 +2838,14 @@
   </sheetPr>
   <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="1" sqref="3:3 H12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P25" activeCellId="0" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2832,12 +2853,12 @@
         <v>93</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -2845,7 +2866,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -2853,7 +2874,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0</v>
@@ -2861,7 +2882,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -2869,7 +2890,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0</v>
@@ -2877,7 +2898,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0</v>
@@ -2885,7 +2906,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
@@ -2893,7 +2914,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0</v>
@@ -2901,7 +2922,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0</v>
@@ -2909,7 +2930,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0</v>
@@ -2917,7 +2938,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0</v>
@@ -2925,7 +2946,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0</v>
@@ -2933,7 +2954,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0</v>
@@ -2941,7 +2962,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0</v>
@@ -2949,7 +2970,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0</v>
@@ -2957,7 +2978,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0</v>
@@ -2965,7 +2986,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0</v>
@@ -2973,7 +2994,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0</v>
@@ -2981,7 +3002,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0</v>
@@ -2989,7 +3010,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0</v>
@@ -2997,7 +3018,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0</v>
@@ -3005,7 +3026,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>0</v>
@@ -3013,7 +3034,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>0</v>
@@ -3021,7 +3042,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>0</v>
@@ -3029,7 +3050,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>0</v>
@@ -3037,7 +3058,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>0</v>
@@ -3045,7 +3066,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>0</v>
@@ -3053,7 +3074,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0</v>
@@ -3061,7 +3082,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>0</v>
@@ -3069,7 +3090,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>0</v>
@@ -3077,7 +3098,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>0</v>
@@ -3085,7 +3106,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>0</v>
@@ -3093,7 +3114,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>0</v>
@@ -3101,7 +3122,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>0</v>
@@ -3109,7 +3130,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>0</v>
@@ -3117,7 +3138,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>0</v>
@@ -3125,7 +3146,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>0</v>
@@ -3133,7 +3154,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>0</v>
@@ -3141,7 +3162,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>0</v>
@@ -3149,7 +3170,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>0</v>
@@ -3157,7 +3178,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>0</v>
@@ -3165,7 +3186,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>0</v>
@@ -3173,7 +3194,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>0</v>
@@ -3181,7 +3202,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>0</v>
@@ -3189,7 +3210,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>0</v>
@@ -3197,7 +3218,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>0</v>
@@ -3205,7 +3226,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>0</v>
@@ -3213,7 +3234,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>0</v>
@@ -3221,7 +3242,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>0</v>
@@ -3229,7 +3250,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>0</v>
@@ -3237,7 +3258,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>0</v>
@@ -3245,7 +3266,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>0</v>
@@ -3253,7 +3274,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>0</v>
@@ -3261,7 +3282,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>0</v>
@@ -3269,7 +3290,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>0</v>
@@ -3277,7 +3298,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>0</v>
@@ -3285,7 +3306,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>0</v>
@@ -3293,7 +3314,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>0</v>
@@ -3301,7 +3322,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>0</v>
@@ -3309,7 +3330,7 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>0</v>
@@ -3317,7 +3338,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>0</v>
@@ -3325,7 +3346,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>0</v>
@@ -3333,7 +3354,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>0</v>
@@ -3341,7 +3362,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>0</v>
@@ -3349,7 +3370,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>0</v>
@@ -3357,7 +3378,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>0</v>
@@ -3365,7 +3386,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>0</v>
@@ -3373,7 +3394,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>0</v>
@@ -3381,7 +3402,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>0</v>
@@ -3389,7 +3410,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>0</v>
@@ -3397,7 +3418,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>0</v>
@@ -3405,7 +3426,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>0</v>
@@ -3413,7 +3434,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>0</v>
@@ -3421,7 +3442,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>0</v>
@@ -3429,7 +3450,7 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>0</v>
@@ -3437,7 +3458,7 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>0</v>
@@ -3445,7 +3466,7 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>0</v>
@@ -3453,7 +3474,7 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>0</v>
@@ -3461,7 +3482,7 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>0</v>
@@ -3469,7 +3490,7 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="B81" s="0" t="n">
         <v>0</v>
@@ -3477,7 +3498,7 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>0</v>
@@ -3485,7 +3506,7 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>0</v>
@@ -3493,7 +3514,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>0</v>
@@ -3501,7 +3522,7 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="B85" s="0" t="n">
         <v>0</v>
@@ -3509,7 +3530,7 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="B86" s="0" t="n">
         <v>0</v>
@@ -3517,7 +3538,7 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="B87" s="0" t="n">
         <v>0</v>
@@ -3525,7 +3546,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="B88" s="0" t="n">
         <v>0</v>
@@ -3533,7 +3554,7 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="B89" s="0" t="n">
         <v>0</v>
@@ -3541,7 +3562,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B90" s="0" t="n">
         <v>0</v>
@@ -3549,7 +3570,7 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="B91" s="0" t="n">
         <v>0</v>
@@ -3557,7 +3578,7 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="B92" s="0" t="n">
         <v>0</v>
@@ -3565,7 +3586,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="B93" s="0" t="n">
         <v>0</v>
@@ -3573,7 +3594,7 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="B94" s="0" t="n">
         <v>0</v>
@@ -3581,7 +3602,7 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="B95" s="0" t="n">
         <v>0</v>
@@ -3589,7 +3610,7 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="B96" s="0" t="n">
         <v>0</v>
@@ -3597,7 +3618,7 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="B97" s="0" t="n">
         <v>0</v>
@@ -3605,7 +3626,7 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="B98" s="0" t="n">
         <v>0</v>
@@ -3613,7 +3634,7 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="B99" s="0" t="n">
         <v>0</v>
@@ -3621,7 +3642,7 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="B100" s="0" t="n">
         <v>0</v>
@@ -3629,7 +3650,7 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="B101" s="0" t="n">
         <v>0</v>
@@ -3637,7 +3658,7 @@
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="B102" s="0" t="n">
         <v>0</v>
@@ -3662,12 +3683,12 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="3:3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3675,10 +3696,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3686,18 +3707,18 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -3719,21 +3740,22 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="32" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3741,12 +3763,12 @@
         <v>93</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>159</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>122</v>
@@ -3754,7 +3776,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>126</v>
@@ -3762,7 +3784,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>129</v>
@@ -3770,74 +3792,74 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -3859,21 +3881,22 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="32" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3881,103 +3904,103 @@
         <v>93</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>159</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -3999,18 +4022,19 @@
   <dimension ref="A1:B89"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="32" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="B1" s="32"/>
     </row>
@@ -4019,703 +4043,703 @@
         <v>96</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -4737,12 +4761,14 @@
   <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="1" sqref="3:3 B30"/>
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="174.137755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="172.25"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4935,42 +4961,42 @@
   <dimension ref="A1:AW9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="1" sqref="3:3 B25"/>
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="45" min="27" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="7" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="8" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="49" min="48" style="7" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="50" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="45" min="27" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="7" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="8" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="49" min="48" style="7" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="50" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5409,48 +5435,48 @@
   <dimension ref="A1:AX8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="3:3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5730,47 +5756,47 @@
   <dimension ref="A1:BE7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="1" sqref="3:3 C12"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="6" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="6" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6037,18 +6063,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="1" sqref="3:3 C16"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="14.5867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6059,6 +6086,7 @@
       <c r="C1" s="31" t="s">
         <v>67</v>
       </c>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="32" t="s">
@@ -6070,6 +6098,9 @@
       <c r="C2" s="33" t="s">
         <v>130</v>
       </c>
+      <c r="D2" s="33" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="11.15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="32" t="s">
@@ -6081,6 +6112,9 @@
       <c r="C3" s="33" t="s">
         <v>94</v>
       </c>
+      <c r="D3" s="33" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -6092,6 +6126,9 @@
       <c r="C4" s="0" t="s">
         <v>148</v>
       </c>
+      <c r="D4" s="0" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -6102,6 +6139,9 @@
       </c>
       <c r="C5" s="0" t="s">
         <v>150</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -6123,49 +6163,57 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="3:3 A1"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.515306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="31" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1" s="31"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="32" t="s">
         <v>69</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C2" s="33" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="33" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="32" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B3" s="32" t="s">
         <v>93</v>
       </c>
       <c r="C3" s="33" t="s">
         <v>94</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -6188,37 +6236,40 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E65536"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="1" sqref="3:3 E5"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="13.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="23" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="1016" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="23" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="23" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1017" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1018" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="49.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="32" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>155</v>
-      </c>
-      <c r="C1" s="32" t="s">
         <v>156</v>
       </c>
+      <c r="C1" s="32"/>
       <c r="D1" s="32" t="s">
         <v>157</v>
       </c>
       <c r="E1" s="32" t="s">
         <v>158</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="9.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6226,15 +6277,18 @@
         <v>93</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>159</v>
+        <v>94</v>
       </c>
       <c r="C2" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="E2" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="F2" s="32" t="s">
         <v>162</v>
       </c>
     </row>
@@ -6245,13 +6299,16 @@
       <c r="B3" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="0" t="s">
         <v>164</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>165</v>
       </c>
       <c r="E3" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>133</v>
       </c>
     </row>
@@ -6260,32 +6317,21 @@
         <v>140</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="C4" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="D4" s="23" t="s">
-        <v>167</v>
-      </c>
       <c r="E4" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="F4" s="23" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C3:E3" type="none">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D3:F3" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6307,49 +6353,57 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H18" activeCellId="1" sqref="3:3 H18"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.3214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="31" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1" s="31"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="32" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C2" s="33" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="33" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="32" t="s">
         <v>93</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C3" s="33" t="s">
         <v>94</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6357,7 +6411,10 @@
         <v>133</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -6365,7 +6422,7 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4:D4" type="none">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Fix missing currencies (cf PIM-5978)
</commit_message>
<xml_diff>
--- a/src/Resources/fixtures/minimal/init.xlsx
+++ b/src/Resources/fixtures/minimal/init.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="14"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="README-EN" sheetId="1" state="visible" r:id="rId2"/>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="643">
   <si>
     <t xml:space="preserve">End user HOWTO</t>
   </si>
@@ -830,9 +830,24 @@
     <t xml:space="preserve">AFA</t>
   </si>
   <si>
+    <t xml:space="preserve">AFN</t>
+  </si>
+  <si>
     <t xml:space="preserve">ALK</t>
   </si>
   <si>
+    <t xml:space="preserve">ALL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AOA</t>
+  </si>
+  <si>
     <t xml:space="preserve">AOK</t>
   </si>
   <si>
@@ -842,27 +857,51 @@
     <t xml:space="preserve">AOR</t>
   </si>
   <si>
+    <t xml:space="preserve">ARA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARL</t>
+  </si>
+  <si>
     <t xml:space="preserve">ARM</t>
   </si>
   <si>
     <t xml:space="preserve">ARP</t>
   </si>
   <si>
-    <t xml:space="preserve">ARL</t>
+    <t xml:space="preserve">ARS</t>
   </si>
   <si>
     <t xml:space="preserve">ATS</t>
   </si>
   <si>
+    <t xml:space="preserve">AUD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWG</t>
+  </si>
+  <si>
     <t xml:space="preserve">AZM</t>
   </si>
   <si>
+    <t xml:space="preserve">AZN</t>
+  </si>
+  <si>
     <t xml:space="preserve">BAD</t>
   </si>
   <si>
+    <t xml:space="preserve">BAM</t>
+  </si>
+  <si>
     <t xml:space="preserve">BAN</t>
   </si>
   <si>
+    <t xml:space="preserve">BBD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BDT</t>
+  </si>
+  <si>
     <t xml:space="preserve">BEC</t>
   </si>
   <si>
@@ -878,15 +917,36 @@
     <t xml:space="preserve">BGM</t>
   </si>
   <si>
+    <t xml:space="preserve">BGN</t>
+  </si>
+  <si>
     <t xml:space="preserve">BGO</t>
   </si>
   <si>
+    <t xml:space="preserve">BHD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BIF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOB</t>
+  </si>
+  <si>
     <t xml:space="preserve">BOL</t>
   </si>
   <si>
     <t xml:space="preserve">BOP</t>
   </si>
   <si>
+    <t xml:space="preserve">BOV</t>
+  </si>
+  <si>
     <t xml:space="preserve">BRB</t>
   </si>
   <si>
@@ -896,36 +956,132 @@
     <t xml:space="preserve">BRE</t>
   </si>
   <si>
+    <t xml:space="preserve">BRL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRN</t>
+  </si>
+  <si>
     <t xml:space="preserve">BRR</t>
   </si>
   <si>
-    <t xml:space="preserve">BRN</t>
-  </si>
-  <si>
     <t xml:space="preserve">BRZ</t>
   </si>
   <si>
+    <t xml:space="preserve">BSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BTN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BWP</t>
+  </si>
+  <si>
     <t xml:space="preserve">BYB</t>
   </si>
   <si>
+    <t xml:space="preserve">BYR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BZD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CDF</t>
+  </si>
+  <si>
     <t xml:space="preserve">CHE</t>
   </si>
   <si>
+    <t xml:space="preserve">CHF</t>
+  </si>
+  <si>
     <t xml:space="preserve">CHW</t>
   </si>
   <si>
+    <t xml:space="preserve">CLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CNX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CNY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRC</t>
+  </si>
+  <si>
     <t xml:space="preserve">CSD</t>
   </si>
   <si>
     <t xml:space="preserve">CSK</t>
   </si>
   <si>
+    <t xml:space="preserve">CUC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CVE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CYP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CZK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DDM</t>
+  </si>
+  <si>
     <t xml:space="preserve">DEM</t>
   </si>
   <si>
+    <t xml:space="preserve">DJF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DKK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DZD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECV</t>
+  </si>
+  <si>
     <t xml:space="preserve">EEK</t>
   </si>
   <si>
+    <t xml:space="preserve">EGP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERN</t>
+  </si>
+  <si>
     <t xml:space="preserve">ESA</t>
   </si>
   <si>
@@ -935,120 +1091,516 @@
     <t xml:space="preserve">ESP</t>
   </si>
   <si>
+    <t xml:space="preserve">ETB</t>
+  </si>
+  <si>
     <t xml:space="preserve">FIM</t>
   </si>
   <si>
+    <t xml:space="preserve">FJD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FKP</t>
+  </si>
+  <si>
     <t xml:space="preserve">FRF</t>
   </si>
   <si>
+    <t xml:space="preserve">GBP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GEK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GEL</t>
+  </si>
+  <si>
     <t xml:space="preserve">GHC</t>
   </si>
   <si>
-    <t xml:space="preserve">GBP</t>
+    <t xml:space="preserve">GHS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GQE</t>
   </si>
   <si>
     <t xml:space="preserve">GRD</t>
   </si>
   <si>
+    <t xml:space="preserve">GTQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GWE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GWP</t>
+  </si>
+  <si>
     <t xml:space="preserve">GYD</t>
   </si>
   <si>
+    <t xml:space="preserve">HKD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HNL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HRD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HRK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HUF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDR</t>
+  </si>
+  <si>
     <t xml:space="preserve">IEP</t>
   </si>
   <si>
+    <t xml:space="preserve">ILP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IQD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRR</t>
+  </si>
+  <si>
     <t xml:space="preserve">ISJ</t>
   </si>
   <si>
-    <t xml:space="preserve">ILR</t>
+    <t xml:space="preserve">ISK</t>
   </si>
   <si>
     <t xml:space="preserve">ITL</t>
   </si>
   <si>
+    <t xml:space="preserve">JMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JPY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KHR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KMF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPW</t>
+  </si>
+  <si>
     <t xml:space="preserve">KRH</t>
   </si>
   <si>
     <t xml:space="preserve">KRO</t>
   </si>
   <si>
+    <t xml:space="preserve">KRW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KWD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KYD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KZT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LBP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LKR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LRD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LSL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LUC</t>
+  </si>
+  <si>
     <t xml:space="preserve">LUF</t>
   </si>
   <si>
+    <t xml:space="preserve">LUL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LVL</t>
+  </si>
+  <si>
     <t xml:space="preserve">LVR</t>
   </si>
   <si>
+    <t xml:space="preserve">LYD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MDC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MDL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MGA</t>
+  </si>
+  <si>
     <t xml:space="preserve">MGF</t>
   </si>
   <si>
+    <t xml:space="preserve">MKD</t>
+  </si>
+  <si>
     <t xml:space="preserve">MKN</t>
   </si>
   <si>
+    <t xml:space="preserve">MLF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MMK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MNT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MRO</t>
+  </si>
+  <si>
     <t xml:space="preserve">MTL</t>
   </si>
   <si>
+    <t xml:space="preserve">MTP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MVP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MVR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MWK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MXN</t>
+  </si>
+  <si>
     <t xml:space="preserve">MXP</t>
   </si>
   <si>
+    <t xml:space="preserve">MXV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MYR</t>
+  </si>
+  <si>
     <t xml:space="preserve">MZE</t>
   </si>
   <si>
     <t xml:space="preserve">MZM</t>
   </si>
   <si>
+    <t xml:space="preserve">MZN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NGN</t>
+  </si>
+  <si>
     <t xml:space="preserve">NIC</t>
   </si>
   <si>
+    <t xml:space="preserve">NIO</t>
+  </si>
+  <si>
     <t xml:space="preserve">NLG</t>
   </si>
   <si>
+    <t xml:space="preserve">NOK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NPR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NZD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OMR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEN</t>
+  </si>
+  <si>
     <t xml:space="preserve">PES</t>
   </si>
   <si>
+    <t xml:space="preserve">PGK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PKR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLN</t>
+  </si>
+  <si>
     <t xml:space="preserve">PLZ</t>
   </si>
   <si>
     <t xml:space="preserve">PTE</t>
   </si>
   <si>
+    <t xml:space="preserve">PYG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RHD</t>
+  </si>
+  <si>
     <t xml:space="preserve">ROL</t>
   </si>
   <si>
+    <t xml:space="preserve">RON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RUB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RWF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCR</t>
+  </si>
+  <si>
     <t xml:space="preserve">SDD</t>
   </si>
   <si>
+    <t xml:space="preserve">SDG</t>
+  </si>
+  <si>
     <t xml:space="preserve">SDP</t>
   </si>
   <si>
+    <t xml:space="preserve">SEK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SGD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHP</t>
+  </si>
+  <si>
     <t xml:space="preserve">SIT</t>
   </si>
   <si>
     <t xml:space="preserve">SKK</t>
   </si>
   <si>
+    <t xml:space="preserve">SLL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STD</t>
+  </si>
+  <si>
     <t xml:space="preserve">SUR</t>
   </si>
   <si>
+    <t xml:space="preserve">SVC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SYP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SZL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TJR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TJS</t>
+  </si>
+  <si>
     <t xml:space="preserve">TMM</t>
   </si>
   <si>
+    <t xml:space="preserve">TMT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOP</t>
+  </si>
+  <si>
     <t xml:space="preserve">TPE</t>
   </si>
   <si>
     <t xml:space="preserve">TRL</t>
   </si>
   <si>
+    <t xml:space="preserve">TRY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TZS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UAH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UAK</t>
+  </si>
+  <si>
     <t xml:space="preserve">UGS</t>
   </si>
   <si>
+    <t xml:space="preserve">UGX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UYI</t>
+  </si>
+  <si>
     <t xml:space="preserve">UYP</t>
   </si>
   <si>
+    <t xml:space="preserve">UYU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UZS</t>
+  </si>
+  <si>
     <t xml:space="preserve">VEB</t>
   </si>
   <si>
+    <t xml:space="preserve">VEF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VND</t>
+  </si>
+  <si>
     <t xml:space="preserve">VNN</t>
   </si>
   <si>
+    <t xml:space="preserve">VUV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XAF</t>
+  </si>
+  <si>
     <t xml:space="preserve">XAU</t>
   </si>
   <si>
@@ -1064,6 +1616,12 @@
     <t xml:space="preserve">XBD</t>
   </si>
   <si>
+    <t xml:space="preserve">XCD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XDR</t>
+  </si>
+  <si>
     <t xml:space="preserve">XEU</t>
   </si>
   <si>
@@ -1073,10 +1631,16 @@
     <t xml:space="preserve">XFU</t>
   </si>
   <si>
+    <t xml:space="preserve">XOF</t>
+  </si>
+  <si>
     <t xml:space="preserve">XPD</t>
   </si>
   <si>
-    <t xml:space="preserve">XDR</t>
+    <t xml:space="preserve">XPF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XRE</t>
   </si>
   <si>
     <t xml:space="preserve">XSU</t>
@@ -1088,6 +1652,12 @@
     <t xml:space="preserve">XXX</t>
   </si>
   <si>
+    <t xml:space="preserve">YDD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YER</t>
+  </si>
+  <si>
     <t xml:space="preserve">YUD</t>
   </si>
   <si>
@@ -1100,7 +1670,16 @@
     <t xml:space="preserve">YUR</t>
   </si>
   <si>
+    <t xml:space="preserve">ZAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZAR</t>
+  </si>
+  <si>
     <t xml:space="preserve">ZMK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZMW</t>
   </si>
   <si>
     <t xml:space="preserve">ZRN</t>
@@ -1912,9 +2491,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>377640</xdr:colOff>
+      <xdr:colOff>377280</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>137880</xdr:rowOff>
+      <xdr:rowOff>137520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1924,7 +2503,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="7156800" cy="9563760"/>
+          <a:ext cx="7062120" cy="9563400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1957,9 +2536,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>377640</xdr:colOff>
+      <xdr:colOff>377280</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>137880</xdr:rowOff>
+      <xdr:rowOff>137520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1969,7 +2548,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="7156800" cy="9563760"/>
+          <a:ext cx="7062120" cy="9563400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2007,9 +2586,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>130320</xdr:colOff>
+      <xdr:colOff>129960</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>110160</xdr:rowOff>
+      <xdr:rowOff>109800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2019,7 +2598,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="6986520" cy="8418960"/>
+          <a:ext cx="6881400" cy="8418600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2052,9 +2631,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>130320</xdr:colOff>
+      <xdr:colOff>129960</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>110160</xdr:rowOff>
+      <xdr:rowOff>109800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2064,7 +2643,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="6986520" cy="8418960"/>
+          <a:ext cx="6881400" cy="8418600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2102,9 +2681,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>378000</xdr:colOff>
+      <xdr:colOff>377640</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>138240</xdr:rowOff>
+      <xdr:rowOff>137880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2114,7 +2693,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="9545400" cy="9400680"/>
+          <a:ext cx="9405360" cy="9400320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2147,9 +2726,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>378000</xdr:colOff>
+      <xdr:colOff>377640</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>138240</xdr:rowOff>
+      <xdr:rowOff>137880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2159,7 +2738,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="9545400" cy="9400680"/>
+          <a:ext cx="9405360" cy="9400320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2194,14 +2773,14 @@
   <dimension ref="A1:B58"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="A:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.45408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="112.448979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.32142857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="111.09693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2417,14 +2996,14 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2493,15 +3072,15 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="A:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="34" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="34" width="27.780612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="34" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="34" width="27.4030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="35" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2596,14 +3175,13 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.1479591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2651,8 +3229,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2665,14 +3243,13 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+      <selection pane="topLeft" activeCell="E21" activeCellId="1" sqref="A:B E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5612244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.25"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2712,8 +3289,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2726,22 +3303,23 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="1" sqref="A:B H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2825,8 +3403,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2836,16 +3414,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B102"/>
+  <dimension ref="A1:B295"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P25" activeCellId="0" sqref="P25"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="A:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3664,13 +4241,1557 @@
         <v>0</v>
       </c>
     </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="B103" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="B104" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="B105" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="B106" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="B107" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="B108" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="B109" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="B110" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="B111" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
+        <v>332</v>
+      </c>
+      <c r="B112" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="B113" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="B114" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="B115" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="B116" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="B117" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>338</v>
+      </c>
+      <c r="B118" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="B119" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="B120" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="B121" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>342</v>
+      </c>
+      <c r="B122" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="B123" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="B124" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="s">
+        <v>345</v>
+      </c>
+      <c r="B125" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="B126" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="B127" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="B128" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="B129" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="B130" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="B131" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="B132" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="B133" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="B134" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="B135" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="B136" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="s">
+        <v>357</v>
+      </c>
+      <c r="B137" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="B138" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="B139" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="B140" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="B141" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="s">
+        <v>362</v>
+      </c>
+      <c r="B142" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="B143" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="s">
+        <v>364</v>
+      </c>
+      <c r="B144" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="B145" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="s">
+        <v>366</v>
+      </c>
+      <c r="B146" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="B147" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="s">
+        <v>368</v>
+      </c>
+      <c r="B148" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="B149" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="B150" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="B151" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0" t="s">
+        <v>372</v>
+      </c>
+      <c r="B152" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="B153" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="B154" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="B155" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="B156" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="B157" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="B158" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="0" t="s">
+        <v>379</v>
+      </c>
+      <c r="B159" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="B160" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="s">
+        <v>381</v>
+      </c>
+      <c r="B161" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="B162" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="B163" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="B164" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="B165" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="B166" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="B167" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="s">
+        <v>388</v>
+      </c>
+      <c r="B168" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="B169" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="B170" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="B171" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="B172" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="s">
+        <v>393</v>
+      </c>
+      <c r="B173" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="B174" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="s">
+        <v>395</v>
+      </c>
+      <c r="B175" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="B176" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="s">
+        <v>397</v>
+      </c>
+      <c r="B177" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="B178" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="B179" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="B180" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="B181" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0" t="s">
+        <v>402</v>
+      </c>
+      <c r="B182" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="s">
+        <v>403</v>
+      </c>
+      <c r="B183" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="B184" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="0" t="s">
+        <v>405</v>
+      </c>
+      <c r="B185" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="0" t="s">
+        <v>406</v>
+      </c>
+      <c r="B186" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="0" t="s">
+        <v>407</v>
+      </c>
+      <c r="B187" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="B188" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="0" t="s">
+        <v>409</v>
+      </c>
+      <c r="B189" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="B190" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="0" t="s">
+        <v>411</v>
+      </c>
+      <c r="B191" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="0" t="s">
+        <v>412</v>
+      </c>
+      <c r="B192" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="B193" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="0" t="s">
+        <v>414</v>
+      </c>
+      <c r="B194" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="0" t="s">
+        <v>415</v>
+      </c>
+      <c r="B195" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="0" t="s">
+        <v>416</v>
+      </c>
+      <c r="B196" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="0" t="s">
+        <v>417</v>
+      </c>
+      <c r="B197" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="B198" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="0" t="s">
+        <v>419</v>
+      </c>
+      <c r="B199" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="0" t="s">
+        <v>420</v>
+      </c>
+      <c r="B200" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="0" t="s">
+        <v>421</v>
+      </c>
+      <c r="B201" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="0" t="s">
+        <v>422</v>
+      </c>
+      <c r="B202" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="0" t="s">
+        <v>423</v>
+      </c>
+      <c r="B203" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="0" t="s">
+        <v>424</v>
+      </c>
+      <c r="B204" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="0" t="s">
+        <v>425</v>
+      </c>
+      <c r="B205" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="0" t="s">
+        <v>426</v>
+      </c>
+      <c r="B206" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="0" t="s">
+        <v>427</v>
+      </c>
+      <c r="B207" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="B208" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="0" t="s">
+        <v>429</v>
+      </c>
+      <c r="B209" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="0" t="s">
+        <v>430</v>
+      </c>
+      <c r="B210" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="B211" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="0" t="s">
+        <v>432</v>
+      </c>
+      <c r="B212" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="B213" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="0" t="s">
+        <v>434</v>
+      </c>
+      <c r="B214" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="B215" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="0" t="s">
+        <v>436</v>
+      </c>
+      <c r="B216" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="B217" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="B218" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="B219" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="0" t="s">
+        <v>440</v>
+      </c>
+      <c r="B220" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="0" t="s">
+        <v>441</v>
+      </c>
+      <c r="B221" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A222" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="B222" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="0" t="s">
+        <v>443</v>
+      </c>
+      <c r="B223" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="B224" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A225" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="B225" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A226" s="0" t="s">
+        <v>446</v>
+      </c>
+      <c r="B226" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A227" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="B227" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="B228" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="0" t="s">
+        <v>449</v>
+      </c>
+      <c r="B229" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="0" t="s">
+        <v>450</v>
+      </c>
+      <c r="B230" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A231" s="0" t="s">
+        <v>451</v>
+      </c>
+      <c r="B231" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A232" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="B232" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A233" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="B233" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A234" s="0" t="s">
+        <v>454</v>
+      </c>
+      <c r="B234" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A235" s="0" t="s">
+        <v>455</v>
+      </c>
+      <c r="B235" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A236" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="B236" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A237" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="B237" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A238" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="B238" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A239" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="B239" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A240" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="B240" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A241" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="B241" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A242" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="B242" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A243" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="B243" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="0" t="s">
+        <v>464</v>
+      </c>
+      <c r="B244" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A245" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="B245" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A246" s="0" t="s">
+        <v>466</v>
+      </c>
+      <c r="B246" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="0" t="s">
+        <v>467</v>
+      </c>
+      <c r="B247" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="0" t="s">
+        <v>468</v>
+      </c>
+      <c r="B248" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="B249" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="B250" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A251" s="0" t="s">
+        <v>471</v>
+      </c>
+      <c r="B251" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A252" s="0" t="s">
+        <v>472</v>
+      </c>
+      <c r="B252" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A253" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="B253" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A254" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B254" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="B255" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A256" s="0" t="s">
+        <v>476</v>
+      </c>
+      <c r="B256" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A257" s="0" t="s">
+        <v>477</v>
+      </c>
+      <c r="B257" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A258" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="B258" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="0" t="s">
+        <v>479</v>
+      </c>
+      <c r="B259" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A260" s="0" t="s">
+        <v>480</v>
+      </c>
+      <c r="B260" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A261" s="0" t="s">
+        <v>481</v>
+      </c>
+      <c r="B261" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A262" s="0" t="s">
+        <v>482</v>
+      </c>
+      <c r="B262" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A263" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="B263" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A264" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="B264" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A265" s="0" t="s">
+        <v>485</v>
+      </c>
+      <c r="B265" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A266" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="B266" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A267" s="0" t="s">
+        <v>487</v>
+      </c>
+      <c r="B267" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A268" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="B268" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A269" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="B269" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A270" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="B270" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="0" t="s">
+        <v>491</v>
+      </c>
+      <c r="B271" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A272" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="B272" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A273" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="B273" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="B274" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A275" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="B275" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A276" s="0" t="s">
+        <v>496</v>
+      </c>
+      <c r="B276" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A277" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="B277" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A278" s="0" t="s">
+        <v>498</v>
+      </c>
+      <c r="B278" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A279" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="B279" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A280" s="0" t="s">
+        <v>500</v>
+      </c>
+      <c r="B280" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A281" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="B281" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A282" s="0" t="s">
+        <v>502</v>
+      </c>
+      <c r="B282" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A283" s="0" t="s">
+        <v>503</v>
+      </c>
+      <c r="B283" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A284" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="B284" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A285" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="B285" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A286" s="0" t="s">
+        <v>506</v>
+      </c>
+      <c r="B286" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A287" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="B287" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A288" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="B288" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A289" s="0" t="s">
+        <v>509</v>
+      </c>
+      <c r="B289" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A290" s="0" t="s">
+        <v>510</v>
+      </c>
+      <c r="B290" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A291" s="0" t="s">
+        <v>511</v>
+      </c>
+      <c r="B291" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A292" s="0" t="s">
+        <v>512</v>
+      </c>
+      <c r="B292" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A293" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="B293" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A294" s="0" t="s">
+        <v>514</v>
+      </c>
+      <c r="B294" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A295" s="0" t="s">
+        <v>515</v>
+      </c>
+      <c r="B295" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -3683,12 +5804,12 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="A:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3696,10 +5817,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>323</v>
+        <v>516</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>324</v>
+        <v>517</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3710,15 +5831,15 @@
         <v>209</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>325</v>
+        <v>518</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>326</v>
+        <v>519</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>327</v>
+        <v>520</v>
       </c>
     </row>
   </sheetData>
@@ -3740,22 +5861,22 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="32" t="s">
-        <v>328</v>
+        <v>521</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>329</v>
+        <v>522</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3768,7 +5889,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>330</v>
+        <v>523</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>122</v>
@@ -3776,7 +5897,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>331</v>
+        <v>524</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>126</v>
@@ -3784,7 +5905,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>332</v>
+        <v>525</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>129</v>
@@ -3792,74 +5913,74 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>333</v>
+        <v>526</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>334</v>
+        <v>527</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>335</v>
+        <v>528</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>336</v>
+        <v>529</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>337</v>
+        <v>530</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>338</v>
+        <v>531</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>339</v>
+        <v>532</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>340</v>
+        <v>533</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>341</v>
+        <v>534</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>342</v>
+        <v>535</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>343</v>
+        <v>536</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>344</v>
+        <v>537</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>345</v>
+        <v>538</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>346</v>
+        <v>539</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>347</v>
+        <v>540</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>348</v>
+        <v>541</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>349</v>
+        <v>542</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>350</v>
+        <v>543</v>
       </c>
     </row>
   </sheetData>
@@ -3867,8 +5988,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -3881,22 +6002,22 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="32" t="s">
-        <v>328</v>
+        <v>521</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>329</v>
+        <v>522</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3909,98 +6030,98 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>352</v>
+        <v>545</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>352</v>
+        <v>545</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>353</v>
+        <v>546</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>353</v>
+        <v>546</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>355</v>
+        <v>548</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>355</v>
+        <v>548</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>356</v>
+        <v>549</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>356</v>
+        <v>549</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>357</v>
+        <v>550</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>357</v>
+        <v>550</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>359</v>
+        <v>552</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>359</v>
+        <v>552</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>360</v>
+        <v>553</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>360</v>
+        <v>553</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>361</v>
+        <v>554</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>361</v>
+        <v>554</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>362</v>
+        <v>555</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>362</v>
+        <v>555</v>
       </c>
     </row>
   </sheetData>
@@ -4008,8 +6129,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -4022,19 +6143,19 @@
   <dimension ref="A1:B89"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="32" t="s">
-        <v>328</v>
+        <v>521</v>
       </c>
       <c r="B1" s="32"/>
     </row>
@@ -4043,703 +6164,703 @@
         <v>96</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>363</v>
+        <v>556</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>364</v>
+        <v>557</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>365</v>
+        <v>558</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>366</v>
+        <v>559</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>367</v>
+        <v>560</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>368</v>
+        <v>561</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>369</v>
+        <v>562</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>370</v>
+        <v>563</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>371</v>
+        <v>564</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>372</v>
+        <v>565</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>373</v>
+        <v>566</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>374</v>
+        <v>567</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>375</v>
+        <v>568</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>376</v>
+        <v>569</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>377</v>
+        <v>570</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>378</v>
+        <v>571</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>379</v>
+        <v>572</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>380</v>
+        <v>573</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>381</v>
+        <v>574</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>352</v>
+        <v>545</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>382</v>
+        <v>575</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>352</v>
+        <v>545</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>383</v>
+        <v>576</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>352</v>
+        <v>545</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>384</v>
+        <v>577</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>352</v>
+        <v>545</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>385</v>
+        <v>578</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>352</v>
+        <v>545</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>386</v>
+        <v>579</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>352</v>
+        <v>545</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>387</v>
+        <v>580</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>353</v>
+        <v>546</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>388</v>
+        <v>581</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>353</v>
+        <v>546</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>389</v>
+        <v>582</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>353</v>
+        <v>546</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>390</v>
+        <v>583</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>353</v>
+        <v>546</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>391</v>
+        <v>584</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>353</v>
+        <v>546</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>392</v>
+        <v>585</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>393</v>
+        <v>586</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>394</v>
+        <v>587</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>395</v>
+        <v>588</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>396</v>
+        <v>589</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>397</v>
+        <v>590</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>398</v>
+        <v>591</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>399</v>
+        <v>592</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>400</v>
+        <v>593</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>401</v>
+        <v>594</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>402</v>
+        <v>595</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>403</v>
+        <v>596</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>404</v>
+        <v>597</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>405</v>
+        <v>598</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>406</v>
+        <v>599</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>355</v>
+        <v>548</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>407</v>
+        <v>600</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>355</v>
+        <v>548</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>408</v>
+        <v>601</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>355</v>
+        <v>548</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>409</v>
+        <v>602</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>355</v>
+        <v>548</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>410</v>
+        <v>603</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>355</v>
+        <v>548</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>411</v>
+        <v>604</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>356</v>
+        <v>549</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>412</v>
+        <v>605</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>356</v>
+        <v>549</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>413</v>
+        <v>606</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>356</v>
+        <v>549</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>414</v>
+        <v>607</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>356</v>
+        <v>549</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>415</v>
+        <v>608</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>356</v>
+        <v>549</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>416</v>
+        <v>609</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>356</v>
+        <v>549</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>417</v>
+        <v>610</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>356</v>
+        <v>549</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>418</v>
+        <v>611</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>356</v>
+        <v>549</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>419</v>
+        <v>612</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>357</v>
+        <v>550</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>420</v>
+        <v>613</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>357</v>
+        <v>550</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>421</v>
+        <v>614</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>357</v>
+        <v>550</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>422</v>
+        <v>615</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>357</v>
+        <v>550</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>423</v>
+        <v>616</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>357</v>
+        <v>550</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>424</v>
+        <v>617</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>425</v>
+        <v>618</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>426</v>
+        <v>619</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>427</v>
+        <v>620</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>428</v>
+        <v>621</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>429</v>
+        <v>622</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>430</v>
+        <v>623</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>431</v>
+        <v>624</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>432</v>
+        <v>625</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>433</v>
+        <v>626</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>434</v>
+        <v>627</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>435</v>
+        <v>628</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>436</v>
+        <v>629</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>437</v>
+        <v>630</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>438</v>
+        <v>631</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>439</v>
+        <v>632</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>359</v>
+        <v>552</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>440</v>
+        <v>633</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>359</v>
+        <v>552</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>441</v>
+        <v>634</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>359</v>
+        <v>552</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>442</v>
+        <v>635</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>359</v>
+        <v>552</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>443</v>
+        <v>636</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>359</v>
+        <v>552</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>444</v>
+        <v>637</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>359</v>
+        <v>552</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>445</v>
+        <v>638</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>359</v>
+        <v>552</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>446</v>
+        <v>639</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>359</v>
+        <v>552</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>447</v>
+        <v>640</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>359</v>
+        <v>552</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>438</v>
+        <v>631</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>359</v>
+        <v>552</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>448</v>
+        <v>641</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>359</v>
+        <v>552</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>449</v>
+        <v>642</v>
       </c>
     </row>
   </sheetData>
@@ -4747,8 +6868,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -4761,14 +6882,14 @@
   <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="A:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="172.25"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="170.357142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4947,8 +7068,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -4961,42 +7082,42 @@
   <dimension ref="A1:AW9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="A:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="45" min="27" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="7" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="8" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="49" min="48" style="7" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="50" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="45" min="27" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="7" width="6.75"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="8" width="6.75"/>
+    <col collapsed="false" hidden="false" max="49" min="48" style="7" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="50" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5435,48 +7556,48 @@
   <dimension ref="A1:AX8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="A:B C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="20.25"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="6.75"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="6.75"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="6.75"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5756,47 +7877,47 @@
   <dimension ref="A1:BE7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="1" sqref="A:B C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="6" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="20.25"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="6" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="6.75"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="6.75"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="6.75"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6066,16 +8187,15 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="1" sqref="A:B C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="14.5867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="14.3112244897959"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6166,16 +8286,15 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="1" sqref="A:B D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.515306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3877551020408"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6239,19 +8358,18 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="1" sqref="A:B C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="23" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="23" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1017" min="7" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="1018" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="23" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="23" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="1018" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="49.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6356,16 +8474,15 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="1" sqref="A:B D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.0408163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6785714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Fix missing currencies (cf PIM-5978) (#43)
</commit_message>
<xml_diff>
--- a/src/Resources/fixtures/minimal/init.xlsx
+++ b/src/Resources/fixtures/minimal/init.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="14"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="README-EN" sheetId="1" state="visible" r:id="rId2"/>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="643">
   <si>
     <t xml:space="preserve">End user HOWTO</t>
   </si>
@@ -830,9 +830,24 @@
     <t xml:space="preserve">AFA</t>
   </si>
   <si>
+    <t xml:space="preserve">AFN</t>
+  </si>
+  <si>
     <t xml:space="preserve">ALK</t>
   </si>
   <si>
+    <t xml:space="preserve">ALL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AOA</t>
+  </si>
+  <si>
     <t xml:space="preserve">AOK</t>
   </si>
   <si>
@@ -842,27 +857,51 @@
     <t xml:space="preserve">AOR</t>
   </si>
   <si>
+    <t xml:space="preserve">ARA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARL</t>
+  </si>
+  <si>
     <t xml:space="preserve">ARM</t>
   </si>
   <si>
     <t xml:space="preserve">ARP</t>
   </si>
   <si>
-    <t xml:space="preserve">ARL</t>
+    <t xml:space="preserve">ARS</t>
   </si>
   <si>
     <t xml:space="preserve">ATS</t>
   </si>
   <si>
+    <t xml:space="preserve">AUD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWG</t>
+  </si>
+  <si>
     <t xml:space="preserve">AZM</t>
   </si>
   <si>
+    <t xml:space="preserve">AZN</t>
+  </si>
+  <si>
     <t xml:space="preserve">BAD</t>
   </si>
   <si>
+    <t xml:space="preserve">BAM</t>
+  </si>
+  <si>
     <t xml:space="preserve">BAN</t>
   </si>
   <si>
+    <t xml:space="preserve">BBD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BDT</t>
+  </si>
+  <si>
     <t xml:space="preserve">BEC</t>
   </si>
   <si>
@@ -878,15 +917,36 @@
     <t xml:space="preserve">BGM</t>
   </si>
   <si>
+    <t xml:space="preserve">BGN</t>
+  </si>
+  <si>
     <t xml:space="preserve">BGO</t>
   </si>
   <si>
+    <t xml:space="preserve">BHD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BIF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOB</t>
+  </si>
+  <si>
     <t xml:space="preserve">BOL</t>
   </si>
   <si>
     <t xml:space="preserve">BOP</t>
   </si>
   <si>
+    <t xml:space="preserve">BOV</t>
+  </si>
+  <si>
     <t xml:space="preserve">BRB</t>
   </si>
   <si>
@@ -896,36 +956,132 @@
     <t xml:space="preserve">BRE</t>
   </si>
   <si>
+    <t xml:space="preserve">BRL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRN</t>
+  </si>
+  <si>
     <t xml:space="preserve">BRR</t>
   </si>
   <si>
-    <t xml:space="preserve">BRN</t>
-  </si>
-  <si>
     <t xml:space="preserve">BRZ</t>
   </si>
   <si>
+    <t xml:space="preserve">BSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BTN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BWP</t>
+  </si>
+  <si>
     <t xml:space="preserve">BYB</t>
   </si>
   <si>
+    <t xml:space="preserve">BYR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BZD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CDF</t>
+  </si>
+  <si>
     <t xml:space="preserve">CHE</t>
   </si>
   <si>
+    <t xml:space="preserve">CHF</t>
+  </si>
+  <si>
     <t xml:space="preserve">CHW</t>
   </si>
   <si>
+    <t xml:space="preserve">CLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CNX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CNY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRC</t>
+  </si>
+  <si>
     <t xml:space="preserve">CSD</t>
   </si>
   <si>
     <t xml:space="preserve">CSK</t>
   </si>
   <si>
+    <t xml:space="preserve">CUC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CVE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CYP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CZK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DDM</t>
+  </si>
+  <si>
     <t xml:space="preserve">DEM</t>
   </si>
   <si>
+    <t xml:space="preserve">DJF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DKK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DZD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECV</t>
+  </si>
+  <si>
     <t xml:space="preserve">EEK</t>
   </si>
   <si>
+    <t xml:space="preserve">EGP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERN</t>
+  </si>
+  <si>
     <t xml:space="preserve">ESA</t>
   </si>
   <si>
@@ -935,120 +1091,516 @@
     <t xml:space="preserve">ESP</t>
   </si>
   <si>
+    <t xml:space="preserve">ETB</t>
+  </si>
+  <si>
     <t xml:space="preserve">FIM</t>
   </si>
   <si>
+    <t xml:space="preserve">FJD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FKP</t>
+  </si>
+  <si>
     <t xml:space="preserve">FRF</t>
   </si>
   <si>
+    <t xml:space="preserve">GBP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GEK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GEL</t>
+  </si>
+  <si>
     <t xml:space="preserve">GHC</t>
   </si>
   <si>
-    <t xml:space="preserve">GBP</t>
+    <t xml:space="preserve">GHS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GQE</t>
   </si>
   <si>
     <t xml:space="preserve">GRD</t>
   </si>
   <si>
+    <t xml:space="preserve">GTQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GWE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GWP</t>
+  </si>
+  <si>
     <t xml:space="preserve">GYD</t>
   </si>
   <si>
+    <t xml:space="preserve">HKD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HNL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HRD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HRK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HUF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDR</t>
+  </si>
+  <si>
     <t xml:space="preserve">IEP</t>
   </si>
   <si>
+    <t xml:space="preserve">ILP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IQD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRR</t>
+  </si>
+  <si>
     <t xml:space="preserve">ISJ</t>
   </si>
   <si>
-    <t xml:space="preserve">ILR</t>
+    <t xml:space="preserve">ISK</t>
   </si>
   <si>
     <t xml:space="preserve">ITL</t>
   </si>
   <si>
+    <t xml:space="preserve">JMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JPY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KHR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KMF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPW</t>
+  </si>
+  <si>
     <t xml:space="preserve">KRH</t>
   </si>
   <si>
     <t xml:space="preserve">KRO</t>
   </si>
   <si>
+    <t xml:space="preserve">KRW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KWD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KYD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KZT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LBP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LKR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LRD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LSL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LUC</t>
+  </si>
+  <si>
     <t xml:space="preserve">LUF</t>
   </si>
   <si>
+    <t xml:space="preserve">LUL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LVL</t>
+  </si>
+  <si>
     <t xml:space="preserve">LVR</t>
   </si>
   <si>
+    <t xml:space="preserve">LYD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MDC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MDL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MGA</t>
+  </si>
+  <si>
     <t xml:space="preserve">MGF</t>
   </si>
   <si>
+    <t xml:space="preserve">MKD</t>
+  </si>
+  <si>
     <t xml:space="preserve">MKN</t>
   </si>
   <si>
+    <t xml:space="preserve">MLF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MMK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MNT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MRO</t>
+  </si>
+  <si>
     <t xml:space="preserve">MTL</t>
   </si>
   <si>
+    <t xml:space="preserve">MTP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MVP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MVR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MWK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MXN</t>
+  </si>
+  <si>
     <t xml:space="preserve">MXP</t>
   </si>
   <si>
+    <t xml:space="preserve">MXV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MYR</t>
+  </si>
+  <si>
     <t xml:space="preserve">MZE</t>
   </si>
   <si>
     <t xml:space="preserve">MZM</t>
   </si>
   <si>
+    <t xml:space="preserve">MZN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NGN</t>
+  </si>
+  <si>
     <t xml:space="preserve">NIC</t>
   </si>
   <si>
+    <t xml:space="preserve">NIO</t>
+  </si>
+  <si>
     <t xml:space="preserve">NLG</t>
   </si>
   <si>
+    <t xml:space="preserve">NOK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NPR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NZD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OMR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEN</t>
+  </si>
+  <si>
     <t xml:space="preserve">PES</t>
   </si>
   <si>
+    <t xml:space="preserve">PGK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PKR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLN</t>
+  </si>
+  <si>
     <t xml:space="preserve">PLZ</t>
   </si>
   <si>
     <t xml:space="preserve">PTE</t>
   </si>
   <si>
+    <t xml:space="preserve">PYG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RHD</t>
+  </si>
+  <si>
     <t xml:space="preserve">ROL</t>
   </si>
   <si>
+    <t xml:space="preserve">RON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RUB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RWF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCR</t>
+  </si>
+  <si>
     <t xml:space="preserve">SDD</t>
   </si>
   <si>
+    <t xml:space="preserve">SDG</t>
+  </si>
+  <si>
     <t xml:space="preserve">SDP</t>
   </si>
   <si>
+    <t xml:space="preserve">SEK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SGD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHP</t>
+  </si>
+  <si>
     <t xml:space="preserve">SIT</t>
   </si>
   <si>
     <t xml:space="preserve">SKK</t>
   </si>
   <si>
+    <t xml:space="preserve">SLL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STD</t>
+  </si>
+  <si>
     <t xml:space="preserve">SUR</t>
   </si>
   <si>
+    <t xml:space="preserve">SVC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SYP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SZL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TJR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TJS</t>
+  </si>
+  <si>
     <t xml:space="preserve">TMM</t>
   </si>
   <si>
+    <t xml:space="preserve">TMT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOP</t>
+  </si>
+  <si>
     <t xml:space="preserve">TPE</t>
   </si>
   <si>
     <t xml:space="preserve">TRL</t>
   </si>
   <si>
+    <t xml:space="preserve">TRY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TZS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UAH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UAK</t>
+  </si>
+  <si>
     <t xml:space="preserve">UGS</t>
   </si>
   <si>
+    <t xml:space="preserve">UGX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UYI</t>
+  </si>
+  <si>
     <t xml:space="preserve">UYP</t>
   </si>
   <si>
+    <t xml:space="preserve">UYU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UZS</t>
+  </si>
+  <si>
     <t xml:space="preserve">VEB</t>
   </si>
   <si>
+    <t xml:space="preserve">VEF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VND</t>
+  </si>
+  <si>
     <t xml:space="preserve">VNN</t>
   </si>
   <si>
+    <t xml:space="preserve">VUV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XAF</t>
+  </si>
+  <si>
     <t xml:space="preserve">XAU</t>
   </si>
   <si>
@@ -1064,6 +1616,12 @@
     <t xml:space="preserve">XBD</t>
   </si>
   <si>
+    <t xml:space="preserve">XCD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XDR</t>
+  </si>
+  <si>
     <t xml:space="preserve">XEU</t>
   </si>
   <si>
@@ -1073,10 +1631,16 @@
     <t xml:space="preserve">XFU</t>
   </si>
   <si>
+    <t xml:space="preserve">XOF</t>
+  </si>
+  <si>
     <t xml:space="preserve">XPD</t>
   </si>
   <si>
-    <t xml:space="preserve">XDR</t>
+    <t xml:space="preserve">XPF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XRE</t>
   </si>
   <si>
     <t xml:space="preserve">XSU</t>
@@ -1088,6 +1652,12 @@
     <t xml:space="preserve">XXX</t>
   </si>
   <si>
+    <t xml:space="preserve">YDD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YER</t>
+  </si>
+  <si>
     <t xml:space="preserve">YUD</t>
   </si>
   <si>
@@ -1100,7 +1670,16 @@
     <t xml:space="preserve">YUR</t>
   </si>
   <si>
+    <t xml:space="preserve">ZAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZAR</t>
+  </si>
+  <si>
     <t xml:space="preserve">ZMK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZMW</t>
   </si>
   <si>
     <t xml:space="preserve">ZRN</t>
@@ -1912,9 +2491,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>377640</xdr:colOff>
+      <xdr:colOff>377280</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>137880</xdr:rowOff>
+      <xdr:rowOff>137520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1924,7 +2503,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="7156800" cy="9563760"/>
+          <a:ext cx="7062120" cy="9563400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1957,9 +2536,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>377640</xdr:colOff>
+      <xdr:colOff>377280</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>137880</xdr:rowOff>
+      <xdr:rowOff>137520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1969,7 +2548,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="7156800" cy="9563760"/>
+          <a:ext cx="7062120" cy="9563400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2007,9 +2586,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>130320</xdr:colOff>
+      <xdr:colOff>129960</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>110160</xdr:rowOff>
+      <xdr:rowOff>109800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2019,7 +2598,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="6986520" cy="8418960"/>
+          <a:ext cx="6881400" cy="8418600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2052,9 +2631,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>130320</xdr:colOff>
+      <xdr:colOff>129960</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>110160</xdr:rowOff>
+      <xdr:rowOff>109800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2064,7 +2643,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="6986520" cy="8418960"/>
+          <a:ext cx="6881400" cy="8418600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2102,9 +2681,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>378000</xdr:colOff>
+      <xdr:colOff>377640</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>138240</xdr:rowOff>
+      <xdr:rowOff>137880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2114,7 +2693,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="9545400" cy="9400680"/>
+          <a:ext cx="9405360" cy="9400320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2147,9 +2726,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>378000</xdr:colOff>
+      <xdr:colOff>377640</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>138240</xdr:rowOff>
+      <xdr:rowOff>137880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2159,7 +2738,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="9545400" cy="9400680"/>
+          <a:ext cx="9405360" cy="9400320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2194,14 +2773,14 @@
   <dimension ref="A1:B58"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="A:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.45408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="112.448979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.32142857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="111.09693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2417,14 +2996,14 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2493,15 +3072,15 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="A:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="34" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="34" width="27.780612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="34" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="34" width="27.4030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="35" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2596,14 +3175,13 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.1479591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2651,8 +3229,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2665,14 +3243,13 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+      <selection pane="topLeft" activeCell="E21" activeCellId="1" sqref="A:B E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5612244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.25"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2712,8 +3289,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2726,22 +3303,23 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="1" sqref="A:B H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2825,8 +3403,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2836,16 +3414,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B102"/>
+  <dimension ref="A1:B295"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P25" activeCellId="0" sqref="P25"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="A:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3664,13 +4241,1557 @@
         <v>0</v>
       </c>
     </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="B103" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="B104" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="B105" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="B106" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="B107" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="B108" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="B109" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="B110" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="B111" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
+        <v>332</v>
+      </c>
+      <c r="B112" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="B113" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="B114" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="B115" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="B116" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="B117" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>338</v>
+      </c>
+      <c r="B118" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="B119" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="B120" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="B121" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>342</v>
+      </c>
+      <c r="B122" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="B123" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="B124" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="s">
+        <v>345</v>
+      </c>
+      <c r="B125" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="B126" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="B127" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="B128" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="B129" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="B130" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="B131" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="B132" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="B133" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="B134" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="B135" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="B136" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="s">
+        <v>357</v>
+      </c>
+      <c r="B137" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="B138" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="B139" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="B140" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="B141" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="s">
+        <v>362</v>
+      </c>
+      <c r="B142" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="B143" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="s">
+        <v>364</v>
+      </c>
+      <c r="B144" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="B145" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="s">
+        <v>366</v>
+      </c>
+      <c r="B146" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="B147" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="s">
+        <v>368</v>
+      </c>
+      <c r="B148" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="B149" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="B150" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="B151" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0" t="s">
+        <v>372</v>
+      </c>
+      <c r="B152" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="B153" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="B154" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="B155" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="B156" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="B157" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="B158" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="0" t="s">
+        <v>379</v>
+      </c>
+      <c r="B159" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="B160" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="s">
+        <v>381</v>
+      </c>
+      <c r="B161" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="B162" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="B163" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="B164" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="B165" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="B166" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="B167" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="s">
+        <v>388</v>
+      </c>
+      <c r="B168" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="B169" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="B170" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="B171" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="B172" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="s">
+        <v>393</v>
+      </c>
+      <c r="B173" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="B174" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="s">
+        <v>395</v>
+      </c>
+      <c r="B175" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="B176" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="s">
+        <v>397</v>
+      </c>
+      <c r="B177" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="B178" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="B179" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="B180" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="B181" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0" t="s">
+        <v>402</v>
+      </c>
+      <c r="B182" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="s">
+        <v>403</v>
+      </c>
+      <c r="B183" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="B184" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="0" t="s">
+        <v>405</v>
+      </c>
+      <c r="B185" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="0" t="s">
+        <v>406</v>
+      </c>
+      <c r="B186" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="0" t="s">
+        <v>407</v>
+      </c>
+      <c r="B187" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="B188" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="0" t="s">
+        <v>409</v>
+      </c>
+      <c r="B189" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="B190" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="0" t="s">
+        <v>411</v>
+      </c>
+      <c r="B191" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="0" t="s">
+        <v>412</v>
+      </c>
+      <c r="B192" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="B193" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="0" t="s">
+        <v>414</v>
+      </c>
+      <c r="B194" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="0" t="s">
+        <v>415</v>
+      </c>
+      <c r="B195" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="0" t="s">
+        <v>416</v>
+      </c>
+      <c r="B196" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="0" t="s">
+        <v>417</v>
+      </c>
+      <c r="B197" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="B198" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="0" t="s">
+        <v>419</v>
+      </c>
+      <c r="B199" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="0" t="s">
+        <v>420</v>
+      </c>
+      <c r="B200" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="0" t="s">
+        <v>421</v>
+      </c>
+      <c r="B201" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="0" t="s">
+        <v>422</v>
+      </c>
+      <c r="B202" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="0" t="s">
+        <v>423</v>
+      </c>
+      <c r="B203" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="0" t="s">
+        <v>424</v>
+      </c>
+      <c r="B204" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="0" t="s">
+        <v>425</v>
+      </c>
+      <c r="B205" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="0" t="s">
+        <v>426</v>
+      </c>
+      <c r="B206" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="0" t="s">
+        <v>427</v>
+      </c>
+      <c r="B207" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="B208" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="0" t="s">
+        <v>429</v>
+      </c>
+      <c r="B209" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="0" t="s">
+        <v>430</v>
+      </c>
+      <c r="B210" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="B211" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="0" t="s">
+        <v>432</v>
+      </c>
+      <c r="B212" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="B213" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="0" t="s">
+        <v>434</v>
+      </c>
+      <c r="B214" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="B215" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="0" t="s">
+        <v>436</v>
+      </c>
+      <c r="B216" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="B217" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="B218" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="B219" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="0" t="s">
+        <v>440</v>
+      </c>
+      <c r="B220" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="0" t="s">
+        <v>441</v>
+      </c>
+      <c r="B221" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A222" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="B222" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="0" t="s">
+        <v>443</v>
+      </c>
+      <c r="B223" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="B224" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A225" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="B225" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A226" s="0" t="s">
+        <v>446</v>
+      </c>
+      <c r="B226" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A227" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="B227" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="B228" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="0" t="s">
+        <v>449</v>
+      </c>
+      <c r="B229" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="0" t="s">
+        <v>450</v>
+      </c>
+      <c r="B230" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A231" s="0" t="s">
+        <v>451</v>
+      </c>
+      <c r="B231" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A232" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="B232" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A233" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="B233" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A234" s="0" t="s">
+        <v>454</v>
+      </c>
+      <c r="B234" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A235" s="0" t="s">
+        <v>455</v>
+      </c>
+      <c r="B235" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A236" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="B236" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A237" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="B237" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A238" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="B238" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A239" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="B239" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A240" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="B240" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A241" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="B241" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A242" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="B242" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A243" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="B243" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="0" t="s">
+        <v>464</v>
+      </c>
+      <c r="B244" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A245" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="B245" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A246" s="0" t="s">
+        <v>466</v>
+      </c>
+      <c r="B246" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="0" t="s">
+        <v>467</v>
+      </c>
+      <c r="B247" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="0" t="s">
+        <v>468</v>
+      </c>
+      <c r="B248" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="B249" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="B250" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A251" s="0" t="s">
+        <v>471</v>
+      </c>
+      <c r="B251" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A252" s="0" t="s">
+        <v>472</v>
+      </c>
+      <c r="B252" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A253" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="B253" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A254" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="B254" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="B255" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A256" s="0" t="s">
+        <v>476</v>
+      </c>
+      <c r="B256" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A257" s="0" t="s">
+        <v>477</v>
+      </c>
+      <c r="B257" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A258" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="B258" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="0" t="s">
+        <v>479</v>
+      </c>
+      <c r="B259" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A260" s="0" t="s">
+        <v>480</v>
+      </c>
+      <c r="B260" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A261" s="0" t="s">
+        <v>481</v>
+      </c>
+      <c r="B261" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A262" s="0" t="s">
+        <v>482</v>
+      </c>
+      <c r="B262" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A263" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="B263" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A264" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="B264" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A265" s="0" t="s">
+        <v>485</v>
+      </c>
+      <c r="B265" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A266" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="B266" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A267" s="0" t="s">
+        <v>487</v>
+      </c>
+      <c r="B267" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A268" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="B268" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A269" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="B269" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A270" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="B270" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="0" t="s">
+        <v>491</v>
+      </c>
+      <c r="B271" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A272" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="B272" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A273" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="B273" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="B274" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A275" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="B275" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A276" s="0" t="s">
+        <v>496</v>
+      </c>
+      <c r="B276" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A277" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="B277" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A278" s="0" t="s">
+        <v>498</v>
+      </c>
+      <c r="B278" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A279" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="B279" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A280" s="0" t="s">
+        <v>500</v>
+      </c>
+      <c r="B280" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A281" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="B281" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A282" s="0" t="s">
+        <v>502</v>
+      </c>
+      <c r="B282" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A283" s="0" t="s">
+        <v>503</v>
+      </c>
+      <c r="B283" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A284" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="B284" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A285" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="B285" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A286" s="0" t="s">
+        <v>506</v>
+      </c>
+      <c r="B286" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A287" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="B287" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A288" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="B288" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A289" s="0" t="s">
+        <v>509</v>
+      </c>
+      <c r="B289" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A290" s="0" t="s">
+        <v>510</v>
+      </c>
+      <c r="B290" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A291" s="0" t="s">
+        <v>511</v>
+      </c>
+      <c r="B291" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A292" s="0" t="s">
+        <v>512</v>
+      </c>
+      <c r="B292" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A293" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="B293" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A294" s="0" t="s">
+        <v>514</v>
+      </c>
+      <c r="B294" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A295" s="0" t="s">
+        <v>515</v>
+      </c>
+      <c r="B295" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -3683,12 +5804,12 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="A:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3696,10 +5817,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>323</v>
+        <v>516</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>324</v>
+        <v>517</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3710,15 +5831,15 @@
         <v>209</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>325</v>
+        <v>518</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>326</v>
+        <v>519</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>327</v>
+        <v>520</v>
       </c>
     </row>
   </sheetData>
@@ -3740,22 +5861,22 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="32" t="s">
-        <v>328</v>
+        <v>521</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>329</v>
+        <v>522</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3768,7 +5889,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>330</v>
+        <v>523</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>122</v>
@@ -3776,7 +5897,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>331</v>
+        <v>524</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>126</v>
@@ -3784,7 +5905,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>332</v>
+        <v>525</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>129</v>
@@ -3792,74 +5913,74 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>333</v>
+        <v>526</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>334</v>
+        <v>527</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>335</v>
+        <v>528</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>336</v>
+        <v>529</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>337</v>
+        <v>530</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>338</v>
+        <v>531</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>339</v>
+        <v>532</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>340</v>
+        <v>533</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>341</v>
+        <v>534</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>342</v>
+        <v>535</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>343</v>
+        <v>536</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>344</v>
+        <v>537</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>345</v>
+        <v>538</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>346</v>
+        <v>539</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>347</v>
+        <v>540</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>348</v>
+        <v>541</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>349</v>
+        <v>542</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>350</v>
+        <v>543</v>
       </c>
     </row>
   </sheetData>
@@ -3867,8 +5988,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -3881,22 +6002,22 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="32" t="s">
-        <v>328</v>
+        <v>521</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>329</v>
+        <v>522</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3909,98 +6030,98 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>352</v>
+        <v>545</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>352</v>
+        <v>545</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>353</v>
+        <v>546</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>353</v>
+        <v>546</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>355</v>
+        <v>548</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>355</v>
+        <v>548</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>356</v>
+        <v>549</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>356</v>
+        <v>549</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>357</v>
+        <v>550</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>357</v>
+        <v>550</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>359</v>
+        <v>552</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>359</v>
+        <v>552</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>360</v>
+        <v>553</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>360</v>
+        <v>553</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>361</v>
+        <v>554</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>361</v>
+        <v>554</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>362</v>
+        <v>555</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>362</v>
+        <v>555</v>
       </c>
     </row>
   </sheetData>
@@ -4008,8 +6129,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -4022,19 +6143,19 @@
   <dimension ref="A1:B89"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="32" t="s">
-        <v>328</v>
+        <v>521</v>
       </c>
       <c r="B1" s="32"/>
     </row>
@@ -4043,703 +6164,703 @@
         <v>96</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>363</v>
+        <v>556</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>364</v>
+        <v>557</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>365</v>
+        <v>558</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>366</v>
+        <v>559</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>367</v>
+        <v>560</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>368</v>
+        <v>561</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>369</v>
+        <v>562</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>370</v>
+        <v>563</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>371</v>
+        <v>564</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>372</v>
+        <v>565</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>373</v>
+        <v>566</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>374</v>
+        <v>567</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>375</v>
+        <v>568</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>376</v>
+        <v>569</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>377</v>
+        <v>570</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>378</v>
+        <v>571</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>379</v>
+        <v>572</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>380</v>
+        <v>573</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>351</v>
+        <v>544</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>381</v>
+        <v>574</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>352</v>
+        <v>545</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>382</v>
+        <v>575</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>352</v>
+        <v>545</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>383</v>
+        <v>576</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>352</v>
+        <v>545</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>384</v>
+        <v>577</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>352</v>
+        <v>545</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>385</v>
+        <v>578</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>352</v>
+        <v>545</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>386</v>
+        <v>579</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>352</v>
+        <v>545</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>387</v>
+        <v>580</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>353</v>
+        <v>546</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>388</v>
+        <v>581</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>353</v>
+        <v>546</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>389</v>
+        <v>582</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>353</v>
+        <v>546</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>390</v>
+        <v>583</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>353</v>
+        <v>546</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>391</v>
+        <v>584</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>353</v>
+        <v>546</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>392</v>
+        <v>585</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>393</v>
+        <v>586</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>394</v>
+        <v>587</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>395</v>
+        <v>588</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>396</v>
+        <v>589</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>397</v>
+        <v>590</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>398</v>
+        <v>591</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>399</v>
+        <v>592</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>400</v>
+        <v>593</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>401</v>
+        <v>594</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>402</v>
+        <v>595</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>403</v>
+        <v>596</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>404</v>
+        <v>597</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>405</v>
+        <v>598</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>406</v>
+        <v>599</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>355</v>
+        <v>548</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>407</v>
+        <v>600</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>355</v>
+        <v>548</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>408</v>
+        <v>601</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>355</v>
+        <v>548</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>409</v>
+        <v>602</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>355</v>
+        <v>548</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>410</v>
+        <v>603</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>355</v>
+        <v>548</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>411</v>
+        <v>604</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>356</v>
+        <v>549</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>412</v>
+        <v>605</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>356</v>
+        <v>549</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>413</v>
+        <v>606</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>356</v>
+        <v>549</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>414</v>
+        <v>607</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>356</v>
+        <v>549</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>415</v>
+        <v>608</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>356</v>
+        <v>549</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>416</v>
+        <v>609</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>356</v>
+        <v>549</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>417</v>
+        <v>610</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>356</v>
+        <v>549</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>418</v>
+        <v>611</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>356</v>
+        <v>549</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>419</v>
+        <v>612</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>357</v>
+        <v>550</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>420</v>
+        <v>613</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>357</v>
+        <v>550</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>421</v>
+        <v>614</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>357</v>
+        <v>550</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>422</v>
+        <v>615</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>357</v>
+        <v>550</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>423</v>
+        <v>616</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>357</v>
+        <v>550</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>424</v>
+        <v>617</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>425</v>
+        <v>618</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>426</v>
+        <v>619</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>427</v>
+        <v>620</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>428</v>
+        <v>621</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>429</v>
+        <v>622</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>430</v>
+        <v>623</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>431</v>
+        <v>624</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>432</v>
+        <v>625</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>433</v>
+        <v>626</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>434</v>
+        <v>627</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>435</v>
+        <v>628</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>436</v>
+        <v>629</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>437</v>
+        <v>630</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>438</v>
+        <v>631</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>358</v>
+        <v>551</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>439</v>
+        <v>632</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>359</v>
+        <v>552</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>440</v>
+        <v>633</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>359</v>
+        <v>552</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>441</v>
+        <v>634</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>359</v>
+        <v>552</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>442</v>
+        <v>635</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>359</v>
+        <v>552</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>443</v>
+        <v>636</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>359</v>
+        <v>552</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>444</v>
+        <v>637</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>359</v>
+        <v>552</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>445</v>
+        <v>638</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>359</v>
+        <v>552</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>446</v>
+        <v>639</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>359</v>
+        <v>552</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>447</v>
+        <v>640</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>359</v>
+        <v>552</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>438</v>
+        <v>631</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>359</v>
+        <v>552</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>448</v>
+        <v>641</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>359</v>
+        <v>552</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>449</v>
+        <v>642</v>
       </c>
     </row>
   </sheetData>
@@ -4747,8 +6868,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -4761,14 +6882,14 @@
   <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="A:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="172.25"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="170.357142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4947,8 +7068,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -4961,42 +7082,42 @@
   <dimension ref="A1:AW9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="A:B"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="45" min="27" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="7" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="8" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="49" min="48" style="7" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="50" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="45" min="27" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="7" width="6.75"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="8" width="6.75"/>
+    <col collapsed="false" hidden="false" max="49" min="48" style="7" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="50" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5435,48 +7556,48 @@
   <dimension ref="A1:AX8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="A:B C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="20.25"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="6.75"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="6.75"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="6.75"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5756,47 +7877,47 @@
   <dimension ref="A1:BE7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="1" sqref="A:B C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="6" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="20.25"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="6" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="6.75"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="6.75"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="6.75"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6066,16 +8187,15 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="1" sqref="A:B C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="14.5867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="14.3112244897959"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6166,16 +8286,15 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="1" sqref="A:B D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.515306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3877551020408"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6239,19 +8358,18 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="1" sqref="A:B C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="23" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="23" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1017" min="7" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="1018" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="23" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="23" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="1018" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="49.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6356,16 +8474,15 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="1" sqref="A:B D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.0408163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6785714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
PIM 2.2 migration (#62)
</commit_message>
<xml_diff>
--- a/src/Resources/fixtures/minimal/init.xlsx
+++ b/src/Resources/fixtures/minimal/init.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="978" firstSheet="0" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="README-EN" sheetId="1" state="visible" r:id="rId2"/>
@@ -779,16 +779,16 @@
     <t xml:space="preserve">password</t>
   </si>
   <si>
-    <t xml:space="preserve">catalog_locale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user_locale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">catalog_scope</t>
-  </si>
-  <si>
-    <t xml:space="preserve">default_tree</t>
+    <t xml:space="preserve">catalog_default_locale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user_default_locale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">catalog_default_scope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default_category_tree</t>
   </si>
   <si>
     <t xml:space="preserve">roles</t>
@@ -2668,9 +2668,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>761760</xdr:colOff>
+      <xdr:colOff>761400</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2680,7 +2680,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9905760" cy="9532080"/>
+          <a:ext cx="9781560" cy="9531720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2713,9 +2713,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>761760</xdr:colOff>
+      <xdr:colOff>761400</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2725,7 +2725,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9905760" cy="9532080"/>
+          <a:ext cx="9781560" cy="9531720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2758,9 +2758,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>761760</xdr:colOff>
+      <xdr:colOff>761400</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2770,7 +2770,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9905760" cy="9532080"/>
+          <a:ext cx="9781560" cy="9531720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2808,9 +2808,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>376920</xdr:colOff>
+      <xdr:colOff>376560</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2820,7 +2820,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="7118640" cy="9526680"/>
+          <a:ext cx="7032600" cy="9526320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2829,7 +2829,7 @@
           <a:srgbClr val="ffffff"/>
         </a:solidFill>
         <a:ln w="9360">
-          <a:miter/>
+          <a:noFill/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -2850,9 +2850,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>376920</xdr:colOff>
+      <xdr:colOff>376560</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2862,7 +2862,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="7118640" cy="9526680"/>
+          <a:ext cx="7032600" cy="9526320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2871,7 +2871,7 @@
           <a:srgbClr val="ffffff"/>
         </a:solidFill>
         <a:ln w="9360">
-          <a:miter/>
+          <a:noFill/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -2897,9 +2897,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>129600</xdr:colOff>
+      <xdr:colOff>129240</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>109440</xdr:rowOff>
+      <xdr:rowOff>109080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2909,7 +2909,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="6776280" cy="8392320"/>
+          <a:ext cx="6680520" cy="8391960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2918,7 +2918,7 @@
           <a:srgbClr val="ffffff"/>
         </a:solidFill>
         <a:ln w="9360">
-          <a:miter/>
+          <a:noFill/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -2939,9 +2939,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>129600</xdr:colOff>
+      <xdr:colOff>129240</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>109440</xdr:rowOff>
+      <xdr:rowOff>109080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2951,7 +2951,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="6776280" cy="8392320"/>
+          <a:ext cx="6680520" cy="8391960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2960,7 +2960,7 @@
           <a:srgbClr val="ffffff"/>
         </a:solidFill>
         <a:ln w="9360">
-          <a:miter/>
+          <a:noFill/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -2981,9 +2981,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>580680</xdr:colOff>
+      <xdr:colOff>580320</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>123480</xdr:rowOff>
+      <xdr:rowOff>123120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2993,7 +2993,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9762480" cy="9539640"/>
+          <a:ext cx="9628920" cy="9539280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3026,9 +3026,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>580680</xdr:colOff>
+      <xdr:colOff>580320</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>123480</xdr:rowOff>
+      <xdr:rowOff>123120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3038,7 +3038,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9762480" cy="9539640"/>
+          <a:ext cx="9628920" cy="9539280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3076,9 +3076,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>377280</xdr:colOff>
+      <xdr:colOff>376920</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>137520</xdr:rowOff>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3088,7 +3088,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="9471960" cy="9365040"/>
+          <a:ext cx="9338040" cy="9364680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3097,7 +3097,7 @@
           <a:srgbClr val="ffffff"/>
         </a:solidFill>
         <a:ln w="9360">
-          <a:miter/>
+          <a:noFill/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -3118,9 +3118,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>377280</xdr:colOff>
+      <xdr:colOff>376920</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>137520</xdr:rowOff>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3130,7 +3130,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="135000" y="0"/>
-          <a:ext cx="9471960" cy="9365040"/>
+          <a:ext cx="9338040" cy="9364680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3139,7 +3139,7 @@
           <a:srgbClr val="ffffff"/>
         </a:solidFill>
         <a:ln w="9360">
-          <a:miter/>
+          <a:noFill/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -3167,8 +3167,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="109.882653061224"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="108.668367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3383,14 +3384,15 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3456,9 +3458,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="34" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="34" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="34" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="34" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="35" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3558,9 +3561,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3608,8 +3611,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -3627,9 +3630,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3669,8 +3672,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -3682,24 +3685,23 @@
   </sheetPr>
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3783,8 +3785,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -3802,7 +3804,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6170,8 +6173,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -6188,6 +6191,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -6243,9 +6249,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6365,8 +6370,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -6384,9 +6389,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6554,8 +6558,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -6573,9 +6577,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="25.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7725,8 +7728,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -7744,9 +7747,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="168.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="166.581632653061"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7925,8 +7926,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -7944,35 +7945,37 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="7" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="8" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="49" min="48" style="7" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="13.5"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="45" min="27" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="7" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="8" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="49" min="48" style="7" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="50" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8402,43 +8405,43 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="6" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8591,42 +8594,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="6" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="6" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="6" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="36" min="28" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="42" min="40" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="46" min="44" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="7" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="8" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="7" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="7" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1021" min="51" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8765,11 +8768,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8865,11 +8868,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8938,14 +8941,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="23" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="23" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="1017" min="7" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="1018" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="23" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="23" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1017" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="49.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9055,11 +9057,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>